<commit_message>
Add auto-scroll to top when switching tabs
- Install streamlit-js-eval package for JS execution
- Track page changes in session_state
- Scroll to top only when page actually changes
- Added streamlit and plotly to requirements.txt

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Strategic_Report.xlsx
+++ b/Strategic_Report.xlsx
@@ -2350,7 +2350,7 @@
       <c r="G8" s="9" t="n"/>
       <c r="I8" s="10" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>12</t>
         </is>
       </c>
       <c r="J8" s="8" t="n"/>
@@ -2875,7 +2875,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:J108"/>
+  <dimension ref="B2:J109"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2907,7 +2907,7 @@
     <row r="3" ht="22" customHeight="1">
       <c r="B3" s="38" t="inlineStr">
         <is>
-          <t>Generated: February 05, 2026 at 08:54  •  Version: 2.2  •  AI Model: gpt-oss:20b</t>
+          <t>Generated: February 05, 2026 at 14:53  •  Version: 2.2  •  AI Model: gpt-oss:20b</t>
         </is>
       </c>
     </row>
@@ -2999,7 +2999,7 @@
     <row r="11" ht="22" customHeight="1">
       <c r="B11" s="53" t="inlineStr">
         <is>
-          <t>Avg Resolution: 5.2 days</t>
+          <t>Avg Resolution: 7.2 days</t>
         </is>
       </c>
       <c r="D11" s="53" t="inlineStr">
@@ -3617,12 +3617,12 @@
     <row r="50" ht="32" customHeight="1">
       <c r="B50" s="92" t="inlineStr">
         <is>
-          <t>🟢</t>
+          <t>🟡</t>
         </is>
       </c>
       <c r="C50" s="93" t="inlineStr">
         <is>
-          <t>Average predicted resolution: 5.2 days</t>
+          <t>Average predicted resolution: 7.2 days</t>
         </is>
       </c>
       <c r="D50" s="65" t="n"/>
@@ -3714,7 +3714,7 @@
     <row r="57" ht="48" customHeight="1">
       <c r="B57" s="104" t="inlineStr">
         <is>
-          <t>Analysis reveals $2.31 million in total financial exposure driven primarily by Scheduling &amp; Planning inefficiencies. Immediate focus on a $14,207 scheduling‑process overhaul can unlock $618,272 in annual savings, delivering a 4,252 % ROI and a payback period of just 0.3 months.</t>
+          <t>Analysis reveals $661,025 in direct financial exposure driven primarily by Scheduling &amp; Planning tickets. Immediate focus on a $14,207 process‑improvement investment can slash costs by $618,272/year (4252 % ROI, 0.3‑month payback).</t>
         </is>
       </c>
       <c r="C57" s="65" t="n"/>
@@ -3756,10 +3756,10 @@
       <c r="I59" s="65" t="n"/>
       <c r="J59" s="57" t="n"/>
     </row>
-    <row r="60" ht="32" customHeight="1">
+    <row r="60" ht="18" customHeight="1">
       <c r="B60" s="104" t="inlineStr">
         <is>
-          <t>- 396 tickets were analyzed during the reporting period, generating a $661,025 direct cost and $1,652,562.50 in revenue at risk.</t>
+          <t>- 396 tickets analyzed over the reporting period, covering all escalation severities.</t>
         </is>
       </c>
       <c r="C60" s="65" t="n"/>
@@ -3774,7 +3774,7 @@
     <row r="61" ht="18" customHeight="1">
       <c r="B61" s="104" t="inlineStr">
         <is>
-          <t>- Severity distribution: Major 222 (56%), Minor 134 (34%), Critical 40 (10%).</t>
+          <t>- Total direct impact: $661,025; revenue at risk: $1,652,562.50.</t>
         </is>
       </c>
       <c r="C61" s="65" t="n"/>
@@ -3789,7 +3789,7 @@
     <row r="62" ht="18" customHeight="1">
       <c r="B62" s="104" t="inlineStr">
         <is>
-          <t>- Scheduling &amp; Planning accounts for 136 tickets (34.3%) and $193,210 (29.2%) of the direct cost.</t>
+          <t>- Severity split: Major 222 (56 %), Minor 134 (34 %), Critical 40 (10 %).</t>
         </is>
       </c>
       <c r="C62" s="65" t="n"/>
@@ -3801,10 +3801,10 @@
       <c r="I62" s="65" t="n"/>
       <c r="J62" s="57" t="n"/>
     </row>
-    <row r="63" ht="32" customHeight="1">
+    <row r="63" ht="18" customHeight="1">
       <c r="B63" s="104" t="inlineStr">
         <is>
-          <t>- Current health: At Risk – high exposure and a cost‑efficiency score of 65/100 signal urgent improvement needs.</t>
+          <t>- Overall health: Stable with a high concentration of costs (33 % from the top 20 % of tickets).</t>
         </is>
       </c>
       <c r="C63" s="65" t="n"/>
@@ -3831,10 +3831,10 @@
       <c r="I64" s="65" t="n"/>
       <c r="J64" s="57" t="n"/>
     </row>
-    <row r="65" ht="26" customHeight="1">
-      <c r="B65" s="103" t="inlineStr">
-        <is>
-          <t>SECTION 3 - KEY FINDINGS (MECE)</t>
+    <row r="65" ht="18" customHeight="1">
+      <c r="B65" s="104" t="inlineStr">
+        <is>
+          <t>SECTION 3 - KEY FINDINGS (MECE Structure)</t>
         </is>
       </c>
       <c r="C65" s="65" t="n"/>
@@ -3861,10 +3861,10 @@
       <c r="I66" s="65" t="n"/>
       <c r="J66" s="57" t="n"/>
     </row>
-    <row r="67" ht="32" customHeight="1">
+    <row r="67" ht="18" customHeight="1">
       <c r="B67" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: 136 tickets (34.3%) in Scheduling &amp; Planning; $193,210 (29.2%) of direct cost; $618,272/year potential savings from a $14,207 investment.</t>
+          <t>- *Data*: 136 Scheduling &amp; Planning tickets (34.3 %) costing $193,210 (29.2 % of total).</t>
         </is>
       </c>
       <c r="C67" s="65" t="n"/>
@@ -3879,7 +3879,7 @@
     <row r="68" ht="32" customHeight="1">
       <c r="B68" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: Inefficient scheduling consumes nearly a third of all escalation costs; correcting the process offers the highest ROI and quickest payback.</t>
+          <t>- *So What*: Inefficient scheduling drives nearly a third of the financial exposure; streamlining workflows yields the highest ROI.</t>
         </is>
       </c>
       <c r="C68" s="65" t="n"/>
@@ -3906,10 +3906,10 @@
       <c r="I69" s="65" t="n"/>
       <c r="J69" s="57" t="n"/>
     </row>
-    <row r="70" ht="32" customHeight="1">
+    <row r="70" ht="18" customHeight="1">
       <c r="B70" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: 49 tickets (12.4%) in Documentation &amp; Reporting; $71,029 (10.7%) of direct cost; $1,449.57 average per ticket.</t>
+          <t>- *Data*: 49 Documentation &amp; Reporting tickets (12.4 %) costing $71,029.</t>
         </is>
       </c>
       <c r="C70" s="65" t="n"/>
@@ -3924,7 +3924,7 @@
     <row r="71" ht="32" customHeight="1">
       <c r="B71" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: Poor documentation forces rework and delays, inflating costs; standardizing templates and training can eliminate these tickets.</t>
+          <t>- *So What*: Incomplete or outdated documentation forces repeat work, inflating costs and delaying resolution.</t>
         </is>
       </c>
       <c r="C71" s="65" t="n"/>
@@ -3951,10 +3951,10 @@
       <c r="I72" s="65" t="n"/>
       <c r="J72" s="57" t="n"/>
     </row>
-    <row r="73" ht="32" customHeight="1">
+    <row r="73" ht="18" customHeight="1">
       <c r="B73" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: 98 tickets (24.7%) in Configuration &amp; Data Mismatch; $153,039 (23.2%) of direct cost; $1,561.62 average per ticket; $489,725/year savings from a $15,616 investment.</t>
+          <t>- *Data*: 98 Configuration &amp; Data Mismatch tickets (24.7 %) costing $153,039.</t>
         </is>
       </c>
       <c r="C73" s="65" t="n"/>
@@ -3969,7 +3969,7 @@
     <row r="74" ht="32" customHeight="1">
       <c r="B74" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: Misconfigurations create repeat escalations; a robust configuration‑management system will cut costs dramatically.</t>
+          <t>- *So What*: Data integrity problems cause cascading delays and re‑work, consuming 23 % of the budget.</t>
         </is>
       </c>
       <c r="C74" s="65" t="n"/>
@@ -3996,10 +3996,10 @@
       <c r="I75" s="65" t="n"/>
       <c r="J75" s="57" t="n"/>
     </row>
-    <row r="76" ht="32" customHeight="1">
+    <row r="76" ht="18" customHeight="1">
       <c r="B76" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: 27 tickets (6.8%) in Validation &amp; QA; $78,110 (11.8%) of direct cost; $2,892.96 average per ticket; $249,952/year savings from a $28,930 investment.</t>
+          <t>- *Data*: Site Readiness (39 tickets, $71,446) and Validation &amp; QA (27 tickets, $78,110).</t>
         </is>
       </c>
       <c r="C76" s="65" t="n"/>
@@ -4014,7 +4014,7 @@
     <row r="77" ht="32" customHeight="1">
       <c r="B77" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: High per‑ticket cost signals hand‑off and QA breakdowns; tightening communication protocols will reduce delays and expenses.</t>
+          <t>- *So What*: Poor handoff and coordination inflate average cost per ticket (up to $2,892.96), eroding margin.</t>
         </is>
       </c>
       <c r="C77" s="65" t="n"/>
@@ -4041,10 +4041,10 @@
       <c r="I78" s="65" t="n"/>
       <c r="J78" s="57" t="n"/>
     </row>
-    <row r="79" ht="26" customHeight="1">
-      <c r="B79" s="103" t="inlineStr">
-        <is>
-          <t>SECTION 4 - 80/20 ANALYSIS</t>
+    <row r="79" ht="18" customHeight="1">
+      <c r="B79" s="104" t="inlineStr">
+        <is>
+          <t>SECTION 4 - 80/20 ANALYSIS (Pareto Principle)</t>
         </is>
       </c>
       <c r="C79" s="65" t="n"/>
@@ -4056,10 +4056,10 @@
       <c r="I79" s="65" t="n"/>
       <c r="J79" s="57" t="n"/>
     </row>
-    <row r="80" ht="48" customHeight="1">
+    <row r="80" ht="32" customHeight="1">
       <c r="B80" s="104" t="inlineStr">
         <is>
-          <t>- Financial Impact: Top four categories—Scheduling &amp; Planning ($193,210), Configuration &amp; Data Mismatch ($153,039), Validation &amp; QA ($78,110), Site Readiness ($71,446)—collectively account for $566,834 (86% of $661,025).</t>
+          <t>- Financial Impact: Scheduling &amp; Planning ($193,210) + Configuration &amp; Data Mismatch ($153,039) + Validation &amp; QA ($78,110) = $424,359 (64 % of total).</t>
         </is>
       </c>
       <c r="C80" s="65" t="n"/>
@@ -4071,10 +4071,10 @@
       <c r="I80" s="65" t="n"/>
       <c r="J80" s="57" t="n"/>
     </row>
-    <row r="81" ht="18" customHeight="1">
+    <row r="81" ht="32" customHeight="1">
       <c r="B81" s="104" t="inlineStr">
         <is>
-          <t>- Ticket Volume: The same four categories generate 322 tickets (81% of 396).</t>
+          <t>- Ticket Volume: Scheduling &amp; Planning (136 tickets, 34.3 %) + Configuration &amp; Data Mismatch (98 tickets, 24.7 %) + Validation &amp; QA (27 tickets, 6.8 %) = 261 tickets (66 % of volume).</t>
         </is>
       </c>
       <c r="C81" s="65" t="n"/>
@@ -4089,7 +4089,7 @@
     <row r="82" ht="32" customHeight="1">
       <c r="B82" s="104" t="inlineStr">
         <is>
-          <t>- Resource Focus: Allocate 60% of improvement budget to Scheduling &amp; Planning, 25% to Configuration &amp; Data Mismatch, and 15% to Validation &amp; QA to capture the bulk of savings.</t>
+          <t>- Resource Focus: Allocate 70 % of improvement budget to Scheduling &amp; Planning and Configuration &amp; Data Mismatch; the remaining 30 % to Validation &amp; QA.</t>
         </is>
       </c>
       <c r="C82" s="65" t="n"/>
@@ -4149,7 +4149,7 @@
     <row r="86" ht="18" customHeight="1">
       <c r="B86" s="104" t="inlineStr">
         <is>
-          <t>1. Automated Scheduling Dashboard – *Impact*: $618,272/year; *Timeline*: Week 1‑2.</t>
+          <t>1. Scheduling &amp; Planning Process Overhaul</t>
         </is>
       </c>
       <c r="C86" s="65" t="n"/>
@@ -4164,7 +4164,7 @@
     <row r="87" ht="18" customHeight="1">
       <c r="B87" s="104" t="inlineStr">
         <is>
-          <t>2. QA Checklist Implementation – *Impact*: $249,952/year; *Timeline*: Week 1‑2.</t>
+          <t>- *Impact*: $618,272/year savings</t>
         </is>
       </c>
       <c r="C87" s="65" t="n"/>
@@ -4179,7 +4179,7 @@
     <row r="88" ht="18" customHeight="1">
       <c r="B88" s="104" t="inlineStr">
         <is>
-          <t>MAJOR PROJECTS (High Impact, High Effort)</t>
+          <t>- *Timeline*: Week 1‑2 (implementation of automated scheduling tool)</t>
         </is>
       </c>
       <c r="C88" s="65" t="n"/>
@@ -4194,7 +4194,7 @@
     <row r="89" ht="18" customHeight="1">
       <c r="B89" s="104" t="inlineStr">
         <is>
-          <t>3. Configuration Management Overhaul – *Impact*: $489,725/year; *Timeline*: Month 2‑3.</t>
+          <t>- *Rationale*: 4252 % ROI, 0.3‑month payback</t>
         </is>
       </c>
       <c r="C89" s="65" t="n"/>
@@ -4209,7 +4209,7 @@
     <row r="90" ht="18" customHeight="1">
       <c r="B90" s="104" t="inlineStr">
         <is>
-          <t>4. Documentation &amp; Reporting Standardization – *Impact*: $71,029/year; *Timeline*: Month 3‑4.</t>
+          <t>2. Configuration &amp; Data Integrity Fixes</t>
         </is>
       </c>
       <c r="C90" s="65" t="n"/>
@@ -4224,7 +4224,7 @@
     <row r="91" ht="18" customHeight="1">
       <c r="B91" s="104" t="inlineStr">
         <is>
-          <t>FILL‑INS (Low Impact, Low Effort)</t>
+          <t>- *Impact*: $489,725/year savings</t>
         </is>
       </c>
       <c r="C91" s="65" t="n"/>
@@ -4239,7 +4239,7 @@
     <row r="92" ht="18" customHeight="1">
       <c r="B92" s="104" t="inlineStr">
         <is>
-          <t>5. Cross‑Functional Handoff Training – *Impact*: $10,000/year (est.); *Timeline*: Ongoing.</t>
+          <t>- *Timeline*: Week 3‑4 (data validation scripts &amp; automated reconciliation)</t>
         </is>
       </c>
       <c r="C92" s="65" t="n"/>
@@ -4251,10 +4251,10 @@
       <c r="I92" s="65" t="n"/>
       <c r="J92" s="57" t="n"/>
     </row>
-    <row r="93" ht="32" customHeight="1">
+    <row r="93" ht="18" customHeight="1">
       <c r="B93" s="104" t="inlineStr">
         <is>
-          <t>All actions are grounded in the data above; each projected saving reflects the current cost or ROI figures provided.</t>
+          <t>- *Rationale*: 3036 % ROI, 0.4‑month payback</t>
         </is>
       </c>
       <c r="C93" s="65" t="n"/>
@@ -4269,7 +4269,7 @@
     <row r="94" ht="18" customHeight="1">
       <c r="B94" s="104" t="inlineStr">
         <is>
-          <t>---</t>
+          <t>MAJOR PROJECTS (High Impact, High Effort)</t>
         </is>
       </c>
       <c r="C94" s="65" t="n"/>
@@ -4284,7 +4284,7 @@
     <row r="95" ht="18" customHeight="1">
       <c r="B95" s="104" t="inlineStr">
         <is>
-          <t>SECTION 6 - RISK ASSESSMENT (RAG Status)</t>
+          <t>3. Validation &amp; QA Enhancement Program</t>
         </is>
       </c>
       <c r="C95" s="65" t="n"/>
@@ -4299,7 +4299,7 @@
     <row r="96" ht="18" customHeight="1">
       <c r="B96" s="104" t="inlineStr">
         <is>
-          <t>| Area | Status | Reason &amp; Key Figures |</t>
+          <t>- *Impact*: $249,952/year savings</t>
         </is>
       </c>
       <c r="C96" s="65" t="n"/>
@@ -4314,7 +4314,7 @@
     <row r="97" ht="18" customHeight="1">
       <c r="B97" s="104" t="inlineStr">
         <is>
-          <t>|------|--------|----------------------|</t>
+          <t>- *Timeline*: Month 2‑3 (standardized QA checklists, automated test harness)</t>
         </is>
       </c>
       <c r="C97" s="65" t="n"/>
@@ -4326,10 +4326,10 @@
       <c r="I97" s="65" t="n"/>
       <c r="J97" s="57" t="n"/>
     </row>
-    <row r="98" ht="32" customHeight="1">
+    <row r="98" ht="18" customHeight="1">
       <c r="B98" s="104" t="inlineStr">
         <is>
-          <t>| Financial Exposure | RED | $2.31 M total exposure; $661,025 direct cost + $1.65 M revenue at risk |</t>
+          <t>- *Rationale*: 764 % ROI, 1.4‑month payback</t>
         </is>
       </c>
       <c r="C98" s="65" t="n"/>
@@ -4341,10 +4341,10 @@
       <c r="I98" s="65" t="n"/>
       <c r="J98" s="57" t="n"/>
     </row>
-    <row r="99" ht="32" customHeight="1">
+    <row r="99" ht="18" customHeight="1">
       <c r="B99" s="104" t="inlineStr">
         <is>
-          <t>| Recurrence Risk | AMBER | Recurrence risk exposure $0.00, but 33 % of costs stem from top 20 % tickets |</t>
+          <t>FILL‑INS (Low Impact, Low Effort)</t>
         </is>
       </c>
       <c r="C99" s="65" t="n"/>
@@ -4359,7 +4359,7 @@
     <row r="100" ht="18" customHeight="1">
       <c r="B100" s="104" t="inlineStr">
         <is>
-          <t>| Process Maturity | AMBER | Cost‑efficiency score 65/100; high potential for process improvement |</t>
+          <t>4. Documentation &amp; Reporting Refresh</t>
         </is>
       </c>
       <c r="C100" s="65" t="n"/>
@@ -4371,10 +4371,10 @@
       <c r="I100" s="65" t="n"/>
       <c r="J100" s="57" t="n"/>
     </row>
-    <row r="101" ht="32" customHeight="1">
+    <row r="101" ht="18" customHeight="1">
       <c r="B101" s="104" t="inlineStr">
         <is>
-          <t>| Resolution Capability | AMBER | SLA penalty exposure $32,163; high average cost per ticket in Validation &amp; QA |</t>
+          <t>- *Impact*: $7,103/year (10 % reduction of $71,029)</t>
         </is>
       </c>
       <c r="C101" s="65" t="n"/>
@@ -4389,7 +4389,7 @@
     <row r="102" ht="18" customHeight="1">
       <c r="B102" s="104" t="inlineStr">
         <is>
-          <t>---</t>
+          <t>- *Timeline*: Ongoing (quarterly review)</t>
         </is>
       </c>
       <c r="C102" s="65" t="n"/>
@@ -4401,10 +4401,10 @@
       <c r="I102" s="65" t="n"/>
       <c r="J102" s="57" t="n"/>
     </row>
-    <row r="103" ht="26" customHeight="1">
-      <c r="B103" s="103" t="inlineStr">
-        <is>
-          <t>SECTION 7 - EXECUTIVE CALLOUT</t>
+    <row r="103" ht="18" customHeight="1">
+      <c r="B103" s="104" t="inlineStr">
+        <is>
+          <t>---</t>
         </is>
       </c>
       <c r="C103" s="65" t="n"/>
@@ -4416,10 +4416,10 @@
       <c r="I103" s="65" t="n"/>
       <c r="J103" s="57" t="n"/>
     </row>
-    <row r="104" ht="48" customHeight="1">
+    <row r="104" ht="18" customHeight="1">
       <c r="B104" s="104" t="inlineStr">
         <is>
-          <t>Scheduling &amp; Planning inefficiencies are the single biggest cost driver, contributing $193,210 (29 % of direct impact). By investing $14,207 in a targeted scheduling overhaul, the company can unlock $618,272 in annual savings and recoup the investment in just 9 days.</t>
+          <t>SECTION 6 - RISK ASSESSMENT (RAG Status)</t>
         </is>
       </c>
       <c r="C104" s="65" t="n"/>
@@ -4431,23 +4431,38 @@
       <c r="I104" s="65" t="n"/>
       <c r="J104" s="57" t="n"/>
     </row>
-    <row r="106" ht="8" customHeight="1"/>
-    <row r="107" ht="18" customHeight="1">
-      <c r="B107" s="105" t="inlineStr">
+    <row r="105" ht="18" customHeight="1">
+      <c r="B105" s="104" t="inlineStr">
+        <is>
+          <t>| Area | Status | Reason |</t>
+        </is>
+      </c>
+      <c r="C105" s="65" t="n"/>
+      <c r="D105" s="65" t="n"/>
+      <c r="E105" s="65" t="n"/>
+      <c r="F105" s="65" t="n"/>
+      <c r="G105" s="65" t="n"/>
+      <c r="H105" s="65" t="n"/>
+      <c r="I105" s="65" t="n"/>
+      <c r="J105" s="57" t="n"/>
+    </row>
+    <row r="107" ht="8" customHeight="1"/>
+    <row r="108" ht="18" customHeight="1">
+      <c r="B108" s="105" t="inlineStr">
         <is>
           <t>────────────────────────────────────────────────────────────────────────────────</t>
         </is>
       </c>
     </row>
-    <row r="108">
-      <c r="B108" s="106" t="inlineStr">
-        <is>
-          <t>Report generated by Escalation AI v2.2 • February 05, 2026 at 08:54</t>
+    <row r="109">
+      <c r="B109" s="106" t="inlineStr">
+        <is>
+          <t>Report generated by Escalation AI v2.2 • February 05, 2026 at 14:53</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="121">
+  <mergeCells count="122">
     <mergeCell ref="B67:J67"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="B61:J61"/>
@@ -4510,11 +4525,11 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="B56:J56"/>
     <mergeCell ref="B71:J71"/>
+    <mergeCell ref="B105:J105"/>
     <mergeCell ref="B58:J58"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="B98:J98"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B107:J107"/>
     <mergeCell ref="B60:J60"/>
     <mergeCell ref="B57:J57"/>
     <mergeCell ref="B88:J88"/>
@@ -4536,6 +4551,7 @@
     <mergeCell ref="B94:J94"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B75:J75"/>
+    <mergeCell ref="B109:J109"/>
     <mergeCell ref="B62:J62"/>
     <mergeCell ref="B59:J59"/>
     <mergeCell ref="B96:J96"/>
@@ -5041,7 +5057,7 @@
       </c>
       <c r="AR2" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>10.5</t>
         </is>
       </c>
       <c r="AS2" t="n">
@@ -5247,7 +5263,7 @@
       </c>
       <c r="AR3" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS3" t="n">
@@ -5441,7 +5457,7 @@
       </c>
       <c r="AR4" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS4" t="n">
@@ -5624,7 +5640,7 @@
       </c>
       <c r="AR5" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS5" t="n">
@@ -5820,7 +5836,7 @@
       </c>
       <c r="AR6" t="inlineStr">
         <is>
-          <t>18.8</t>
+          <t>22.2</t>
         </is>
       </c>
       <c r="AS6" t="n">
@@ -6018,11 +6034,11 @@
       </c>
       <c r="AR7" t="inlineStr">
         <is>
-          <t>20.2</t>
+          <t>20.1</t>
         </is>
       </c>
       <c r="AS7" t="n">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="8">
@@ -6220,11 +6236,11 @@
       </c>
       <c r="AR8" t="inlineStr">
         <is>
-          <t>20.2</t>
+          <t>20.1</t>
         </is>
       </c>
       <c r="AS8" t="n">
-        <v>0.39</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="9">
@@ -6410,7 +6426,7 @@
       </c>
       <c r="AR9" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS9" t="n">
@@ -6608,7 +6624,7 @@
       </c>
       <c r="AR10" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS10" t="n">
@@ -6798,7 +6814,7 @@
       </c>
       <c r="AR11" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS11" t="n">
@@ -6983,7 +6999,7 @@
       </c>
       <c r="AR12" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS12" t="n">
@@ -7185,7 +7201,7 @@
       </c>
       <c r="AR13" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS13" t="n">
@@ -7383,11 +7399,11 @@
       </c>
       <c r="AR14" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>16.3</t>
         </is>
       </c>
       <c r="AS14" t="n">
-        <v>0.3</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="15">
@@ -7577,11 +7593,11 @@
       </c>
       <c r="AR15" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS15" t="n">
-        <v>0.3</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="16">
@@ -7773,7 +7789,7 @@
       </c>
       <c r="AR16" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS16" t="n">
@@ -7954,11 +7970,11 @@
       </c>
       <c r="AR17" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="AS17" t="n">
-        <v>0.42</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="18">
@@ -8144,7 +8160,7 @@
       </c>
       <c r="AR18" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="AS18" t="n">
@@ -8334,7 +8350,7 @@
       </c>
       <c r="AR19" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="AS19" t="n">
@@ -8517,7 +8533,7 @@
       </c>
       <c r="AR20" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS20" t="n">
@@ -8703,7 +8719,7 @@
       </c>
       <c r="AR21" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS21" t="n">
@@ -8897,11 +8913,11 @@
       </c>
       <c r="AR22" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS22" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="23">
@@ -9095,7 +9111,7 @@
       </c>
       <c r="AR23" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="AS23" t="n">
@@ -9298,7 +9314,7 @@
       </c>
       <c r="AR24" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="AS24" t="n">
@@ -9492,7 +9508,7 @@
       </c>
       <c r="AR25" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS25" t="n">
@@ -9677,7 +9693,7 @@
       </c>
       <c r="AR26" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS26" t="n">
@@ -9875,7 +9891,7 @@
       </c>
       <c r="AR27" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="AS27" t="n">
@@ -10068,11 +10084,11 @@
       </c>
       <c r="AR28" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="AS28" t="n">
-        <v>0.57</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="29">
@@ -10259,7 +10275,7 @@
       </c>
       <c r="AR29" t="inlineStr">
         <is>
-          <t>11.7</t>
+          <t>8.7</t>
         </is>
       </c>
       <c r="AS29" t="n">
@@ -10463,7 +10479,7 @@
       </c>
       <c r="AR30" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS30" t="n">
@@ -10661,7 +10677,7 @@
       </c>
       <c r="AR31" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS31" t="n">
@@ -10859,11 +10875,11 @@
       </c>
       <c r="AR32" t="inlineStr">
         <is>
-          <t>21.1</t>
+          <t>15.6</t>
         </is>
       </c>
       <c r="AS32" t="n">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="33">
@@ -11057,7 +11073,7 @@
       </c>
       <c r="AR33" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS33" t="n">
@@ -11255,7 +11271,7 @@
       </c>
       <c r="AR34" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS34" t="n">
@@ -11456,11 +11472,11 @@
       </c>
       <c r="AR35" t="inlineStr">
         <is>
-          <t>11.3</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS35" t="n">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="36">
@@ -11642,7 +11658,7 @@
       </c>
       <c r="AR36" t="inlineStr">
         <is>
-          <t>12.7</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="AS36" t="n">
@@ -11836,11 +11852,11 @@
       </c>
       <c r="AR37" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="AS37" t="n">
-        <v>0.3</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="38">
@@ -12029,11 +12045,11 @@
       </c>
       <c r="AR38" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS38" t="n">
-        <v>0.53</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="39">
@@ -12226,7 +12242,7 @@
       </c>
       <c r="AR39" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS39" t="n">
@@ -12427,7 +12443,7 @@
       </c>
       <c r="AR40" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS40" t="n">
@@ -12620,11 +12636,11 @@
       </c>
       <c r="AR41" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS41" t="n">
-        <v>0.3</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="42">
@@ -12814,7 +12830,7 @@
       </c>
       <c r="AR42" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS42" t="n">
@@ -13008,11 +13024,11 @@
       </c>
       <c r="AR43" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>12.0</t>
         </is>
       </c>
       <c r="AS43" t="n">
-        <v>0.3</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="44">
@@ -13198,7 +13214,7 @@
       </c>
       <c r="AR44" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="AS44" t="n">
@@ -13393,11 +13409,11 @@
       </c>
       <c r="AR45" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="AS45" t="n">
-        <v>0.34</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="46">
@@ -13594,11 +13610,11 @@
       </c>
       <c r="AR46" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS46" t="n">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="47">
@@ -13784,7 +13800,7 @@
       </c>
       <c r="AR47" t="inlineStr">
         <is>
-          <t>14.5</t>
+          <t>13.4</t>
         </is>
       </c>
       <c r="AS47" t="n">
@@ -13983,7 +13999,7 @@
       </c>
       <c r="AR48" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS48" t="n">
@@ -14183,7 +14199,7 @@
       </c>
       <c r="AR49" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS49" t="n">
@@ -14383,11 +14399,11 @@
       </c>
       <c r="AR50" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="AS50" t="n">
-        <v>0.47</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="51">
@@ -14586,11 +14602,11 @@
       </c>
       <c r="AR51" t="inlineStr">
         <is>
-          <t>9.2</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="AS51" t="n">
-        <v>0.63</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="52">
@@ -14771,11 +14787,11 @@
       </c>
       <c r="AR52" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="AS52" t="n">
-        <v>0.52</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="53">
@@ -14965,7 +14981,7 @@
       </c>
       <c r="AR53" t="inlineStr">
         <is>
-          <t>1.9</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS53" t="n">
@@ -15163,7 +15179,7 @@
       </c>
       <c r="AR54" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS54" t="n">
@@ -15348,11 +15364,11 @@
       </c>
       <c r="AR55" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="AS55" t="n">
-        <v>0.49</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="56">
@@ -15542,11 +15558,11 @@
       </c>
       <c r="AR56" t="inlineStr">
         <is>
-          <t>11.2</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS56" t="n">
-        <v>0.45</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="57">
@@ -15720,11 +15736,11 @@
       </c>
       <c r="AR57" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="AS57" t="n">
-        <v>0.3</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="58">
@@ -15889,7 +15905,7 @@
       </c>
       <c r="AR58" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS58" t="n">
@@ -16070,7 +16086,7 @@
       </c>
       <c r="AR59" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS59" t="n">
@@ -16240,11 +16256,11 @@
       </c>
       <c r="AR60" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="AS60" t="n">
-        <v>0.3</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="61">
@@ -16425,7 +16441,7 @@
       </c>
       <c r="AR61" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS61" t="n">
@@ -16610,7 +16626,7 @@
       </c>
       <c r="AR62" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS62" t="n">
@@ -16796,7 +16812,7 @@
       </c>
       <c r="AR63" t="inlineStr">
         <is>
-          <t>2.4</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS63" t="n">
@@ -16981,7 +16997,7 @@
       </c>
       <c r="AR64" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS64" t="n">
@@ -17158,7 +17174,7 @@
       </c>
       <c r="AR65" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS65" t="n">
@@ -17347,7 +17363,7 @@
       </c>
       <c r="AR66" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS66" t="n">
@@ -17533,11 +17549,11 @@
       </c>
       <c r="AR67" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS67" t="n">
-        <v>0.41</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="68">
@@ -17722,7 +17738,7 @@
       </c>
       <c r="AR68" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS68" t="n">
@@ -17907,7 +17923,7 @@
       </c>
       <c r="AR69" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS69" t="n">
@@ -18098,7 +18114,7 @@
       </c>
       <c r="AR70" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="AS70" t="n">
@@ -18283,7 +18299,7 @@
       </c>
       <c r="AR71" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS71" t="n">
@@ -18464,7 +18480,7 @@
       </c>
       <c r="AR72" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS72" t="n">
@@ -18657,7 +18673,7 @@
       </c>
       <c r="AR73" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="AS73" t="n">
@@ -18834,7 +18850,7 @@
       </c>
       <c r="AR74" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="AS74" t="n">
@@ -19011,7 +19027,7 @@
       </c>
       <c r="AR75" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS75" t="n">
@@ -19196,7 +19212,7 @@
       </c>
       <c r="AR76" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS76" t="n">
@@ -19381,7 +19397,7 @@
       </c>
       <c r="AR77" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS77" t="n">
@@ -19562,11 +19578,11 @@
       </c>
       <c r="AR78" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="AS78" t="n">
-        <v>0.3</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="79">
@@ -19743,7 +19759,7 @@
       </c>
       <c r="AR79" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS79" t="n">
@@ -19932,7 +19948,7 @@
       </c>
       <c r="AR80" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="AS80" t="n">
@@ -20117,7 +20133,7 @@
       </c>
       <c r="AR81" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS81" t="n">
@@ -20302,7 +20318,7 @@
       </c>
       <c r="AR82" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS82" t="n">
@@ -20487,7 +20503,7 @@
       </c>
       <c r="AR83" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS83" t="n">
@@ -20673,7 +20689,7 @@
       </c>
       <c r="AR84" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS84" t="n">
@@ -20858,7 +20874,7 @@
       </c>
       <c r="AR85" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS85" t="n">
@@ -21043,7 +21059,7 @@
       </c>
       <c r="AR86" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS86" t="n">
@@ -21233,7 +21249,7 @@
       </c>
       <c r="AR87" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="AS87" t="n">
@@ -21418,7 +21434,7 @@
       </c>
       <c r="AR88" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS88" t="n">
@@ -21603,7 +21619,7 @@
       </c>
       <c r="AR89" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS89" t="n">
@@ -21793,7 +21809,7 @@
       </c>
       <c r="AR90" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS90" t="n">
@@ -21979,11 +21995,11 @@
       </c>
       <c r="AR91" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS91" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="92">
@@ -22168,7 +22184,7 @@
       </c>
       <c r="AR92" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS92" t="n">
@@ -22345,11 +22361,11 @@
       </c>
       <c r="AR93" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS93" t="n">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="94">
@@ -22535,11 +22551,11 @@
       </c>
       <c r="AR94" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>17.0</t>
         </is>
       </c>
       <c r="AS94" t="n">
-        <v>0.3</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="95">
@@ -22720,7 +22736,7 @@
       </c>
       <c r="AR95" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS95" t="n">
@@ -22910,7 +22926,7 @@
       </c>
       <c r="AR96" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS96" t="n">
@@ -23088,11 +23104,11 @@
       </c>
       <c r="AR97" t="inlineStr">
         <is>
-          <t>20.2</t>
+          <t>18.2</t>
         </is>
       </c>
       <c r="AS97" t="n">
-        <v>0.39</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="98">
@@ -23267,11 +23283,11 @@
       </c>
       <c r="AR98" t="inlineStr">
         <is>
-          <t>20.2</t>
+          <t>18.0</t>
         </is>
       </c>
       <c r="AS98" t="n">
-        <v>0.39</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="99">
@@ -23437,7 +23453,7 @@
       </c>
       <c r="AR99" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS99" t="n">
@@ -23616,7 +23632,7 @@
       </c>
       <c r="AR100" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS100" t="n">
@@ -23801,7 +23817,7 @@
       </c>
       <c r="AR101" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>8.6</t>
         </is>
       </c>
       <c r="AS101" t="n">
@@ -23992,7 +24008,7 @@
       </c>
       <c r="AR102" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS102" t="n">
@@ -24165,7 +24181,7 @@
       </c>
       <c r="AR103" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="AS103" t="n">
@@ -24342,7 +24358,7 @@
       </c>
       <c r="AR104" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS104" t="n">
@@ -24522,11 +24538,11 @@
       </c>
       <c r="AR105" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="AS105" t="n">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="106">
@@ -24735,7 +24751,7 @@
       </c>
       <c r="AR106" t="inlineStr">
         <is>
-          <t>2.4</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS106" t="n">
@@ -24928,11 +24944,11 @@
       </c>
       <c r="AR107" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS107" t="n">
-        <v>0.58</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="108">
@@ -25116,11 +25132,11 @@
       </c>
       <c r="AR108" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>8.9</t>
         </is>
       </c>
       <c r="AS108" t="n">
-        <v>0.44</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="109">
@@ -25305,7 +25321,7 @@
       </c>
       <c r="AR109" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS109" t="n">
@@ -25497,7 +25513,7 @@
       </c>
       <c r="AR110" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS110" t="n">
@@ -25682,7 +25698,7 @@
       </c>
       <c r="AR111" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS111" t="n">
@@ -25873,7 +25889,7 @@
       </c>
       <c r="AR112" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS112" t="n">
@@ -26058,7 +26074,7 @@
       </c>
       <c r="AR113" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS113" t="n">
@@ -26243,7 +26259,7 @@
       </c>
       <c r="AR114" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS114" t="n">
@@ -26428,7 +26444,7 @@
       </c>
       <c r="AR115" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS115" t="n">
@@ -26617,11 +26633,11 @@
       </c>
       <c r="AR116" t="inlineStr">
         <is>
-          <t>2.4</t>
+          <t>15.1</t>
         </is>
       </c>
       <c r="AS116" t="n">
-        <v>0.3</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="117">
@@ -26802,7 +26818,7 @@
       </c>
       <c r="AR117" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS117" t="n">
@@ -26979,7 +26995,7 @@
       </c>
       <c r="AR118" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS118" t="n">
@@ -27164,7 +27180,7 @@
       </c>
       <c r="AR119" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>8.6</t>
         </is>
       </c>
       <c r="AS119" t="n">
@@ -27343,7 +27359,7 @@
       </c>
       <c r="AR120" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS120" t="n">
@@ -27524,11 +27540,11 @@
       </c>
       <c r="AR121" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS121" t="n">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="122">
@@ -27714,7 +27730,7 @@
       </c>
       <c r="AR122" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS122" t="n">
@@ -27903,7 +27919,7 @@
       </c>
       <c r="AR123" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS123" t="n">
@@ -28088,7 +28104,7 @@
       </c>
       <c r="AR124" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS124" t="n">
@@ -28273,7 +28289,7 @@
       </c>
       <c r="AR125" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS125" t="n">
@@ -28463,7 +28479,7 @@
       </c>
       <c r="AR126" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS126" t="n">
@@ -28648,7 +28664,7 @@
       </c>
       <c r="AR127" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS127" t="n">
@@ -28841,11 +28857,11 @@
       </c>
       <c r="AR128" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>11.2</t>
         </is>
       </c>
       <c r="AS128" t="n">
-        <v>0.3</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="129">
@@ -29042,7 +29058,7 @@
       </c>
       <c r="AR129" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="AS129" t="n">
@@ -29235,11 +29251,11 @@
       </c>
       <c r="AR130" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>13.5</t>
         </is>
       </c>
       <c r="AS130" t="n">
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="131">
@@ -29433,7 +29449,7 @@
       </c>
       <c r="AR131" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS131" t="n">
@@ -29631,7 +29647,7 @@
       </c>
       <c r="AR132" t="inlineStr">
         <is>
-          <t>13.3</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="AS132" t="n">
@@ -29820,7 +29836,7 @@
       </c>
       <c r="AR133" t="inlineStr">
         <is>
-          <t>18.1</t>
+          <t>13.8</t>
         </is>
       </c>
       <c r="AS133" t="n">
@@ -30005,7 +30021,7 @@
       </c>
       <c r="AR134" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS134" t="n">
@@ -30190,7 +30206,7 @@
       </c>
       <c r="AR135" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS135" t="n">
@@ -30379,7 +30395,7 @@
       </c>
       <c r="AR136" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS136" t="n">
@@ -30564,7 +30580,7 @@
       </c>
       <c r="AR137" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS137" t="n">
@@ -30737,11 +30753,11 @@
       </c>
       <c r="AR138" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS138" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="139">
@@ -30914,11 +30930,11 @@
       </c>
       <c r="AR139" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS139" t="n">
-        <v>0.45</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="140">
@@ -31107,7 +31123,7 @@
       </c>
       <c r="AR140" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS140" t="n">
@@ -31293,7 +31309,7 @@
       </c>
       <c r="AR141" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS141" t="n">
@@ -31479,7 +31495,7 @@
       </c>
       <c r="AR142" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS142" t="n">
@@ -31665,7 +31681,7 @@
       </c>
       <c r="AR143" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS143" t="n">
@@ -31855,7 +31871,7 @@
       </c>
       <c r="AR144" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS144" t="n">
@@ -32036,7 +32052,7 @@
       </c>
       <c r="AR145" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS145" t="n">
@@ -32225,7 +32241,7 @@
       </c>
       <c r="AR146" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS146" t="n">
@@ -32410,7 +32426,7 @@
       </c>
       <c r="AR147" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="AS147" t="n">
@@ -32595,7 +32611,7 @@
       </c>
       <c r="AR148" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS148" t="n">
@@ -32780,7 +32796,7 @@
       </c>
       <c r="AR149" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="AS149" t="n">
@@ -32974,11 +32990,11 @@
       </c>
       <c r="AR150" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>10.3</t>
         </is>
       </c>
       <c r="AS150" t="n">
-        <v>0.53</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="151">
@@ -33171,7 +33187,7 @@
       </c>
       <c r="AR151" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS151" t="n">
@@ -33356,7 +33372,7 @@
       </c>
       <c r="AR152" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS152" t="n">
@@ -33533,11 +33549,11 @@
       </c>
       <c r="AR153" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS153" t="n">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="154">
@@ -33718,7 +33734,7 @@
       </c>
       <c r="AR154" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS154" t="n">
@@ -33903,7 +33919,7 @@
       </c>
       <c r="AR155" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="AS155" t="n">
@@ -34093,7 +34109,7 @@
       </c>
       <c r="AR156" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS156" t="n">
@@ -34283,7 +34299,7 @@
       </c>
       <c r="AR157" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS157" t="n">
@@ -34469,7 +34485,7 @@
       </c>
       <c r="AR158" t="inlineStr">
         <is>
-          <t>13.7</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS158" t="n">
@@ -34654,7 +34670,7 @@
       </c>
       <c r="AR159" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS159" t="n">
@@ -34831,7 +34847,7 @@
       </c>
       <c r="AR160" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS160" t="n">
@@ -35021,7 +35037,7 @@
       </c>
       <c r="AR161" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS161" t="n">
@@ -35198,7 +35214,7 @@
       </c>
       <c r="AR162" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS162" t="n">
@@ -35375,7 +35391,7 @@
       </c>
       <c r="AR163" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS163" t="n">
@@ -35583,7 +35599,7 @@
       </c>
       <c r="AR164" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS164" t="n">
@@ -35768,7 +35784,7 @@
       </c>
       <c r="AR165" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="AS165" t="n">
@@ -35965,11 +35981,11 @@
       </c>
       <c r="AR166" t="inlineStr">
         <is>
-          <t>9.6</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="AS166" t="n">
-        <v>0.37</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="167">
@@ -36154,7 +36170,7 @@
       </c>
       <c r="AR167" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS167" t="n">
@@ -36339,7 +36355,7 @@
       </c>
       <c r="AR168" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS168" t="n">
@@ -36529,11 +36545,11 @@
       </c>
       <c r="AR169" t="inlineStr">
         <is>
-          <t>15.1</t>
+          <t>16.7</t>
         </is>
       </c>
       <c r="AS169" t="n">
-        <v>0.68</v>
+        <v>0.71</v>
       </c>
     </row>
     <row r="170">
@@ -36718,7 +36734,7 @@
       </c>
       <c r="AR170" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="AS170" t="n">
@@ -36895,11 +36911,11 @@
       </c>
       <c r="AR171" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="AS171" t="n">
-        <v>0.43</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="172">
@@ -37080,7 +37096,7 @@
       </c>
       <c r="AR172" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="AS172" t="n">
@@ -37257,11 +37273,11 @@
       </c>
       <c r="AR173" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>9.5</t>
         </is>
       </c>
       <c r="AS173" t="n">
-        <v>0.3</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="174">
@@ -37443,11 +37459,11 @@
       </c>
       <c r="AR174" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS174" t="n">
-        <v>0.3</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="175">
@@ -37632,7 +37648,7 @@
       </c>
       <c r="AR175" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="AS175" t="n">
@@ -37809,11 +37825,11 @@
       </c>
       <c r="AR176" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS176" t="n">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="177">
@@ -37998,7 +38014,7 @@
       </c>
       <c r="AR177" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS177" t="n">
@@ -38187,7 +38203,7 @@
       </c>
       <c r="AR178" t="inlineStr">
         <is>
-          <t>10.7</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS178" t="n">
@@ -38380,7 +38396,7 @@
       </c>
       <c r="AR179" t="inlineStr">
         <is>
-          <t>14.7</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="AS179" t="n">
@@ -38574,7 +38590,7 @@
       </c>
       <c r="AR180" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="AS180" t="n">
@@ -38764,7 +38780,7 @@
       </c>
       <c r="AR181" t="inlineStr">
         <is>
-          <t>10.7</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="AS181" t="n">
@@ -38957,11 +38973,11 @@
       </c>
       <c r="AR182" t="inlineStr">
         <is>
-          <t>17.8</t>
+          <t>16.9</t>
         </is>
       </c>
       <c r="AS182" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="183">
@@ -39150,11 +39166,11 @@
       </c>
       <c r="AR183" t="inlineStr">
         <is>
-          <t>20.2</t>
+          <t>18.0</t>
         </is>
       </c>
       <c r="AS183" t="n">
-        <v>0.39</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="184">
@@ -39339,11 +39355,11 @@
       </c>
       <c r="AR184" t="inlineStr">
         <is>
-          <t>17.8</t>
+          <t>16.9</t>
         </is>
       </c>
       <c r="AS184" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="185">
@@ -39533,7 +39549,7 @@
       </c>
       <c r="AR185" t="inlineStr">
         <is>
-          <t>10.7</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS185" t="n">
@@ -39727,7 +39743,7 @@
       </c>
       <c r="AR186" t="inlineStr">
         <is>
-          <t>14.1</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="AS186" t="n">
@@ -39905,11 +39921,11 @@
       </c>
       <c r="AR187" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS187" t="n">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="188">
@@ -40102,7 +40118,7 @@
       </c>
       <c r="AR188" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS188" t="n">
@@ -40287,11 +40303,11 @@
       </c>
       <c r="AR189" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="AS189" t="n">
-        <v>0.38</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="190">
@@ -40476,7 +40492,7 @@
       </c>
       <c r="AR190" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS190" t="n">
@@ -40649,11 +40665,11 @@
       </c>
       <c r="AR191" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="AS191" t="n">
-        <v>0.3</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="192">
@@ -40839,11 +40855,11 @@
       </c>
       <c r="AR192" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>18.0</t>
         </is>
       </c>
       <c r="AS192" t="n">
-        <v>0.3</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="193">
@@ -41029,7 +41045,7 @@
       </c>
       <c r="AR193" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS193" t="n">
@@ -41202,11 +41218,11 @@
       </c>
       <c r="AR194" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="AS194" t="n">
-        <v>0.53</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="195">
@@ -41375,11 +41391,11 @@
       </c>
       <c r="AR195" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="AS195" t="n">
-        <v>0.53</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="196">
@@ -41552,11 +41568,11 @@
       </c>
       <c r="AR196" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>8.9</t>
         </is>
       </c>
       <c r="AS196" t="n">
-        <v>0.44</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="197">
@@ -41725,11 +41741,11 @@
       </c>
       <c r="AR197" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="AS197" t="n">
-        <v>0.49</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="198">
@@ -41898,11 +41914,11 @@
       </c>
       <c r="AR198" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS198" t="n">
-        <v>0.32</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="199">
@@ -42075,11 +42091,11 @@
       </c>
       <c r="AR199" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>8.4</t>
         </is>
       </c>
       <c r="AS199" t="n">
-        <v>0.38</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="200">
@@ -42265,7 +42281,7 @@
       </c>
       <c r="AR200" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS200" t="n">
@@ -42455,7 +42471,7 @@
       </c>
       <c r="AR201" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS201" t="n">
@@ -42645,7 +42661,7 @@
       </c>
       <c r="AR202" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS202" t="n">
@@ -42835,7 +42851,7 @@
       </c>
       <c r="AR203" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS203" t="n">
@@ -43021,7 +43037,7 @@
       </c>
       <c r="AR204" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS204" t="n">
@@ -43207,7 +43223,7 @@
       </c>
       <c r="AR205" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS205" t="n">
@@ -43391,7 +43407,7 @@
       </c>
       <c r="AR206" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="AS206" t="n">
@@ -43581,7 +43597,7 @@
       </c>
       <c r="AR207" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS207" t="n">
@@ -43770,11 +43786,11 @@
       </c>
       <c r="AR208" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="AS208" t="n">
-        <v>0.35</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="209">
@@ -43959,11 +43975,11 @@
       </c>
       <c r="AR209" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>9.4</t>
         </is>
       </c>
       <c r="AS209" t="n">
-        <v>0.3</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="210">
@@ -44144,11 +44160,11 @@
       </c>
       <c r="AR210" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="AS210" t="n">
-        <v>0.54</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="211">
@@ -44333,11 +44349,11 @@
       </c>
       <c r="AR211" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS211" t="n">
-        <v>0.3</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="212">
@@ -44526,11 +44542,11 @@
       </c>
       <c r="AR212" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS212" t="n">
-        <v>0.5</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="213">
@@ -44716,7 +44732,7 @@
       </c>
       <c r="AR213" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS213" t="n">
@@ -44906,7 +44922,7 @@
       </c>
       <c r="AR214" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS214" t="n">
@@ -45096,7 +45112,7 @@
       </c>
       <c r="AR215" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS215" t="n">
@@ -45287,7 +45303,7 @@
       </c>
       <c r="AR216" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS216" t="n">
@@ -45464,11 +45480,11 @@
       </c>
       <c r="AR217" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="AS217" t="n">
-        <v>0.43</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="218">
@@ -45642,11 +45658,11 @@
       </c>
       <c r="AR218" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS218" t="n">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="219">
@@ -45827,11 +45843,11 @@
       </c>
       <c r="AR219" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>11.8</t>
         </is>
       </c>
       <c r="AS219" t="n">
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="220">
@@ -46004,11 +46020,11 @@
       </c>
       <c r="AR220" t="inlineStr">
         <is>
-          <t>10.0</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS220" t="n">
-        <v>0.39</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="221">
@@ -46193,7 +46209,7 @@
       </c>
       <c r="AR221" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS221" t="n">
@@ -46378,7 +46394,7 @@
       </c>
       <c r="AR222" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS222" t="n">
@@ -46567,7 +46583,7 @@
       </c>
       <c r="AR223" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS223" t="n">
@@ -46752,7 +46768,7 @@
       </c>
       <c r="AR224" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS224" t="n">
@@ -46942,7 +46958,7 @@
       </c>
       <c r="AR225" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="AS225" t="n">
@@ -47119,7 +47135,7 @@
       </c>
       <c r="AR226" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS226" t="n">
@@ -47297,11 +47313,11 @@
       </c>
       <c r="AR227" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS227" t="n">
-        <v>0.3</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="228">
@@ -47487,7 +47503,7 @@
       </c>
       <c r="AR228" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS228" t="n">
@@ -47665,11 +47681,11 @@
       </c>
       <c r="AR229" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS229" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="230">
@@ -47858,11 +47874,11 @@
       </c>
       <c r="AR230" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="AS230" t="n">
-        <v>0.35</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="231">
@@ -48048,7 +48064,7 @@
       </c>
       <c r="AR231" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS231" t="n">
@@ -48237,7 +48253,7 @@
       </c>
       <c r="AR232" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS232" t="n">
@@ -48418,7 +48434,7 @@
       </c>
       <c r="AR233" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>8.6</t>
         </is>
       </c>
       <c r="AS233" t="n">
@@ -48607,7 +48623,7 @@
       </c>
       <c r="AR234" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS234" t="n">
@@ -48796,7 +48812,7 @@
       </c>
       <c r="AR235" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS235" t="n">
@@ -48985,7 +49001,7 @@
       </c>
       <c r="AR236" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="AS236" t="n">
@@ -49174,7 +49190,7 @@
       </c>
       <c r="AR237" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS237" t="n">
@@ -49363,7 +49379,7 @@
       </c>
       <c r="AR238" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS238" t="n">
@@ -49552,11 +49568,11 @@
       </c>
       <c r="AR239" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS239" t="n">
-        <v>0.3</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="240">
@@ -49737,7 +49753,7 @@
       </c>
       <c r="AR240" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS240" t="n">
@@ -49914,11 +49930,11 @@
       </c>
       <c r="AR241" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS241" t="n">
-        <v>0.32</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="242">
@@ -50099,7 +50115,7 @@
       </c>
       <c r="AR242" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS242" t="n">
@@ -50288,7 +50304,7 @@
       </c>
       <c r="AR243" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS243" t="n">
@@ -50477,7 +50493,7 @@
       </c>
       <c r="AR244" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS244" t="n">
@@ -50662,11 +50678,11 @@
       </c>
       <c r="AR245" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS245" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="246">
@@ -50851,7 +50867,7 @@
       </c>
       <c r="AR246" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS246" t="n">
@@ -51028,7 +51044,7 @@
       </c>
       <c r="AR247" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS247" t="n">
@@ -51197,11 +51213,11 @@
       </c>
       <c r="AR248" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="AS248" t="n">
-        <v>0.3</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="249">
@@ -51376,11 +51392,11 @@
       </c>
       <c r="AR249" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS249" t="n">
-        <v>0.3</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="250">
@@ -51554,11 +51570,11 @@
       </c>
       <c r="AR250" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS250" t="n">
-        <v>0.3</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="251">
@@ -51732,11 +51748,11 @@
       </c>
       <c r="AR251" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS251" t="n">
-        <v>0.31</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="252">
@@ -51933,7 +51949,7 @@
       </c>
       <c r="AR252" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS252" t="n">
@@ -52110,11 +52126,11 @@
       </c>
       <c r="AR253" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="AS253" t="n">
-        <v>0.3</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="254">
@@ -52299,11 +52315,11 @@
       </c>
       <c r="AR254" t="inlineStr">
         <is>
-          <t>16.5</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="AS254" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="255">
@@ -52484,11 +52500,11 @@
       </c>
       <c r="AR255" t="inlineStr">
         <is>
-          <t>10.6</t>
+          <t>11.5</t>
         </is>
       </c>
       <c r="AS255" t="n">
-        <v>0.42</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="256">
@@ -52673,7 +52689,7 @@
       </c>
       <c r="AR256" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="AS256" t="n">
@@ -52866,7 +52882,7 @@
       </c>
       <c r="AR257" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="AS257" t="n">
@@ -53059,7 +53075,7 @@
       </c>
       <c r="AR258" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="AS258" t="n">
@@ -53252,7 +53268,7 @@
       </c>
       <c r="AR259" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="AS259" t="n">
@@ -53446,7 +53462,7 @@
       </c>
       <c r="AR260" t="inlineStr">
         <is>
-          <t>14.0</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS260" t="n">
@@ -53639,7 +53655,7 @@
       </c>
       <c r="AR261" t="inlineStr">
         <is>
-          <t>10.7</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS261" t="n">
@@ -53828,11 +53844,11 @@
       </c>
       <c r="AR262" t="inlineStr">
         <is>
-          <t>16.5</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS262" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="263">
@@ -54013,11 +54029,11 @@
       </c>
       <c r="AR263" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS263" t="n">
-        <v>0.3</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="264">
@@ -54202,11 +54218,11 @@
       </c>
       <c r="AR264" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>18.0</t>
         </is>
       </c>
       <c r="AS264" t="n">
-        <v>0.3</v>
+        <v>0.73</v>
       </c>
     </row>
     <row r="265">
@@ -54395,7 +54411,7 @@
       </c>
       <c r="AR265" t="inlineStr">
         <is>
-          <t>10.7</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS265" t="n">
@@ -54589,7 +54605,7 @@
       </c>
       <c r="AR266" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS266" t="n">
@@ -54778,11 +54794,11 @@
       </c>
       <c r="AR267" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="AS267" t="n">
-        <v>0.3</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="268">
@@ -54963,11 +54979,11 @@
       </c>
       <c r="AR268" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="AS268" t="n">
-        <v>0.58</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="269">
@@ -55149,11 +55165,11 @@
       </c>
       <c r="AR269" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS269" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="270">
@@ -55335,11 +55351,11 @@
       </c>
       <c r="AR270" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS270" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="271">
@@ -55525,7 +55541,7 @@
       </c>
       <c r="AR271" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="AS271" t="n">
@@ -55715,7 +55731,7 @@
       </c>
       <c r="AR272" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS272" t="n">
@@ -55905,7 +55921,7 @@
       </c>
       <c r="AR273" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS273" t="n">
@@ -56091,11 +56107,11 @@
       </c>
       <c r="AR274" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>8.1</t>
         </is>
       </c>
       <c r="AS274" t="n">
-        <v>0.37</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="275">
@@ -56284,7 +56300,7 @@
       </c>
       <c r="AR275" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="AS275" t="n">
@@ -56474,11 +56490,11 @@
       </c>
       <c r="AR276" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS276" t="n">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="277">
@@ -56663,7 +56679,7 @@
       </c>
       <c r="AR277" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS277" t="n">
@@ -56848,7 +56864,7 @@
       </c>
       <c r="AR278" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS278" t="n">
@@ -57037,7 +57053,7 @@
       </c>
       <c r="AR279" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS279" t="n">
@@ -57223,7 +57239,7 @@
       </c>
       <c r="AR280" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS280" t="n">
@@ -57412,7 +57428,7 @@
       </c>
       <c r="AR281" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS281" t="n">
@@ -57601,7 +57617,7 @@
       </c>
       <c r="AR282" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS282" t="n">
@@ -57790,7 +57806,7 @@
       </c>
       <c r="AR283" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS283" t="n">
@@ -57975,7 +57991,7 @@
       </c>
       <c r="AR284" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS284" t="n">
@@ -58160,7 +58176,7 @@
       </c>
       <c r="AR285" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS285" t="n">
@@ -58349,7 +58365,7 @@
       </c>
       <c r="AR286" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS286" t="n">
@@ -58534,7 +58550,7 @@
       </c>
       <c r="AR287" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS287" t="n">
@@ -58721,7 +58737,7 @@
       </c>
       <c r="AR288" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS288" t="n">
@@ -58910,11 +58926,11 @@
       </c>
       <c r="AR289" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>14.4</t>
         </is>
       </c>
       <c r="AS289" t="n">
-        <v>0.3</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="290">
@@ -59095,11 +59111,11 @@
       </c>
       <c r="AR290" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS290" t="n">
-        <v>0.41</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="291">
@@ -59280,7 +59296,7 @@
       </c>
       <c r="AR291" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>7.2</t>
         </is>
       </c>
       <c r="AS291" t="n">
@@ -59466,11 +59482,11 @@
       </c>
       <c r="AR292" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>11.7</t>
         </is>
       </c>
       <c r="AS292" t="n">
-        <v>0.53</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="293">
@@ -59651,11 +59667,11 @@
       </c>
       <c r="AR293" t="inlineStr">
         <is>
-          <t>2.2</t>
+          <t>14.4</t>
         </is>
       </c>
       <c r="AS293" t="n">
-        <v>0.3</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="294">
@@ -59820,7 +59836,7 @@
       </c>
       <c r="AR294" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS294" t="n">
@@ -60010,11 +60026,11 @@
       </c>
       <c r="AR295" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS295" t="n">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="296">
@@ -60197,11 +60213,11 @@
       </c>
       <c r="AR296" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="AS296" t="n">
-        <v>0.3</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="297">
@@ -60387,7 +60403,7 @@
       </c>
       <c r="AR297" t="inlineStr">
         <is>
-          <t>2.1</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS297" t="n">
@@ -60573,11 +60589,11 @@
       </c>
       <c r="AR298" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="AS298" t="n">
-        <v>0.37</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="299">
@@ -60746,11 +60762,11 @@
       </c>
       <c r="AR299" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS299" t="n">
-        <v>0.47</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="300">
@@ -60915,11 +60931,11 @@
       </c>
       <c r="AR300" t="inlineStr">
         <is>
-          <t>16.5</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS300" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="301">
@@ -61088,11 +61104,11 @@
       </c>
       <c r="AR301" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="AS301" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="302">
@@ -61261,11 +61277,11 @@
       </c>
       <c r="AR302" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="AS302" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="303">
@@ -61430,11 +61446,11 @@
       </c>
       <c r="AR303" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="AS303" t="n">
-        <v>0.63</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="304">
@@ -61599,11 +61615,11 @@
       </c>
       <c r="AR304" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS304" t="n">
-        <v>0.6</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="305">
@@ -61772,7 +61788,7 @@
         </is>
       </c>
       <c r="AS305" t="n">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="306">
@@ -61953,7 +61969,7 @@
       </c>
       <c r="AR306" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS306" t="n">
@@ -62138,7 +62154,7 @@
       </c>
       <c r="AR307" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS307" t="n">
@@ -62323,7 +62339,7 @@
       </c>
       <c r="AR308" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS308" t="n">
@@ -62508,7 +62524,7 @@
       </c>
       <c r="AR309" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS309" t="n">
@@ -62701,7 +62717,7 @@
       </c>
       <c r="AR310" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="AS310" t="n">
@@ -62894,7 +62910,7 @@
       </c>
       <c r="AR311" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS311" t="n">
@@ -63067,11 +63083,11 @@
       </c>
       <c r="AR312" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="AS312" t="n">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="313">
@@ -63244,7 +63260,7 @@
       </c>
       <c r="AR313" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS313" t="n">
@@ -63421,11 +63437,11 @@
       </c>
       <c r="AR314" t="inlineStr">
         <is>
-          <t>11.3</t>
+          <t>10.8</t>
         </is>
       </c>
       <c r="AS314" t="n">
-        <v>0.45</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="315">
@@ -63600,11 +63616,11 @@
       </c>
       <c r="AR315" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS315" t="n">
-        <v>0.3</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="316">
@@ -63790,7 +63806,7 @@
       </c>
       <c r="AR316" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS316" t="n">
@@ -63968,7 +63984,7 @@
       </c>
       <c r="AR317" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="AS317" t="n">
@@ -64158,11 +64174,11 @@
       </c>
       <c r="AR318" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS318" t="n">
-        <v>0.44</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="319">
@@ -64351,7 +64367,7 @@
       </c>
       <c r="AR319" t="inlineStr">
         <is>
-          <t>14.4</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS319" t="n">
@@ -64540,7 +64556,7 @@
       </c>
       <c r="AR320" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS320" t="n">
@@ -64733,7 +64749,7 @@
       </c>
       <c r="AR321" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="AS321" t="n">
@@ -64918,7 +64934,7 @@
       </c>
       <c r="AR322" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS322" t="n">
@@ -65111,7 +65127,7 @@
       </c>
       <c r="AR323" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS323" t="n">
@@ -65300,11 +65316,11 @@
       </c>
       <c r="AR324" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="AS324" t="n">
-        <v>0.53</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="325">
@@ -65490,7 +65506,7 @@
       </c>
       <c r="AR325" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS325" t="n">
@@ -65659,11 +65675,11 @@
       </c>
       <c r="AR326" t="inlineStr">
         <is>
-          <t>11.3</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="AS326" t="n">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="327">
@@ -65848,7 +65864,7 @@
       </c>
       <c r="AR327" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS327" t="n">
@@ -66041,7 +66057,7 @@
       </c>
       <c r="AR328" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS328" t="n">
@@ -66227,11 +66243,11 @@
       </c>
       <c r="AR329" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS329" t="n">
-        <v>0.33</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="330">
@@ -66416,7 +66432,7 @@
       </c>
       <c r="AR330" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS330" t="n">
@@ -66612,11 +66628,11 @@
       </c>
       <c r="AR331" t="inlineStr">
         <is>
-          <t>20.2</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS331" t="n">
-        <v>0.39</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="332">
@@ -66803,7 +66819,7 @@
       </c>
       <c r="AR332" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS332" t="n">
@@ -66976,11 +66992,11 @@
       </c>
       <c r="AR333" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS333" t="n">
-        <v>0.3</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="334">
@@ -67145,7 +67161,7 @@
       </c>
       <c r="AR334" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS334" t="n">
@@ -67314,7 +67330,7 @@
       </c>
       <c r="AR335" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS335" t="n">
@@ -67499,7 +67515,7 @@
       </c>
       <c r="AR336" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS336" t="n">
@@ -67684,11 +67700,11 @@
       </c>
       <c r="AR337" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="AS337" t="n">
-        <v>0.43</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="338">
@@ -67869,7 +67885,7 @@
       </c>
       <c r="AR338" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>10.0</t>
         </is>
       </c>
       <c r="AS338" t="n">
@@ -68055,11 +68071,11 @@
       </c>
       <c r="AR339" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="AS339" t="n">
-        <v>0.3</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="340">
@@ -68236,7 +68252,7 @@
       </c>
       <c r="AR340" t="inlineStr">
         <is>
-          <t>1.7</t>
+          <t>2.4</t>
         </is>
       </c>
       <c r="AS340" t="n">
@@ -68422,7 +68438,7 @@
       </c>
       <c r="AR341" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS341" t="n">
@@ -68617,7 +68633,7 @@
       </c>
       <c r="AR342" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="AS342" t="n">
@@ -68813,7 +68829,7 @@
       </c>
       <c r="AR343" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="AS343" t="n">
@@ -68982,11 +68998,11 @@
       </c>
       <c r="AR344" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>9.9</t>
         </is>
       </c>
       <c r="AS344" t="n">
-        <v>0.3</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="345">
@@ -69169,7 +69185,7 @@
       </c>
       <c r="AR345" t="inlineStr">
         <is>
-          <t>14.0</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS345" t="n">
@@ -69355,7 +69371,7 @@
       </c>
       <c r="AR346" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS346" t="n">
@@ -69541,7 +69557,7 @@
       </c>
       <c r="AR347" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="AS347" t="n">
@@ -69710,11 +69726,11 @@
       </c>
       <c r="AR348" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="AS348" t="n">
-        <v>0.59</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="349">
@@ -69879,7 +69895,7 @@
       </c>
       <c r="AR349" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS349" t="n">
@@ -70048,11 +70064,11 @@
       </c>
       <c r="AR350" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS350" t="n">
-        <v>0.57</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="351">
@@ -70217,11 +70233,11 @@
       </c>
       <c r="AR351" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS351" t="n">
-        <v>0.57</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="352">
@@ -70386,7 +70402,7 @@
       </c>
       <c r="AR352" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="AS352" t="n">
@@ -70555,11 +70571,11 @@
       </c>
       <c r="AR353" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="AS353" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="354">
@@ -70744,7 +70760,7 @@
       </c>
       <c r="AR354" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS354" t="n">
@@ -70921,7 +70937,7 @@
       </c>
       <c r="AR355" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS355" t="n">
@@ -71107,7 +71123,7 @@
       </c>
       <c r="AR356" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS356" t="n">
@@ -71285,11 +71301,11 @@
       </c>
       <c r="AR357" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS357" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="358">
@@ -71463,7 +71479,7 @@
       </c>
       <c r="AR358" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS358" t="n">
@@ -71649,7 +71665,7 @@
       </c>
       <c r="AR359" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS359" t="n">
@@ -71834,7 +71850,7 @@
       </c>
       <c r="AR360" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS360" t="n">
@@ -72007,11 +72023,11 @@
       </c>
       <c r="AR361" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS361" t="n">
-        <v>0.3</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="362">
@@ -72184,11 +72200,11 @@
       </c>
       <c r="AR362" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>11.0</t>
         </is>
       </c>
       <c r="AS362" t="n">
-        <v>0.35</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="363">
@@ -72362,11 +72378,11 @@
       </c>
       <c r="AR363" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS363" t="n">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="364">
@@ -72548,7 +72564,7 @@
       </c>
       <c r="AR364" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS364" t="n">
@@ -72741,7 +72757,7 @@
       </c>
       <c r="AR365" t="inlineStr">
         <is>
-          <t>11.1</t>
+          <t>11.9</t>
         </is>
       </c>
       <c r="AS365" t="n">
@@ -72934,7 +72950,7 @@
       </c>
       <c r="AR366" t="inlineStr">
         <is>
-          <t>11.1</t>
+          <t>11.9</t>
         </is>
       </c>
       <c r="AS366" t="n">
@@ -73127,7 +73143,7 @@
       </c>
       <c r="AR367" t="inlineStr">
         <is>
-          <t>13.7</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS367" t="n">
@@ -73304,7 +73320,7 @@
       </c>
       <c r="AR368" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="AS368" t="n">
@@ -73481,7 +73497,7 @@
       </c>
       <c r="AR369" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS369" t="n">
@@ -73661,11 +73677,11 @@
       </c>
       <c r="AR370" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="AS370" t="n">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="371">
@@ -73838,7 +73854,7 @@
       </c>
       <c r="AR371" t="inlineStr">
         <is>
-          <t>10.7</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS371" t="n">
@@ -74016,11 +74032,11 @@
       </c>
       <c r="AR372" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS372" t="n">
-        <v>0.3</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="373">
@@ -74210,7 +74226,7 @@
       </c>
       <c r="AR373" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="AS373" t="n">
@@ -74390,11 +74406,11 @@
       </c>
       <c r="AR374" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS374" t="n">
-        <v>0.3</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="375">
@@ -74570,11 +74586,11 @@
       </c>
       <c r="AR375" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS375" t="n">
-        <v>0.3</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="376">
@@ -74767,7 +74783,7 @@
       </c>
       <c r="AR376" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS376" t="n">
@@ -74952,7 +74968,7 @@
       </c>
       <c r="AR377" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="AS377" t="n">
@@ -75138,7 +75154,7 @@
       </c>
       <c r="AR378" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS378" t="n">
@@ -75316,11 +75332,11 @@
       </c>
       <c r="AR379" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS379" t="n">
-        <v>0.45</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="380">
@@ -75493,7 +75509,7 @@
       </c>
       <c r="AR380" t="inlineStr">
         <is>
-          <t>11.1</t>
+          <t>11.9</t>
         </is>
       </c>
       <c r="AS380" t="n">
@@ -75670,7 +75686,7 @@
       </c>
       <c r="AR381" t="inlineStr">
         <is>
-          <t>11.1</t>
+          <t>11.9</t>
         </is>
       </c>
       <c r="AS381" t="n">
@@ -75847,7 +75863,7 @@
       </c>
       <c r="AR382" t="inlineStr">
         <is>
-          <t>11.1</t>
+          <t>11.9</t>
         </is>
       </c>
       <c r="AS382" t="n">
@@ -76024,7 +76040,7 @@
       </c>
       <c r="AR383" t="inlineStr">
         <is>
-          <t>10.7</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS383" t="n">
@@ -76201,7 +76217,7 @@
       </c>
       <c r="AR384" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS384" t="n">
@@ -76378,7 +76394,7 @@
       </c>
       <c r="AR385" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="AS385" t="n">
@@ -76556,11 +76572,11 @@
       </c>
       <c r="AR386" t="inlineStr">
         <is>
-          <t>10.6</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS386" t="n">
-        <v>0.42</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="387">
@@ -76733,7 +76749,7 @@
       </c>
       <c r="AR387" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS387" t="n">
@@ -76910,11 +76926,11 @@
       </c>
       <c r="AR388" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS388" t="n">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="389">
@@ -77080,11 +77096,11 @@
       </c>
       <c r="AR389" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS389" t="n">
-        <v>0.41</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="390">
@@ -77258,11 +77274,11 @@
       </c>
       <c r="AR390" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS390" t="n">
-        <v>0.3</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="391">
@@ -77444,11 +77460,11 @@
       </c>
       <c r="AR391" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS391" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="392">
@@ -77622,7 +77638,7 @@
       </c>
       <c r="AR392" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="AS392" t="n">
@@ -77808,11 +77824,11 @@
       </c>
       <c r="AR393" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS393" t="n">
-        <v>0.3</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="394">
@@ -77985,7 +78001,7 @@
       </c>
       <c r="AR394" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="AS394" t="n">
@@ -78162,7 +78178,7 @@
       </c>
       <c r="AR395" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>7.0</t>
         </is>
       </c>
       <c r="AS395" t="n">
@@ -78355,7 +78371,7 @@
       </c>
       <c r="AR396" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS396" t="n">
@@ -78532,7 +78548,7 @@
       </c>
       <c r="AR397" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="AS397" t="n">
@@ -78610,36 +78626,36 @@
     <row r="7" ht="90" customHeight="1">
       <c r="A7" s="111" t="inlineStr">
         <is>
-          <t>The chart illustrates the Friction Pareto Analysis of an 80/20 Rule Application, showcasing the distribution of friction points across various categories. | Key: The top two categories, Scheduling &amp; Planning and Configuration &amp; Data, account for a significant proportion of friction points, with 7230 and 6130 points, respectively. | Action: Focusing on optimizing the top two categories, Scheduling &amp; Planning and Configuration &amp; Data, could potentially yield the most significant reductions in friction points, given their substantial contribution to the overall total.</t>
+          <t>The chart presents a Friction Pareto Analysis of an 80/20 Rule Application, illustrating the distribution of friction points across various categories. | Key: The top two categories, Scheduling &amp; Planning and Configuration &amp; Data, account for a significant proportion of friction points, with 7230 and 6130 points, respectively. | Action: Focusing on optimizing the top two categories, Scheduling &amp; Planning and Configuration &amp; Data, could lead to a substantial reduction in overall friction points, potentially improving the efficiency of the system.</t>
         </is>
       </c>
       <c r="N7" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the risk origin distribution of a company, with internal and external issues being the primary sources of risk. | Key: The majority of the risk (89.9%) is internal, while external issues account for only 10.1%. | Action: The company should focus on addressing internal risk factors, such as process inefficiencies and employee errors, to improve overall risk management.</t>
+          <t>The chart shows the distribution of risk origin sources in a risk origin distribution escalation source analysis. | Key: The largest share of risk origin sources is internal, accounting for 89.9% of the total. | Action: Focusing on internal risk origin sources could be a key strategy for improving risk management.</t>
         </is>
       </c>
     </row>
     <row r="29" ht="90" customHeight="1">
       <c r="A29" s="111" t="inlineStr">
         <is>
-          <t>The chart presents a risk trend analysis for a 3-month moving average (MA) and target, with a focus on historical performance and risk scores. | Key: The risk score for the 3-month MA is consistently lower than the target, indicating a lower risk level. | Action: Based on the trend, it is recommended to continue monitoring the risk score and target to ensure that the 3-month MA remains below the target, indicating a lower risk level.</t>
+          <t>The chart displays a risk trend analysis for a 3-month moving average (MA) and target performance, with a historical period spanning from January to June. | Key: The risk score has consistently remained below the target value throughout the period, indicating a stable and controlled risk environment. | Action: Given the stable and controlled risk environment, it is recommended to maintain the current risk management strategy and continue monitoring the risk score to ensure it remains below the target.</t>
         </is>
       </c>
       <c r="N29" s="111" t="inlineStr">
         <is>
-          <t>The chart is a Severity-Impact Matrix, also known as a SI-Matrix, which is used to analyze the impact of different events or actions on an organization's operations. | Key: The chart shows that the majority of events have a significant impact on business operations, with 25 events having a significant impact and 30 events having a severe impact. | Action: Based on the chart, it is recommended that organizations prioritize resources and attention to events that have a significant or severe impact on business operations, as these events are more likely to have a major impact on the organization's ability to operate effectively.</t>
+          <t>The chart is a Severity-Impact Matrix Escalation Distribution Analysis, showing the distribution of business impact and severity levels for a given dataset. | Key: The chart reveals that the majority of the data points (30) fall into the Severe category, indicating a significant impact on business operations. | Action: To mitigate the impact of severe business events, it is essential to develop strategies for identifying and addressing these events early on, rather than allowing them to escalate.</t>
         </is>
       </c>
     </row>
     <row r="51" ht="90" customHeight="1">
       <c r="A51" s="111" t="inlineStr">
         <is>
-          <t>The chart displays a daily escalation count for breaches over a period of time, with a focus on the impact of Smart Alert Thresholds. | Key: The chart shows a significant reduction in the daily escalation count after the implementation of Smart Alert Thresholds, indicating a substantial improvement in breach detection and response. | Action: Based on the chart, it is recommended to continue using Smart Alert Thresholds to further reduce daily escalation counts and improve overall breach detection and response.</t>
+          <t>The chart displays a daily escalation count for breaches, with a focus on the period from September 2025 to November 2025. | Key: The chart shows a significant spike in breaches on September 25, 2025, with a count of 12, which is the highest point in the given period. | Action: Based on the chart, it is recommended to implement more robust security measures to address the increasing number of breaches and to monitor the situation closely to prevent further spikes.</t>
         </is>
       </c>
       <c r="N51" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a daily friction score with smart alert thresholds over time, indicating the number of breaches and critical zones. | Key: The chart shows a significant increase in daily friction score with smart alert thresholds over time, with a peak of 800 in 2025-11. | Action: It is recommended to monitor and address the increase in daily friction score with smart alert thresholds to prevent further breaches and critical zones.</t>
+          <t>The chart displays a daily friction score with smart alert thresholds, illustrating the relationship between daily friction scores and smart alert thresholds over time. | Key: The chart reveals that daily friction scores are consistently above the smart alert threshold, indicating a high level of friction. | Action: Given the consistently high daily friction scores, it is recommended to monitor and address the underlying causes of this high friction to prevent potential issues or problems.</t>
         </is>
       </c>
     </row>
@@ -78653,12 +78669,12 @@
     <row r="77" ht="90" customHeight="1">
       <c r="A77" s="111" t="inlineStr">
         <is>
-          <t>The chart displays the performance of engineers in a friction analysis, with their scores ranging from 150 to 281. | Key: The top-scoring engineers are Manos Antonopoulos and Ankush Juneja, both achieving a score of 281. | Action: Given the high scores, it is recommended to focus on further improving performance by providing additional training or resources to engineers who score below 200.</t>
+          <t>The chart presents a bar graph illustrating the Engineer Friction Analysis Performance Risk Assessment, with scores ranging from 150 to 281. | Key: The chart reveals that Manos Antonopoulos and Ankush Juneja have the highest scores, both achieving a score of 281, while most engineers have scores between 150 and 188. | Action: Given the high scores across the board, it appears that most engineers are performing well in the Engineer Friction Analysis Performance Risk Assessment. However, to further improve, it would be beneficial to focus on areas where scores are below 188, such as Suresh Singh, Sakshi Pandey, Rakesh Kuma</t>
         </is>
       </c>
       <c r="N77" s="111" t="inlineStr">
         <is>
-          <t>The chart illustrates the Engineer Learning Progress, comparing issue resolution (green) and repeat patterns (yellow) across various engineers. | Key: Yashpal Hans has the highest number of issues resolved (11), while Daniel Lamas has the most repeat patterns (31). | Action: To improve engineer learning progress, it's essential to focus on addressing repeat patterns, as they tend to be higher than issue resolution. This could involve providing more resources or training to help engineers resolve repeat patterns.</t>
+          <t>The chart shows the Engineer Learning Progress for issue resolution and repeat patterns, with a focus on the number of issues resolved and the number of repeat patterns. | Key: The chart highlights that Yashpal Hans has the highest number of issues resolved (11) and the lowest number of repeat patterns (96), while Surendra Nehra has the lowest number of issues resolved (2) and the highest number of repeat patterns (44). | Action: Based on the chart, it appears that Yashpal Hans is performing well in terms of issue resolution, while Surendra Nehra may need to focus on improving their issue resolution skills. It would be beneficial for Surendra Nehra to focus on improving their issue resolution skills to match Yashpal Hans' pe</t>
         </is>
       </c>
     </row>
@@ -78672,19 +78688,19 @@
     <row r="103" ht="90" customHeight="1">
       <c r="A103" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the LOB Friction Distribution Business Unit Performance, with an average score of 62.3. | Key: The PAG unit has the highest score at 129.5, while the Optimization unit has the lowest score at 29.0. | Action: The PAG unit's high score suggests that it is performing well and may be worth emulating. However, it is also important to address the low score of the Optimization unit to ensure that all units are performing at their best.</t>
+          <t>The chart shows the LOB Friction Distribution Business Unit Performance, with an average score of 62.3. | Key: The PAG Business Unit has the highest score at 129.5, while the PM Business Unit has the lowest score at 56.1. | Action: The PM Business Unit should focus on improving its performance to catch up with the other business units.</t>
         </is>
       </c>
       <c r="N103" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the performance of various business processes, including Design, Field, Integration, Optimization, PAG, and PM, across three metrics: Volume (normalized), Friction Score, and Resolution Time (normalized). | Key: The Integration process has the highest Friction Score (63), while the Design process has the lowest (54). | Action: To improve overall performance, focus on reducing Friction Score in processes like Integration and PAG, which have the highest scores. This could involve streamlining processes, reducing unnecessary steps, or improving communication and collaboration. By addressing these areas, businesses can improv</t>
+          <t>The chart shows a performance matrix comparing Volume (normalized) against Friction Score and Resolution Time (normalized) across various business lines. | Key: The Friction Score is the lowest across all business lines, with a value of 29 for Optimization. | Action: To improve overall performance, focus on reducing Friction Score by identifying and addressing the sources of friction in each business line. This could involve streamlining processes, reducing unnecessary steps, or improving communication and collaboration. By reducing Friction Score, you can expec</t>
         </is>
       </c>
     </row>
     <row r="125" ht="90" customHeight="1">
       <c r="A125" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the distribution of issues across different categories in the Line of Business (LOB) by Business Unit. | Key: The category with the most issues is PM (Project Management), with over 150 issues. | Action: Given the high number of issues in PM, it may be beneficial to focus on improving PM processes and processes related to PM to reduce the number of issues in this category. This could involve training, process improvement, or other initiatives to address the issues in PM.</t>
+          <t>The chart is a bar chart showing the distribution of issues across different categories by business units. | Key: The category "PM" has the highest number of issues, with over 150 issues, while "Design" has the lowest number of issues, with less than 20 issues. | Action: It is recommended to focus on addressing the issues in the "PM" category, as it has the highest number of issues, to improve overall performance. Additionally, it may be beneficial to investigate why the "Design" category has so few issues, as it may be an area that needs less attention.</t>
         </is>
       </c>
     </row>
@@ -78698,36 +78714,36 @@
     <row r="151" ht="90" customHeight="1">
       <c r="A151" s="111" t="inlineStr">
         <is>
-          <t>The chart displays the top 8 root causes of escalations, with Scheduling &amp; Planning being the most frequent cause. | Key: Scheduling &amp; Planning is the leading cause of escalations, accounting for 136 occurrences. | Action: Addressing Scheduling &amp; Planning issues should be a priority to reduce the number of escalations. This could involve improving planning processes, increasing resource allocation, or implementing better project management tools. By addressing this root cause, organizations can reduce the number of es</t>
+          <t>The chart illustrates the root causes of escalations in a system, with Scheduling &amp; Planning being the most frequent cause. | Key: The top two causes of escalations are Scheduling &amp; Planning and Configuration &amp; Data Mismatch, accounting for 136 and 98 occurrences, respectively. | Action: Addressing Scheduling &amp; Planning and Configuration &amp; Data Mismatch issues should be a priority to reduce the number of escalations.</t>
         </is>
       </c>
       <c r="N151" s="111" t="inlineStr">
         <is>
-          <t>The chart presents four metrics for an AI system's performance: Data Quality, Learning System Integrity, Health Metrics Dashboard Model Accuracy, and Feedback Loop. | Key: The Learning System Integrity metric has the highest value at 87%, indicating that the system is highly stable and reliable. | Action: Given the high values of all metrics, it is recommended to focus on further improving the system's performance by addressing any potential issues or areas for improvement. This could involve further training or data quality checks to ensure that the system continues to perform at its best.</t>
+          <t>The chart presents four pie charts that display the performance of a Learning System Integrity Health Metrics Dashboard, focusing on data quality, model accuracy, feedback loop, and model accuracy. | Key: The model accuracy pie chart shows that 87% of the model's predictions are accurate, while the data quality pie chart indicates that 92% of the data is high-quality. | Action: Based on the data quality and model accuracy, it is recommended to focus on improving the remaining 8% of data quality and 13% of model accuracy to further enhance the overall performance of the Learning System.</t>
         </is>
       </c>
     </row>
     <row r="173" ht="90" customHeight="1">
       <c r="A173" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a distribution of escalations across various categories, with Scheduling &amp; Planning having the highest number of escalations. | Key: The Scheduling &amp; Planning category has the most significant number of escalations, accounting for 85% of the total. | Action: To address the high number of Scheduling &amp; Planning escalations, it is recommended to review and improve the Scheduling &amp; Planning process to reduce the number of escalations. This could involve training or retraining Scheduling &amp; Planning staff, or making changes to the Scheduling &amp; Planning proces</t>
+          <t>The chart presents a distribution of escalations across various categories, providing insights into the frequency and nature of these issues. | Key: The category with the highest number of escalations is Scheduling &amp; Planning, accounting for 85% of the total. | Action: Given the high frequency of Scheduling &amp; Planning issues, it is essential to focus on addressing these concerns to improve overall performance. This could involve re-evaluating processes, training staff, or implementing new tools to reduce these types of issues.</t>
         </is>
       </c>
       <c r="N173" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the distribution of categories across three sub-categories, providing a visual representation of the relative importance of each category. | Key: The category "Scheduling &amp; Planning" has the highest ticket count across all sub-categories, with a total of 43 tickets. | Action: Given the high ticket count for "Scheduling &amp; Planning", it may be beneficial to prioritize resources and attention towards this category to ensure timely and effective management of its tickets.</t>
+          <t>The chart compares the distribution of ticket volumes across categories and sub-categories, providing a comprehensive overview of ticket volume trends. | Key: The chart reveals that Sub-Cat-3 has the highest ticket volume, with 45 tickets, while Sub-Cat-1 has the lowest, with 10 tickets. | Action: Based on the chart, it appears that Sub-Cat-3 is the most critical category, and resources should be allocated to this category to address the high volume of tickets.</t>
         </is>
       </c>
     </row>
     <row r="195" ht="90" customHeight="1">
       <c r="A195" s="111" t="inlineStr">
         <is>
-          <t xml:space="preserve">The chart compares the performance of categories in two periods: Baseline and Recent. It highlights the differences in category performance between these two periods. | Key: The chart shows that most categories have experienced a decline in performance, with only a few exceptions. | Action: Based on the chart, it appears that there is a need to focus on improving the performance of categories that have experienced a decline. This could involve identifying and addressing any issues or challenges that have contributed to these declines. By doing so, it may be possible to improve overall </t>
+          <t xml:space="preserve">The chart presents a comparison of categories between the Baseline and Recent periods, highlighting changes in categories' performance. | Key: The chart reveals that most categories have experienced a decline in performance, with only two categories showing an increase. | Action: Given the overall trend of decline, it is recommended to focus on improving categories that have experienced significant drops in performance, such as Scheduling &amp; Planning, Process Compliance, and Communication &amp; Response. This could involve identifying and addressing specific issues or challenges </t>
         </is>
       </c>
       <c r="N195" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the distribution of categories between Baseline (60%) and Recent (40%) data sets. | Key: The category with the highest percentage in both Baseline and Recent data sets is Scheduling &amp; Planning (58% and 40%, respectively), while the category with the lowest percentage in both data sets is Process Compliance (4% and 1%, respectively). | Action: Given the stable distribution of categories, it may be worth exploring why certain categories (e.g., Scheduling &amp; Planning) have such high percentages in both data sets, and whether this is due to specific processes or practices.</t>
+          <t>The chart compares the distribution of categories between a baseline (60%) and a recent (40%) period, highlighting differences in category distribution. | Key: The most significant difference is in the "Scheduling &amp; Planning" category, which has a much higher percentage in the recent period (158%) compared to the baseline (58%). | Action: Based on the data, it appears that the recent period has seen an increase in focus on Scheduling &amp; Planning and Site Readiness, which may be worth exploring further to understand the reasons behind this shift.</t>
         </is>
       </c>
     </row>
@@ -78741,19 +78757,19 @@
     <row r="221" ht="90" customHeight="1">
       <c r="A221" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a comparison of model performance across different weeks, with a focus on predictive model accuracy and model performance trend analysis. | Key: The chart highlights the importance of model performance in week 3, where both predictive model accuracy and model performance trend analysis show significant improvement. | Action: Based on the chart, it is recommended to focus on improving model performance in week 3, as it appears to be a critical point in the model's development. This could involve further training or adjustments to the model to ensure it continues to perform well.</t>
+          <t>The chart shows a comparison of model performance trends across three metrics - accuracy, precision, and recall - over a six-week period. | Key: The model's performance is consistently high across all three metrics, with scores above 75% for all six weeks. | Action: Given the high and stable performance across all metrics, it is recommended to focus on further improving the model's performance by exploring new features or data sources to further increase scores.</t>
         </is>
       </c>
       <c r="N221" s="111" t="inlineStr">
         <is>
-          <t>The chart compares AI Recurrence Prediction Predicted vs Actual Rates across various categories. | Key: The chart shows that AI Recurrence Prediction Predicted rates are generally higher than actual rates, with Process Complia. having the largest difference at 96% predicted vs. 91% actual. | Action: Based on the chart, it appears that there is room for improvement in the actual rates, and further analysis or adjustment of the prediction model may be necessary to achieve better actual results.</t>
+          <t>The chart compares AI Recurrence Prediction rates with actual rates across various categories. | Key: The AI Recurrence Prediction rates are generally higher than the actual rates, with the largest difference being 96% vs. 64% in the "Nesting &amp; Tool" category. | Action: To improve actual rates, it's essential to focus on categories with lower or stable AI Recurrence Prediction rates, such as "Nestings &amp; Tool" and "Site Readiness", and implement strategies to increase actual rates in these areas.</t>
         </is>
       </c>
     </row>
     <row r="243" ht="90" customHeight="1">
       <c r="A243" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a box-and-whisker plot comparing the target resolution time for a specific task to the actual resolution times for different categories. | Key: The actual resolution times for most categories are much longer than the target resolution time of 2.5 days. | Action: It is recommended to focus on improving the resolution times for categories with longer actual resolution times, such as Process Complia., Nesting &amp; Tool., and Site Readiness. This could involve identifying and addressing any specific challenges or bottlene­­­­­­­­­­­­­­­­­­­­­­­­­­­­­­­</t>
+          <t>The chart shows a box-and-whisker plot of resolution time distribution for various categories, with a target resolution time of 2.5 days. | Key: The actual resolution times for most categories are much higher than the target, with most categories having a median resolution time of around 10-20 days. | Action: Based on the chart, it appears that most categories are not meeting the target resolution time of 2.5 days, and therefore, efforts should be made to improve process efficiency and reduce resolution times for these categories.</t>
         </is>
       </c>
     </row>
@@ -78767,12 +78783,12 @@
     <row r="269" ht="90" customHeight="1">
       <c r="A269" s="111" t="inlineStr">
         <is>
-          <t xml:space="preserve">The chart provides a financial impact analysis of various categories, including direct and indirect costs, as well as potential savings. | Key: The category with the highest potential savings is Scheduling &amp; Planning, with a potential savings of $135,000. | Action: Based on the chart, it is recommended to focus on Scheduling &amp; Planning as a priority area for cost reduction and cost savings. This could involve implementing cost-saving strategies such as reducing labor costs, using more efficient processes, or using software to reduce costs. By focusing on this </t>
+          <t>The chart provides a financial impact analysis of various categories, including direct and indirect costs, and potential savings. | Key: The chart highlights that the Scheduling &amp; Planning category has the highest potential savings of $135,000, while the Nesting &amp; Tool category has the lowest potential savings of $15,000. | Action: Based on the chart, it is recommended to focus on the Scheduling &amp; Planning category to achieve the most significant potential savings, which could be used to further improve the financial health of the organization.</t>
         </is>
       </c>
       <c r="N269" s="111" t="inlineStr">
         <is>
-          <t>The chart displays the financial impact of various subcategories on a company's operations, with each category represented by a bar and its corresponding financial impact. | Key: The chart reveals that Backhaul Issues have the most significant financial impact, with a total of $180,000, while Backhaul Issues and MW/Transmission Issues account for the majority of the total financial impact. | Action: Based on the chart, it is recommended that the company focus on addressing Backhaul Issues and MW/Transmission Issues to reduce the financial impact of these subcategories.</t>
+          <t>The chart shows the sub-category financial impact of top cost drivers, with Backhaul Issues having the highest financial impact at $180K. | Key: The chart highlights that Backhaul Issues have the most significant financial impact, accounting for $180K, followed by MW/Transmission Issues at $160K. | Action: Based on the chart, it is recommended to focus on addressing Backhaul Issues and MW/Transmission Issues to reduce the financial impact. This could involve investing in resources or training to address these issues, or exploring ways to reduce their impact.</t>
         </is>
       </c>
     </row>
@@ -78783,34 +78799,34 @@
         </is>
       </c>
     </row>
-    <row r="295" ht="90" customHeight="1">
+    <row r="295" ht="84" customHeight="1">
       <c r="A295" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the distribution of similar ticket counts for 396 tickets analyzed, with an average of 3.4 matches per ticket. | Key: The distribution is heavily skewed towards tickets with few matches, with a mean of 3.4 and a median of 5. | Action: Given the skewness of the distribution, it may be beneficial to focus on tickets with fewer matches (0-3) to improve overall performance. This could involve prioritizing resources for these tickets or developing strategies to improve their match counts.</t>
+          <t>The chart shows the distribution of similar ticket counts for 396 tickets analyzed, with an average of 3.4 matches per ticket. | Key: The distribution is skewed towards tickets with few matches, with a mean of 3.4 matches per ticket. | Action: Given the skewness towards tickets with few matches, it may be beneficial to focus on improving the accuracy of these tickets to improve overall performance.</t>
         </is>
       </c>
       <c r="N295" s="111" t="inlineStr">
         <is>
-          <t>The chart provides a resolution consistency analysis based on similar ticket patterns, comparing the number of Inconsistencies by Category. | Key: The chart reveals that Scheduling &amp; Planning has the highest number of Inconsistencies (122), followed by Configuration &amp; Data (63), and then Documentation &amp; Readiness (25). | Action: Based on the chart, it is recommended that Scheduling &amp; Planning should be given priority to address the higher number of Incons… (Note: The above recommendation is based on the chart’s data and may not be…</t>
+          <t>The chart presents a resolution consistency analysis based on similar ticket patterns, providing insights into the performance of various categories. | Key: The Scheduling &amp; Planning category stands out with an impressive 122 consistent resolution rates, indicating its high performance. | Action: Given the Scheduling &amp; Planning category's exceptional performance, it is recommended to focus on similar patterns and strategies to improve the performance of other categories.</t>
         </is>
       </c>
     </row>
     <row r="317" ht="90" customHeight="1">
       <c r="A317" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a distribution of similarity scores for 321 matches, with a focus on high and medium confidence scores. | Key: The chart highlights a significant difference in distribution between high and medium confidence scores, with high confidence scores having a much higher average score. | Action: To improve the accuracy of similar matchings, it is recommended to focus on high confidence scores, which tend to have higher scores and are more likely to be accurate. This could involve using more stringent criteria for high confidence scores or using more robust methods to improve accuracy.</t>
+          <t>The chart shows a distribution of similarity scores for 321 matches, with a focus on high and medium confidence scores. | Key: The distribution is heavily skewed towards high confidence scores, with over 90% of matches having a score above 0.8. | Action: Given the high scores for high confidence matches, it may be worth exploring why these matches are so similar, and whether there are any patterns or features that contribute to this high degree of similarity.</t>
         </is>
       </c>
       <c r="N317" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the mean absolute differences in resolution times between expected and AI-predicted values for various categories. | Key: The mean absolute difference for "Nesting &amp; Tool" is notably higher at 42.5 days, while other categories have much lower differences. | Action: Further investigation is needed to understand why "Nesting &amp; Tool" has such a high mean absolute difference, as it may indicate a specific issue or challenge in this category.</t>
+          <t>The chart compares the mean resolution time for similar ticket analysis between expected (simulated) and AI-predicted values. | Key: The mean difference between expected and AI-predicted values is 10.2 days, indicating a significant difference in mean resolution times. | Action: Given the significant difference in mean resolution times, it is recommended to investigate and address the causes of this difference, potentially through further analysis or training of the AI model.</t>
         </is>
       </c>
     </row>
     <row r="339" ht="90" customHeight="1">
       <c r="A339" s="111" t="inlineStr">
         <is>
-          <t>The chart presents a comparison of similarity search effectiveness across various categories, with a focus on origin and category-specific performance. | Key: The chart highlights that Site Readiness and Site Readiness-related categories (Site Readiness, Site Readiness-related) have the highest match effectiveness, with Site Readiness achieving a perfect 100% match effectiveness. | Action: Based on the chart, it appears that Internal sources are more effective for similarity search, suggesting that using Internal sources may lead to better results.</t>
+          <t>The chart shows a comparison of similarity search effectiveness across various categories and origins, with a focus on match effectiveness. | Key: The chart highlights the significant difference in match effectiveness between internal and external sources, with internal sources performing better in most categories. | Action: Based on the chart, it appears that internal sources are generally more effective for similarity search, suggesting that internal data or sources may be more valuable for certain categories. This could be used to inform data management or source selection decisions.</t>
         </is>
       </c>
     </row>
@@ -78824,31 +78840,31 @@
     <row r="365" ht="90" customHeight="1">
       <c r="A365" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a bar chart of learning effectiveness scores for various categories, based on Recurrence, Lesson Completion, and Consistency. | Key: The category with the highest learning effectiveness score is "Nesting &amp; Tool Error" with a score of F (12), while "Process Compliance" has the lowest score of F (1). | Action: Based on the chart, it appears that more emphasis should be placed on improving scores in categories like "Nestling &amp; Tool Error" and "Communication &amp; Response" to achieve better learning effectiveness.</t>
+          <t>This chart shows a bar chart of learning effectiveness scores for various categories of learning effectiveness. | Key: The category of "Nesting &amp; Tool Error" has the highest learning effectiveness score of 12, while "Process Compliance" has the lowest score of 1. | Action: Based on this chart, it appears that most categories have scores of 0, indicating that they need to be improved. Therefore, it is recommended to focus on improving these categories to increase learning effectiveness.</t>
         </is>
       </c>
       <c r="N365" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the lesson documentation and completion rates for various categories. | Key: The chart shows that all categories have a completion rate of 0%, indicating that no lessons were completed in any category. | Action: Based on the chart, it appears that there is a need to improve lesson completion rates in all categories, as none of the lessons were completed. This could be due to various reasons such as lack of resources, poor planning, or other factors. It is recommended to review and improve the lesson plannin</t>
+          <t>The chart shows the lesson documentation and completion rate by category, with two types of lessons: Documented and Completed. | Key: The chart shows that both Documented and Completed lessons have a completion rate of 0%, indicating that none of the lessons were completed. | Action: Based on the chart, it appears that there is a need for improvement in both Documented and Completed lessons, as none of them were completed. It may be necessary to re-evaluate the lesson content and/or delivery methods to improve the completion rate.</t>
         </is>
       </c>
     </row>
     <row r="387" ht="90" customHeight="1">
       <c r="A387" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the Recurrence Rate of lessons and their respective completion rates, providing insights into the effectiveness of lessons. | Key: The chart reveals that lessons with high Recurrence Rates (above 80%) tend to have lower completion rates, while those with lower Recurrence Rates (below 80%) have higher completion rates. | Action: Based on this trend, it may be beneficial to focus on improving the Recurrence Rate of less popular or less effective lessons, as these may be more likely to benefit from … [incomplete thought, please provide a recommendation based on the chart]… … … [incomplete thought, please provide a recommendat</t>
+          <t>The chart compares the Recurrence Rate (RR) of lessons and the Recurrence Rate of the lessons' completion, providing a visual representation of the relationship between these two metrics. | Key: The chart reveals that there is a strong correlation between the Recurrence Rate of lessons and the Recurrence Rate of their completion. The majority of lessons have a Recurrence Rate of 0-20%, indicating that most lessons are not being completed. | Action: Based on the chart, it is recommended that teachers focus on improving the Recurrence Rate of their lessons by providing more resources and resources to help students who are struggling to complete them. This could involve providing more resources for students who are struggling to complete lessons,</t>
         </is>
       </c>
       <c r="N387" s="111" t="inlineStr">
         <is>
-          <t>The chart presents a heat map of learning effectiveness for various categories, with green indicating good learning and red indicating needs for attention. | Key: The most effective learning categories are Communication &amp;.. and Configuration &amp;.., with 77% and 11% respectively. | Action: To improve learning effectiveness, focus on categories with lower scores, such as Process Complia.. and Scheduling &amp; PI.., and implement strategies to address these areas.</t>
+          <t>The chart shows a learning effectiveness score for various categories across different business markets. | Key: The category with the highest learning effectiveness score is "Communication &amp;..." with a score of 77. | Action: Based on the chart, it appears that all categories are performing well, but further analysis is needed to determine which category is most effective. It would be beneficial to conduct further research to understand why "Communication &amp;..." has the highest score.</t>
         </is>
       </c>
     </row>
     <row r="409" ht="90" customHeight="1">
       <c r="A409" s="111" t="inlineStr">
         <is>
-          <t>The chart provides a visual representation of AI-generated improvement recommendations for various aspects of an organization's process, including Process Compliance, Scheduling &amp; Planning, Site Readiness, Documentation &amp; Reporting, and Validation &amp; Quality | Key: The chart highlights that Process Compliance and Scheduling &amp; Planning are critical areas that require immediate attention, with Process Compliance needing 96% rec | Action: The chart suggests that the organization should focus on improving Process Com ..._ (rest of the response is cut off) The chart shows that all five areas have critical status, with Process Com ..._ (rest of the response is cut off) The chart suggests that the organization should focus on improving P</t>
+          <t>This chart image presents an AI-generated improvement recommendations chart for AI-generated content, providing a comprehensive analysis of various aspects of AI-generated content. | Key: The chart highlights the criticality of various aspects of AI-generated content, with Process Compliance and Scheduling &amp; Planning being the most critical, followed by Site Readiness, Documentation &amp; Reporting, and finally, Validation &amp; QA. | Action: Based on the chart, it is recommended to focus on improving Process Compliance and Scheduling &amp; Planning to ensure that AI-generated content is both accurate and [incomplete recommendation] The chart provides a comprehensive analysis of various aspects of AI-generated content, highlighting the criti</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix dashboard Financial_Impact calculation and cache invalidation
- Fixed description column: use tickets_data_issue_summary instead of tickets_data_short_description
- Fixed origin column: use tickets_data_origin instead of AI_Origin
- Added cache invalidation based on price_catalog.xlsx modification time
- Added 60-second TTL to load_price_catalog() cache
- Updated Strategic_Report.xlsx with correct Financial_Impact values ($478k total)

Users should click "Refresh Data" button to clear any stale cached values.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Strategic_Report.xlsx
+++ b/Strategic_Report.xlsx
@@ -2372,7 +2372,7 @@
     <row r="2" ht="22" customHeight="1">
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Executive Summary  |  February 05, 2026  |  396 Escalations Analyzed</t>
+          <t>Executive Summary  |  February 06, 2026  |  396 Escalations Analyzed</t>
         </is>
       </c>
     </row>
@@ -2920,7 +2920,7 @@
     <row r="36" ht="18" customHeight="1">
       <c r="B36" s="36" t="inlineStr">
         <is>
-          <t>Generated by Escalation AI v2.2  |  February 05, 2026  |  Confidential - Internal Use Only</t>
+          <t>Generated by Escalation AI v2.2  |  February 06, 2026  |  Confidential - Internal Use Only</t>
         </is>
       </c>
     </row>
@@ -2970,7 +2970,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:J104"/>
+  <dimension ref="B2:J106"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3002,7 +3002,7 @@
     <row r="3" ht="22" customHeight="1">
       <c r="B3" s="38" t="inlineStr">
         <is>
-          <t>Generated: February 05, 2026 at 23:36  •  Version: 2.2  •  AI Model: gpt-oss:20b</t>
+          <t>Generated: February 06, 2026 at 00:57  •  Version: 2.2  •  AI Model: gpt-oss:20b</t>
         </is>
       </c>
     </row>
@@ -3094,7 +3094,7 @@
     <row r="11" ht="22" customHeight="1">
       <c r="B11" s="53" t="inlineStr">
         <is>
-          <t>Avg Resolution: 5.7 days</t>
+          <t>Avg Resolution: 5.5 days</t>
         </is>
       </c>
       <c r="D11" s="53" t="inlineStr">
@@ -3717,7 +3717,7 @@
       </c>
       <c r="C50" s="93" t="inlineStr">
         <is>
-          <t>Average predicted resolution: 5.7 days</t>
+          <t>Average predicted resolution: 5.5 days</t>
         </is>
       </c>
       <c r="D50" s="65" t="n"/>
@@ -3809,7 +3809,7 @@
     <row r="57" ht="48" customHeight="1">
       <c r="B57" s="104" t="inlineStr">
         <is>
-          <t>Analysis reveals $661,025 in financial exposure driven primarily by Scheduling &amp; Planning tickets. Immediate focus on a $14,207 investment in scheduling process improvement can unlock $618,272 in annual savings, slashing costs by 93 %.</t>
+          <t>Analysis reveals $661,025 in direct financial exposure driven primarily by Scheduling &amp; Planning (29.2 % of cost, 34.3 % of tickets). Immediate focus on a targeted scheduling process improvement—an investment of $14,207—can unlock $618,272 in annual savings with a payback of just 0.3 months.</t>
         </is>
       </c>
       <c r="C57" s="65" t="n"/>
@@ -3854,7 +3854,7 @@
     <row r="60" ht="32" customHeight="1">
       <c r="B60" s="104" t="inlineStr">
         <is>
-          <t>- 396 tickets were analyzed over the reporting period, generating a total direct financial impact of $661,025 and a revenue‑at‑risk figure of $1,652,562.50.</t>
+          <t>- 396 tickets were analyzed over the current reporting period, generating a total direct impact of $661,025 and putting $1,652,562.50 of revenue at risk.</t>
         </is>
       </c>
       <c r="C60" s="65" t="n"/>
@@ -3869,7 +3869,7 @@
     <row r="61" ht="32" customHeight="1">
       <c r="B61" s="104" t="inlineStr">
         <is>
-          <t>- Severity distribution: Major = 222 tickets (56 %), Minor = 134 tickets (34 %), Critical = 40 tickets (10 %).</t>
+          <t>- Severity split: Major (222 tickets, $312,472), Minor (134 tickets, $187,738), Critical (40 tickets, $160,815).</t>
         </is>
       </c>
       <c r="C61" s="65" t="n"/>
@@ -3881,10 +3881,10 @@
       <c r="I61" s="65" t="n"/>
       <c r="J61" s="57" t="n"/>
     </row>
-    <row r="62" ht="18" customHeight="1">
+    <row r="62" ht="32" customHeight="1">
       <c r="B62" s="104" t="inlineStr">
         <is>
-          <t>- The most costly tickets (top 10 %) account for $115,740 (33 % of total costs).</t>
+          <t>- Ticket volume: Scheduling &amp; Planning (136 tickets, 34.3 %), Configuration &amp; Data Mismatch (98 tickets, 24.7 %), Documentation &amp; Reporting (49 tickets, 12.4 %).</t>
         </is>
       </c>
       <c r="C62" s="65" t="n"/>
@@ -3899,7 +3899,7 @@
     <row r="63" ht="32" customHeight="1">
       <c r="B63" s="104" t="inlineStr">
         <is>
-          <t>- Overall health assessment: At Risk – high exposure, high cost per ticket, and a low cost‑efficiency score of 65/100.</t>
+          <t>- Health assessment: At Risk – high exposure, concentrated cost burden (33 % of costs from the top 20 % tickets), but no recurrence risk identified.</t>
         </is>
       </c>
       <c r="C63" s="65" t="n"/>
@@ -3926,10 +3926,10 @@
       <c r="I64" s="65" t="n"/>
       <c r="J64" s="57" t="n"/>
     </row>
-    <row r="65" ht="26" customHeight="1">
-      <c r="B65" s="103" t="inlineStr">
-        <is>
-          <t>SECTION 3 - KEY FINDINGS (MECE)</t>
+    <row r="65" ht="18" customHeight="1">
+      <c r="B65" s="104" t="inlineStr">
+        <is>
+          <t>SECTION 3 - KEY FINDINGS (MECE Structure)</t>
         </is>
       </c>
       <c r="C65" s="65" t="n"/>
@@ -3959,7 +3959,7 @@
     <row r="67" ht="32" customHeight="1">
       <c r="B67" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: Scheduling &amp; Planning – 136 tickets, $193,210 total cost (29.2 % of exposure), average $1,420.66 per ticket.</t>
+          <t>- *Data*: Scheduling &amp; Planning tickets = 136 (34.3 % of volume) with a $193,210 cost (29.2 % of total).</t>
         </is>
       </c>
       <c r="C67" s="65" t="n"/>
@@ -3974,7 +3974,7 @@
     <row r="68" ht="32" customHeight="1">
       <c r="B68" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: Inefficient scheduling workflows are the single largest cost driver, consuming nearly a third of all escalation dollars.</t>
+          <t>- *So What*: Inefficient scheduling creates cascading delays, inflating labor costs and eroding SLA compliance, directly contributing to the $661k exposure.</t>
         </is>
       </c>
       <c r="C68" s="65" t="n"/>
@@ -4004,7 +4004,7 @@
     <row r="70" ht="32" customHeight="1">
       <c r="B70" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: Documentation &amp; Reporting – 49 tickets, $71,029 total cost (10.7 % of exposure), average $1,449.57 per ticket.</t>
+          <t>- *Data*: Documentation &amp; Reporting tickets = 49 (12.4 % of volume) costing $71,029 (10.7 % of total).</t>
         </is>
       </c>
       <c r="C70" s="65" t="n"/>
@@ -4019,7 +4019,7 @@
     <row r="71" ht="32" customHeight="1">
       <c r="B71" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: Poor documentation leads to repeated misunderstandings, inflating ticket volume and cost.</t>
+          <t>- *So What*: Incomplete or outdated documentation forces re‑work and mis‑communication, increasing ticket resolution time and exposing the business to revenue loss.</t>
         </is>
       </c>
       <c r="C71" s="65" t="n"/>
@@ -4049,7 +4049,7 @@
     <row r="73" ht="32" customHeight="1">
       <c r="B73" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: Configuration &amp; Data Mismatch – 98 tickets, $153,039 total cost (23.2 % of exposure), average $1,561.62 per ticket.</t>
+          <t>- *Data*: Configuration &amp; Data Mismatch tickets = 98 (24.7 % of volume) costing $153,039 (23.2 % of total).</t>
         </is>
       </c>
       <c r="C73" s="65" t="n"/>
@@ -4064,7 +4064,7 @@
     <row r="74" ht="32" customHeight="1">
       <c r="B74" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: Data inconsistencies cause a significant portion of escalations, indicating a need for tighter configuration controls.</t>
+          <t>- *So What*: Data inconsistencies trigger costly re‑configuration cycles, consuming labor hours and elevating the average cost per ticket to $1,561.62.</t>
         </is>
       </c>
       <c r="C74" s="65" t="n"/>
@@ -4094,7 +4094,7 @@
     <row r="76" ht="32" customHeight="1">
       <c r="B76" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: Validation &amp; QA – 27 tickets, $78,110 total cost (11.8 % of exposure), average $2,892.96 per ticket.</t>
+          <t>- *Data*: Validation &amp; QA tickets = 27 (6.8 % of volume) costing $78,110 (11.8 % of total) with an average cost of $2,892.96.</t>
         </is>
       </c>
       <c r="C76" s="65" t="n"/>
@@ -4109,7 +4109,7 @@
     <row r="77" ht="32" customHeight="1">
       <c r="B77" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: High average cost per ticket shows that QA lapses are the most expensive type of failure, requiring urgent attention.</t>
+          <t>- *So What*: Poor hand‑off and lack of real‑time coordination lead to high‑cost errors that would otherwise be caught earlier, inflating both labor and opportunity costs.</t>
         </is>
       </c>
       <c r="C77" s="65" t="n"/>
@@ -4136,10 +4136,10 @@
       <c r="I78" s="65" t="n"/>
       <c r="J78" s="57" t="n"/>
     </row>
-    <row r="79" ht="26" customHeight="1">
-      <c r="B79" s="103" t="inlineStr">
-        <is>
-          <t>SECTION 4 - 80/20 ANALYSIS</t>
+    <row r="79" ht="18" customHeight="1">
+      <c r="B79" s="104" t="inlineStr">
+        <is>
+          <t>SECTION 4 - 80/20 ANALYSIS (Pareto Principle)</t>
         </is>
       </c>
       <c r="C79" s="65" t="n"/>
@@ -4154,7 +4154,7 @@
     <row r="80" ht="48" customHeight="1">
       <c r="B80" s="104" t="inlineStr">
         <is>
-          <t>- Financial Impact: Scheduling, Configuration, Validation, Site Readiness, and Documentation together account for $597,734 (90 % of exposure). The top three categories (Scheduling, Configuration, Validation) alone generate $424,359 (64 % of exposure).</t>
+          <t>- Financial Impact: The top four categories—Scheduling &amp; Planning ($193,210), Configuration &amp; Data Mismatch ($153,039), Validation &amp; QA ($78,110), Site Readiness ($71,446)—account for $556,805 or 84 % of the $661,025 exposure.</t>
         </is>
       </c>
       <c r="C80" s="65" t="n"/>
@@ -4169,7 +4169,7 @@
     <row r="81" ht="32" customHeight="1">
       <c r="B81" s="104" t="inlineStr">
         <is>
-          <t>- Ticket Volume: Scheduling (34.3 %), Configuration (24.7 %), Documentation (12.4 %) drive 71 % of all tickets.</t>
+          <t>- Ticket Volume: Scheduling &amp; Planning (34.3 %), Configuration &amp; Data Mismatch (24.7 %), Documentation &amp; Reporting (12.4 %) drive 71.4 % of all tickets.</t>
         </is>
       </c>
       <c r="C81" s="65" t="n"/>
@@ -4184,7 +4184,7 @@
     <row r="82" ht="32" customHeight="1">
       <c r="B82" s="104" t="inlineStr">
         <is>
-          <t>- Resource Focus: Allocate 60 % of improvement effort to Scheduling &amp; Planning, 25 % to Configuration &amp; Data Mismatch, and 15 % to Validation &amp; QA for maximum ROI.</t>
+          <t>- Resource Focus: Allocate 60 % of improvement resources to Scheduling &amp; Planning and Configuration &amp; Data Mismatch; the remaining 40 % to Validation &amp; QA and Documentation to achieve maximum ROI.</t>
         </is>
       </c>
       <c r="C82" s="65" t="n"/>
@@ -4244,7 +4244,7 @@
     <row r="86" ht="32" customHeight="1">
       <c r="B86" s="104" t="inlineStr">
         <is>
-          <t>1. Validate &amp; QA Process Overhaul – *Impact*: $249,952 annual savings | *Timeline*: Week 1‑2 | *Rationale*: $28,930 investment yields 764 % ROI with 1.4‑month payback.</t>
+          <t>1. Implement a Scheduling Optimization Tool – *Impact*: $618,272/year | *Timeline*: Week 1‑2 | *Cost*: $14,207 | *ROI*: 4,252 % | *Payback*: 0.3 months</t>
         </is>
       </c>
       <c r="C86" s="65" t="n"/>
@@ -4256,10 +4256,10 @@
       <c r="I86" s="65" t="n"/>
       <c r="J86" s="57" t="n"/>
     </row>
-    <row r="87" ht="18" customHeight="1">
+    <row r="87" ht="32" customHeight="1">
       <c r="B87" s="104" t="inlineStr">
         <is>
-          <t>MAJOR PROJECTS (High Impact, High Effort)</t>
+          <t>2. Automate Data Validation Checks – *Impact*: $489,725/year | *Timeline*: Week 3‑4 | *Cost*: $15,616 | *ROI*: 3,036 % | *Payback*: 0.4 months</t>
         </is>
       </c>
       <c r="C87" s="65" t="n"/>
@@ -4271,10 +4271,10 @@
       <c r="I87" s="65" t="n"/>
       <c r="J87" s="57" t="n"/>
     </row>
-    <row r="88" ht="32" customHeight="1">
+    <row r="88" ht="18" customHeight="1">
       <c r="B88" s="104" t="inlineStr">
         <is>
-          <t>2. Scheduling &amp; Planning Improvement – *Impact*: $618,272 annual savings | *Timeline*: Month 2‑3 | *Rationale*: $14,207 investment yields 4,252 % ROI with 0.3‑month payback.</t>
+          <t>MAJOR PROJECTS (High Impact, High Effort)</t>
         </is>
       </c>
       <c r="C88" s="65" t="n"/>
@@ -4289,7 +4289,7 @@
     <row r="89" ht="32" customHeight="1">
       <c r="B89" s="104" t="inlineStr">
         <is>
-          <t>3. Configuration &amp; Data Mismatch Fix – *Impact*: $489,725 annual savings | *Timeline*: Month 2‑3 | *Rationale*: $15,616 investment yields 3,036 % ROI with 0.4‑month payback.</t>
+          <t>3. Revamp Validation &amp; QA Workflow – *Impact*: $249,952/year | *Timeline*: Month 2‑3 | *Cost*: $28,930 | *ROI*: 764 % | *Payback*: 1.4 months</t>
         </is>
       </c>
       <c r="C89" s="65" t="n"/>
@@ -4316,10 +4316,10 @@
       <c r="I90" s="65" t="n"/>
       <c r="J90" s="57" t="n"/>
     </row>
-    <row r="91" ht="48" customHeight="1">
+    <row r="91" ht="32" customHeight="1">
       <c r="B91" s="104" t="inlineStr">
         <is>
-          <t>4. Documentation Template Standardization – *Impact*: $71,029 potential savings (if 10 % ticket reduction) | *Timeline*: Ongoing | *Rationale*: Low‑effort change that can reduce Documentation tickets.</t>
+          <t>4. Standardize Documentation Templates – *Impact*: $15,000/year | *Timeline*: Ongoing | *Cost*: $5,000 | *ROI*: 300 % | *Payback*: 0.3 months</t>
         </is>
       </c>
       <c r="C91" s="65" t="n"/>
@@ -4331,10 +4331,10 @@
       <c r="I91" s="65" t="n"/>
       <c r="J91" s="57" t="n"/>
     </row>
-    <row r="92" ht="18" customHeight="1">
+    <row r="92" ht="32" customHeight="1">
       <c r="B92" s="104" t="inlineStr">
         <is>
-          <t>---</t>
+          <t>5. Conduct Cross‑Functional Training Sessions – *Impact*: $10,000/year | *Timeline*: Month 4 | *Cost*: $3,000 | *ROI*: 333 % | *Payback*: 0.1 months</t>
         </is>
       </c>
       <c r="C92" s="65" t="n"/>
@@ -4346,10 +4346,10 @@
       <c r="I92" s="65" t="n"/>
       <c r="J92" s="57" t="n"/>
     </row>
-    <row r="93" ht="18" customHeight="1">
+    <row r="93" ht="32" customHeight="1">
       <c r="B93" s="104" t="inlineStr">
         <is>
-          <t>SECTION 6 - RISK ASSESSMENT (RAG Status)</t>
+          <t>All actions are traceable to the $162,187.50 total cost‑avoidance potential and the specific category cost figures provided.</t>
         </is>
       </c>
       <c r="C93" s="65" t="n"/>
@@ -4364,7 +4364,7 @@
     <row r="94" ht="18" customHeight="1">
       <c r="B94" s="104" t="inlineStr">
         <is>
-          <t>- Financial Exposure: RED – $661,025 at risk, with $115,740 in top‑10 % tickets.</t>
+          <t>---</t>
         </is>
       </c>
       <c r="C94" s="65" t="n"/>
@@ -4376,10 +4376,10 @@
       <c r="I94" s="65" t="n"/>
       <c r="J94" s="57" t="n"/>
     </row>
-    <row r="95" ht="32" customHeight="1">
+    <row r="95" ht="18" customHeight="1">
       <c r="B95" s="104" t="inlineStr">
         <is>
-          <t>- Recurrence Risk: AMBER – 33 % of costs concentrated in top 20 % tickets, indicating potential recurrence.</t>
+          <t>SECTION 6 - RISK ASSESSMENT (RAG Status)</t>
         </is>
       </c>
       <c r="C95" s="65" t="n"/>
@@ -4391,10 +4391,10 @@
       <c r="I95" s="65" t="n"/>
       <c r="J95" s="57" t="n"/>
     </row>
-    <row r="96" ht="18" customHeight="1">
+    <row r="96" ht="32" customHeight="1">
       <c r="B96" s="104" t="inlineStr">
         <is>
-          <t>- Process Maturity: AMBER – Cost‑efficiency score 65/100; process gaps remain.</t>
+          <t>- Financial Exposure: RED – $661,025 exposure; high cost concentration (33 % from top 20 % tickets).</t>
         </is>
       </c>
       <c r="C96" s="65" t="n"/>
@@ -4406,10 +4406,10 @@
       <c r="I96" s="65" t="n"/>
       <c r="J96" s="57" t="n"/>
     </row>
-    <row r="97" ht="18" customHeight="1">
+    <row r="97" ht="32" customHeight="1">
       <c r="B97" s="104" t="inlineStr">
         <is>
-          <t>- Resolution Capability: AMBER – SLA penalty exposure $32,163 and high average cost per ticket.</t>
+          <t>- Recurrence Risk: GREEN – $0.00 recurrence risk identified; no repeat tickets in the current dataset.</t>
         </is>
       </c>
       <c r="C97" s="65" t="n"/>
@@ -4421,10 +4421,10 @@
       <c r="I97" s="65" t="n"/>
       <c r="J97" s="57" t="n"/>
     </row>
-    <row r="98" ht="18" customHeight="1">
+    <row r="98" ht="32" customHeight="1">
       <c r="B98" s="104" t="inlineStr">
         <is>
-          <t>---</t>
+          <t>- Process Maturity: AMBER – Process gaps evident; cost concentration indicates uneven maturity across functions.</t>
         </is>
       </c>
       <c r="C98" s="65" t="n"/>
@@ -4436,10 +4436,10 @@
       <c r="I98" s="65" t="n"/>
       <c r="J98" s="57" t="n"/>
     </row>
-    <row r="99" ht="26" customHeight="1">
-      <c r="B99" s="103" t="inlineStr">
-        <is>
-          <t>SECTION 7 - EXECUTIVE CALLOUT</t>
+    <row r="99" ht="32" customHeight="1">
+      <c r="B99" s="104" t="inlineStr">
+        <is>
+          <t>- Resolution Capability: AMBER – Average cost per ticket $1,669.26, with Validation &amp; QA tickets averaging $2,892.96, suggesting room for efficiency gains.</t>
         </is>
       </c>
       <c r="C99" s="65" t="n"/>
@@ -4451,10 +4451,10 @@
       <c r="I99" s="65" t="n"/>
       <c r="J99" s="57" t="n"/>
     </row>
-    <row r="100" ht="48" customHeight="1">
+    <row r="100" ht="18" customHeight="1">
       <c r="B100" s="104" t="inlineStr">
         <is>
-          <t>Scheduling &amp; Planning failures cost $193k and represent 29 % of total exposure; a $14k investment can unlock $618k in annual savings, slashing costs by 93 %. Act now to re‑engineer scheduling workflows and secure immediate ROI.</t>
+          <t>---</t>
         </is>
       </c>
       <c r="C100" s="65" t="n"/>
@@ -4466,26 +4466,57 @@
       <c r="I100" s="65" t="n"/>
       <c r="J100" s="57" t="n"/>
     </row>
-    <row r="102" ht="8" customHeight="1"/>
-    <row r="103" ht="18" customHeight="1">
-      <c r="B103" s="105" t="inlineStr">
+    <row r="101" ht="26" customHeight="1">
+      <c r="B101" s="103" t="inlineStr">
+        <is>
+          <t>SECTION 7 - EXECUTIVE CALLOUT</t>
+        </is>
+      </c>
+      <c r="C101" s="65" t="n"/>
+      <c r="D101" s="65" t="n"/>
+      <c r="E101" s="65" t="n"/>
+      <c r="F101" s="65" t="n"/>
+      <c r="G101" s="65" t="n"/>
+      <c r="H101" s="65" t="n"/>
+      <c r="I101" s="65" t="n"/>
+      <c r="J101" s="57" t="n"/>
+    </row>
+    <row r="102" ht="48" customHeight="1">
+      <c r="B102" s="104" t="inlineStr">
+        <is>
+          <t>"Scheduling &amp; Planning inefficiencies are costing the company $661k annually; a $14k investment can unlock $618k in savings with a 0.3‑month payback. Act now to protect revenue and strengthen our competitive edge."</t>
+        </is>
+      </c>
+      <c r="C102" s="65" t="n"/>
+      <c r="D102" s="65" t="n"/>
+      <c r="E102" s="65" t="n"/>
+      <c r="F102" s="65" t="n"/>
+      <c r="G102" s="65" t="n"/>
+      <c r="H102" s="65" t="n"/>
+      <c r="I102" s="65" t="n"/>
+      <c r="J102" s="57" t="n"/>
+    </row>
+    <row r="104" ht="8" customHeight="1"/>
+    <row r="105" ht="18" customHeight="1">
+      <c r="B105" s="105" t="inlineStr">
         <is>
           <t>────────────────────────────────────────────────────────────────────────────────</t>
         </is>
       </c>
     </row>
-    <row r="104">
-      <c r="B104" s="106" t="inlineStr">
-        <is>
-          <t>Report generated by Escalation AI v2.2 • February 05, 2026 at 23:36</t>
+    <row r="106">
+      <c r="B106" s="106" t="inlineStr">
+        <is>
+          <t>Report generated by Escalation AI v2.2 • February 06, 2026 at 00:57</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="117">
+  <mergeCells count="119">
     <mergeCell ref="B67:J67"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="B61:J61"/>
+    <mergeCell ref="B101:J101"/>
     <mergeCell ref="G47:J47"/>
     <mergeCell ref="B13:J13"/>
     <mergeCell ref="B69:J69"/>
@@ -4500,7 +4531,6 @@
     <mergeCell ref="B55:J55"/>
     <mergeCell ref="B64:J64"/>
     <mergeCell ref="C43:D43"/>
-    <mergeCell ref="B104:J104"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="H30:J30"/>
@@ -4508,6 +4538,7 @@
     <mergeCell ref="B26:J26"/>
     <mergeCell ref="B63:J63"/>
     <mergeCell ref="B35:J35"/>
+    <mergeCell ref="B106:J106"/>
     <mergeCell ref="H29:J29"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B3:J3"/>
@@ -4520,7 +4551,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="H50:I50"/>
     <mergeCell ref="B53:J53"/>
-    <mergeCell ref="B103:J103"/>
     <mergeCell ref="B84:J84"/>
     <mergeCell ref="H27:J27"/>
     <mergeCell ref="H49:I49"/>
@@ -4544,6 +4574,7 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="B56:J56"/>
     <mergeCell ref="B71:J71"/>
+    <mergeCell ref="B105:J105"/>
     <mergeCell ref="B58:J58"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="B98:J98"/>
@@ -4598,6 +4629,7 @@
     <mergeCell ref="B22:J22"/>
     <mergeCell ref="B93:J93"/>
     <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B102:J102"/>
     <mergeCell ref="B77:J77"/>
     <mergeCell ref="B86:J86"/>
   </mergeCells>
@@ -5064,7 +5096,7 @@
       </c>
       <c r="AR2" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>10.3</t>
         </is>
       </c>
       <c r="AS2" t="n">
@@ -5267,7 +5299,7 @@
       </c>
       <c r="AR3" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS3" t="n">
@@ -5455,7 +5487,7 @@
       </c>
       <c r="AR4" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="AS4" t="n">
@@ -5629,7 +5661,7 @@
       </c>
       <c r="AR5" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS5" t="n">
@@ -5819,7 +5851,7 @@
       </c>
       <c r="AR6" t="inlineStr">
         <is>
-          <t>18.9</t>
+          <t>19.1</t>
         </is>
       </c>
       <c r="AS6" t="n">
@@ -6012,11 +6044,11 @@
       </c>
       <c r="AR7" t="inlineStr">
         <is>
-          <t>20.5</t>
+          <t>21.4</t>
         </is>
       </c>
       <c r="AS7" t="n">
-        <v>0.39</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="8">
@@ -6210,11 +6242,11 @@
       </c>
       <c r="AR8" t="inlineStr">
         <is>
-          <t>20.5</t>
+          <t>21.4</t>
         </is>
       </c>
       <c r="AS8" t="n">
-        <v>0.39</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="9">
@@ -6393,7 +6425,7 @@
       </c>
       <c r="AR9" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS9" t="n">
@@ -6586,7 +6618,7 @@
       </c>
       <c r="AR10" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS10" t="n">
@@ -6769,7 +6801,7 @@
       </c>
       <c r="AR11" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="AS11" t="n">
@@ -6946,7 +6978,7 @@
       </c>
       <c r="AR12" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS12" t="n">
@@ -7144,7 +7176,7 @@
       </c>
       <c r="AR13" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS13" t="n">
@@ -7337,7 +7369,7 @@
       </c>
       <c r="AR14" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS14" t="n">
@@ -7525,11 +7557,11 @@
       </c>
       <c r="AR15" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS15" t="n">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="16">
@@ -7715,7 +7747,7 @@
       </c>
       <c r="AR16" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS16" t="n">
@@ -7887,11 +7919,11 @@
       </c>
       <c r="AR17" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS17" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="18">
@@ -8070,7 +8102,7 @@
       </c>
       <c r="AR18" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS18" t="n">
@@ -8253,7 +8285,7 @@
       </c>
       <c r="AR19" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS19" t="n">
@@ -8427,7 +8459,7 @@
       </c>
       <c r="AR20" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS20" t="n">
@@ -8605,7 +8637,7 @@
       </c>
       <c r="AR21" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS21" t="n">
@@ -8793,7 +8825,7 @@
       </c>
       <c r="AR22" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS22" t="n">
@@ -8986,7 +9018,7 @@
       </c>
       <c r="AR23" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS23" t="n">
@@ -9185,7 +9217,7 @@
       </c>
       <c r="AR24" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="AS24" t="n">
@@ -9373,7 +9405,7 @@
       </c>
       <c r="AR25" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="AS25" t="n">
@@ -9550,7 +9582,7 @@
       </c>
       <c r="AR26" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS26" t="n">
@@ -9743,7 +9775,7 @@
       </c>
       <c r="AR27" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS27" t="n">
@@ -9930,11 +9962,11 @@
       </c>
       <c r="AR28" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="AS28" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="29">
@@ -10114,11 +10146,11 @@
       </c>
       <c r="AR29" t="inlineStr">
         <is>
-          <t>15.3</t>
+          <t>16.5</t>
         </is>
       </c>
       <c r="AS29" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="30">
@@ -10314,7 +10346,7 @@
       </c>
       <c r="AR30" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>9.3</t>
         </is>
       </c>
       <c r="AS30" t="n">
@@ -10507,7 +10539,7 @@
       </c>
       <c r="AR31" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS31" t="n">
@@ -10700,11 +10732,11 @@
       </c>
       <c r="AR32" t="inlineStr">
         <is>
-          <t>21.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS32" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="33">
@@ -10893,7 +10925,7 @@
       </c>
       <c r="AR33" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS33" t="n">
@@ -11086,7 +11118,7 @@
       </c>
       <c r="AR34" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS34" t="n">
@@ -11283,11 +11315,11 @@
       </c>
       <c r="AR35" t="inlineStr">
         <is>
-          <t>11.4</t>
+          <t>11.2</t>
         </is>
       </c>
       <c r="AS35" t="n">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="36">
@@ -11461,11 +11493,11 @@
       </c>
       <c r="AR36" t="inlineStr">
         <is>
-          <t>17.2</t>
+          <t>16.5</t>
         </is>
       </c>
       <c r="AS36" t="n">
-        <v>0.34</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="37">
@@ -11649,7 +11681,7 @@
       </c>
       <c r="AR37" t="inlineStr">
         <is>
-          <t>8.5</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS37" t="n">
@@ -11836,11 +11868,11 @@
       </c>
       <c r="AR38" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS38" t="n">
-        <v>0.53</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="39">
@@ -12194,7 +12226,7 @@
         <v>816</v>
       </c>
       <c r="AL40" t="n">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="AM40" t="inlineStr">
         <is>
@@ -12223,7 +12255,7 @@
       </c>
       <c r="AR40" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>9.3</t>
         </is>
       </c>
       <c r="AS40" t="n">
@@ -12410,7 +12442,7 @@
       </c>
       <c r="AR41" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS41" t="n">
@@ -12598,7 +12630,7 @@
       </c>
       <c r="AR42" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS42" t="n">
@@ -12786,7 +12818,7 @@
       </c>
       <c r="AR43" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS43" t="n">
@@ -12969,7 +13001,7 @@
       </c>
       <c r="AR44" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS44" t="n">
@@ -13158,11 +13190,11 @@
       </c>
       <c r="AR45" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS45" t="n">
-        <v>0.35</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="46">
@@ -13355,11 +13387,11 @@
       </c>
       <c r="AR46" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS46" t="n">
-        <v>0.44</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="47">
@@ -13538,7 +13570,7 @@
       </c>
       <c r="AR47" t="inlineStr">
         <is>
-          <t>14.1</t>
+          <t>16.2</t>
         </is>
       </c>
       <c r="AS47" t="n">
@@ -13732,7 +13764,7 @@
       </c>
       <c r="AR48" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS48" t="n">
@@ -14122,11 +14154,11 @@
       </c>
       <c r="AR50" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS50" t="n">
-        <v>0.51</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="51">
@@ -14320,11 +14352,11 @@
       </c>
       <c r="AR51" t="inlineStr">
         <is>
-          <t>9.2</t>
+          <t>8.7</t>
         </is>
       </c>
       <c r="AS51" t="n">
-        <v>0.63</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="52">
@@ -14468,7 +14500,7 @@
         <v>1680</v>
       </c>
       <c r="AL52" t="n">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="AM52" t="inlineStr">
         <is>
@@ -14497,11 +14529,11 @@
       </c>
       <c r="AR52" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS52" t="n">
-        <v>0.53</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="53">
@@ -14685,7 +14717,7 @@
       </c>
       <c r="AR53" t="inlineStr">
         <is>
-          <t>2.1</t>
+          <t>2.4</t>
         </is>
       </c>
       <c r="AS53" t="n">
@@ -14849,7 +14881,7 @@
         <v>680</v>
       </c>
       <c r="AL54" t="n">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="AM54" t="inlineStr">
         <is>
@@ -14878,7 +14910,7 @@
       </c>
       <c r="AR54" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS54" t="n">
@@ -15055,11 +15087,11 @@
       </c>
       <c r="AR55" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="AS55" t="n">
-        <v>0.51</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="56">
@@ -15243,11 +15275,11 @@
       </c>
       <c r="AR56" t="inlineStr">
         <is>
-          <t>10.6</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS56" t="n">
-        <v>0.42</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="57">
@@ -15411,7 +15443,7 @@
       </c>
       <c r="AR57" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS57" t="n">
@@ -15568,7 +15600,7 @@
       </c>
       <c r="AR58" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS58" t="n">
@@ -15740,7 +15772,7 @@
       </c>
       <c r="AR59" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS59" t="n">
@@ -15898,7 +15930,7 @@
       </c>
       <c r="AR60" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>2.4</t>
         </is>
       </c>
       <c r="AS60" t="n">
@@ -16075,7 +16107,7 @@
       </c>
       <c r="AR61" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS61" t="n">
@@ -16252,7 +16284,7 @@
       </c>
       <c r="AR62" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS62" t="n">
@@ -16430,7 +16462,7 @@
       </c>
       <c r="AR63" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS63" t="n">
@@ -16607,7 +16639,7 @@
       </c>
       <c r="AR64" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS64" t="n">
@@ -16956,7 +16988,7 @@
       </c>
       <c r="AR66" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS66" t="n">
@@ -17134,11 +17166,11 @@
       </c>
       <c r="AR67" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS67" t="n">
-        <v>0.39</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="68">
@@ -17316,7 +17348,7 @@
       </c>
       <c r="AR68" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS68" t="n">
@@ -17493,7 +17525,7 @@
       </c>
       <c r="AR69" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS69" t="n">
@@ -17677,7 +17709,7 @@
       </c>
       <c r="AR70" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS70" t="n">
@@ -17854,7 +17886,7 @@
       </c>
       <c r="AR71" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS71" t="n">
@@ -18026,7 +18058,7 @@
       </c>
       <c r="AR72" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS72" t="n">
@@ -18213,7 +18245,7 @@
       </c>
       <c r="AR73" t="inlineStr">
         <is>
-          <t>8.5</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS73" t="n">
@@ -18380,7 +18412,7 @@
       </c>
       <c r="AR74" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS74" t="n">
@@ -18547,7 +18579,7 @@
       </c>
       <c r="AR75" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="AS75" t="n">
@@ -18724,7 +18756,7 @@
       </c>
       <c r="AR76" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS76" t="n">
@@ -18901,7 +18933,7 @@
       </c>
       <c r="AR77" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS77" t="n">
@@ -19073,7 +19105,7 @@
       </c>
       <c r="AR78" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS78" t="n">
@@ -19427,7 +19459,7 @@
       </c>
       <c r="AR80" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="AS80" t="n">
@@ -19604,7 +19636,7 @@
       </c>
       <c r="AR81" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS81" t="n">
@@ -19781,7 +19813,7 @@
       </c>
       <c r="AR82" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS82" t="n">
@@ -19958,7 +19990,7 @@
       </c>
       <c r="AR83" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS83" t="n">
@@ -20136,7 +20168,7 @@
       </c>
       <c r="AR84" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS84" t="n">
@@ -20313,7 +20345,7 @@
       </c>
       <c r="AR85" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS85" t="n">
@@ -20490,7 +20522,7 @@
       </c>
       <c r="AR86" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS86" t="n">
@@ -20673,7 +20705,7 @@
       </c>
       <c r="AR87" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS87" t="n">
@@ -20850,7 +20882,7 @@
       </c>
       <c r="AR88" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS88" t="n">
@@ -21027,7 +21059,7 @@
       </c>
       <c r="AR89" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS89" t="n">
@@ -21210,7 +21242,7 @@
       </c>
       <c r="AR90" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS90" t="n">
@@ -21388,7 +21420,7 @@
       </c>
       <c r="AR91" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS91" t="n">
@@ -21570,7 +21602,7 @@
       </c>
       <c r="AR92" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS92" t="n">
@@ -21737,7 +21769,7 @@
       </c>
       <c r="AR93" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS93" t="n">
@@ -21920,7 +21952,7 @@
       </c>
       <c r="AR94" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS94" t="n">
@@ -22097,7 +22129,7 @@
       </c>
       <c r="AR95" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS95" t="n">
@@ -22280,7 +22312,7 @@
       </c>
       <c r="AR96" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS96" t="n">
@@ -22448,11 +22480,11 @@
       </c>
       <c r="AR97" t="inlineStr">
         <is>
-          <t>20.5</t>
+          <t>21.3</t>
         </is>
       </c>
       <c r="AS97" t="n">
-        <v>0.39</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="98">
@@ -22617,11 +22649,11 @@
       </c>
       <c r="AR98" t="inlineStr">
         <is>
-          <t>20.5</t>
+          <t>21.0</t>
         </is>
       </c>
       <c r="AS98" t="n">
-        <v>0.39</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="99">
@@ -22775,7 +22807,7 @@
       </c>
       <c r="AR99" t="inlineStr">
         <is>
-          <t>21.1</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS99" t="n">
@@ -22944,7 +22976,7 @@
       </c>
       <c r="AR100" t="inlineStr">
         <is>
-          <t>21.1</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="AS100" t="n">
@@ -23121,7 +23153,7 @@
       </c>
       <c r="AR101" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS101" t="n">
@@ -23305,7 +23337,7 @@
       </c>
       <c r="AR102" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS102" t="n">
@@ -23467,7 +23499,7 @@
       </c>
       <c r="AR103" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS103" t="n">
@@ -23634,7 +23666,7 @@
       </c>
       <c r="AR104" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS104" t="n">
@@ -23804,11 +23836,11 @@
       </c>
       <c r="AR105" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="AS105" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="106">
@@ -24015,7 +24047,7 @@
       </c>
       <c r="AR106" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS106" t="n">
@@ -24202,11 +24234,11 @@
       </c>
       <c r="AR107" t="inlineStr">
         <is>
-          <t>8.6</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS107" t="n">
-        <v>0.61</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="108">
@@ -24382,11 +24414,11 @@
       </c>
       <c r="AR108" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS108" t="n">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="109">
@@ -24564,7 +24596,7 @@
       </c>
       <c r="AR109" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="AS109" t="n">
@@ -24749,7 +24781,7 @@
       </c>
       <c r="AR110" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS110" t="n">
@@ -24926,7 +24958,7 @@
       </c>
       <c r="AR111" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS111" t="n">
@@ -25110,7 +25142,7 @@
       </c>
       <c r="AR112" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS112" t="n">
@@ -25287,7 +25319,7 @@
       </c>
       <c r="AR113" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS113" t="n">
@@ -25464,7 +25496,7 @@
       </c>
       <c r="AR114" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS114" t="n">
@@ -25641,7 +25673,7 @@
       </c>
       <c r="AR115" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS115" t="n">
@@ -25823,7 +25855,7 @@
       </c>
       <c r="AR116" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="AS116" t="n">
@@ -26000,7 +26032,7 @@
       </c>
       <c r="AR117" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS117" t="n">
@@ -26167,7 +26199,7 @@
       </c>
       <c r="AR118" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS118" t="n">
@@ -26344,7 +26376,7 @@
       </c>
       <c r="AR119" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS119" t="n">
@@ -26513,7 +26545,7 @@
       </c>
       <c r="AR120" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS120" t="n">
@@ -26685,7 +26717,7 @@
       </c>
       <c r="AR121" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS121" t="n">
@@ -26868,7 +26900,7 @@
       </c>
       <c r="AR122" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS122" t="n">
@@ -27050,11 +27082,11 @@
       </c>
       <c r="AR123" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="AS123" t="n">
-        <v>0.3</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="124">
@@ -27227,7 +27259,7 @@
       </c>
       <c r="AR124" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS124" t="n">
@@ -27404,7 +27436,7 @@
       </c>
       <c r="AR125" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS125" t="n">
@@ -27587,7 +27619,7 @@
       </c>
       <c r="AR126" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS126" t="n">
@@ -27764,7 +27796,7 @@
       </c>
       <c r="AR127" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS127" t="n">
@@ -27951,7 +27983,7 @@
       </c>
       <c r="AR128" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS128" t="n">
@@ -28148,7 +28180,7 @@
       </c>
       <c r="AR129" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS129" t="n">
@@ -28335,7 +28367,7 @@
       </c>
       <c r="AR130" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS130" t="n">
@@ -28527,7 +28559,7 @@
       </c>
       <c r="AR131" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS131" t="n">
@@ -28720,7 +28752,7 @@
       </c>
       <c r="AR132" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>12.0</t>
         </is>
       </c>
       <c r="AS132" t="n">
@@ -28902,7 +28934,7 @@
       </c>
       <c r="AR133" t="inlineStr">
         <is>
-          <t>14.7</t>
+          <t>19.2</t>
         </is>
       </c>
       <c r="AS133" t="n">
@@ -29079,7 +29111,7 @@
       </c>
       <c r="AR134" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS134" t="n">
@@ -29256,7 +29288,7 @@
       </c>
       <c r="AR135" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS135" t="n">
@@ -29438,7 +29470,7 @@
       </c>
       <c r="AR136" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS136" t="n">
@@ -29615,7 +29647,7 @@
       </c>
       <c r="AR137" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS137" t="n">
@@ -29777,7 +29809,7 @@
       </c>
       <c r="AR138" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS138" t="n">
@@ -29944,11 +29976,11 @@
       </c>
       <c r="AR139" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS139" t="n">
-        <v>0.4</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="140">
@@ -30308,7 +30340,7 @@
       </c>
       <c r="AR141" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS141" t="n">
@@ -30486,7 +30518,7 @@
       </c>
       <c r="AR142" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS142" t="n">
@@ -30664,7 +30696,7 @@
       </c>
       <c r="AR143" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS143" t="n">
@@ -30847,7 +30879,7 @@
       </c>
       <c r="AR144" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS144" t="n">
@@ -31019,7 +31051,7 @@
       </c>
       <c r="AR145" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS145" t="n">
@@ -31201,7 +31233,7 @@
       </c>
       <c r="AR146" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS146" t="n">
@@ -31378,7 +31410,7 @@
       </c>
       <c r="AR147" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="AS147" t="n">
@@ -31555,7 +31587,7 @@
       </c>
       <c r="AR148" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS148" t="n">
@@ -31732,7 +31764,7 @@
       </c>
       <c r="AR149" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="AS149" t="n">
@@ -31920,7 +31952,7 @@
       </c>
       <c r="AR150" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS150" t="n">
@@ -32111,7 +32143,7 @@
       </c>
       <c r="AR151" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS151" t="n">
@@ -32288,7 +32320,7 @@
       </c>
       <c r="AR152" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS152" t="n">
@@ -32455,11 +32487,11 @@
       </c>
       <c r="AR153" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="AS153" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="154">
@@ -32632,7 +32664,7 @@
       </c>
       <c r="AR154" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS154" t="n">
@@ -32809,7 +32841,7 @@
       </c>
       <c r="AR155" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="AS155" t="n">
@@ -32992,7 +33024,7 @@
       </c>
       <c r="AR156" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="AS156" t="n">
@@ -33175,7 +33207,7 @@
       </c>
       <c r="AR157" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS157" t="n">
@@ -33353,7 +33385,7 @@
       </c>
       <c r="AR158" t="inlineStr">
         <is>
-          <t>10.8</t>
+          <t>12.2</t>
         </is>
       </c>
       <c r="AS158" t="n">
@@ -33530,7 +33562,7 @@
       </c>
       <c r="AR159" t="inlineStr">
         <is>
-          <t>2.1</t>
+          <t>2.4</t>
         </is>
       </c>
       <c r="AS159" t="n">
@@ -33697,7 +33729,7 @@
       </c>
       <c r="AR160" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="AS160" t="n">
@@ -33880,7 +33912,7 @@
       </c>
       <c r="AR161" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS161" t="n">
@@ -34047,7 +34079,7 @@
       </c>
       <c r="AR162" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.2</t>
         </is>
       </c>
       <c r="AS162" t="n">
@@ -34214,7 +34246,7 @@
       </c>
       <c r="AR163" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.2</t>
         </is>
       </c>
       <c r="AS163" t="n">
@@ -34419,7 +34451,7 @@
       </c>
       <c r="AR164" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS164" t="n">
@@ -34596,7 +34628,7 @@
       </c>
       <c r="AR165" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS165" t="n">
@@ -34788,11 +34820,11 @@
       </c>
       <c r="AR166" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="AS166" t="n">
-        <v>0.37</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="167">
@@ -34970,7 +35002,7 @@
       </c>
       <c r="AR167" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS167" t="n">
@@ -35330,11 +35362,11 @@
       </c>
       <c r="AR169" t="inlineStr">
         <is>
-          <t>15.1</t>
+          <t>12.1</t>
         </is>
       </c>
       <c r="AS169" t="n">
-        <v>0.68</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="170">
@@ -35512,7 +35544,7 @@
       </c>
       <c r="AR170" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS170" t="n">
@@ -35679,11 +35711,11 @@
       </c>
       <c r="AR171" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="AS171" t="n">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="172">
@@ -36201,11 +36233,11 @@
       </c>
       <c r="AR174" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS174" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="175">
@@ -36383,7 +36415,7 @@
       </c>
       <c r="AR175" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="AS175" t="n">
@@ -36550,7 +36582,7 @@
       </c>
       <c r="AR176" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS176" t="n">
@@ -36732,7 +36764,7 @@
       </c>
       <c r="AR177" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS177" t="n">
@@ -36914,7 +36946,7 @@
       </c>
       <c r="AR178" t="inlineStr">
         <is>
-          <t>14.2</t>
+          <t>13.3</t>
         </is>
       </c>
       <c r="AS178" t="n">
@@ -37101,7 +37133,7 @@
       </c>
       <c r="AR179" t="inlineStr">
         <is>
-          <t>14.2</t>
+          <t>13.6</t>
         </is>
       </c>
       <c r="AS179" t="n">
@@ -37289,7 +37321,7 @@
       </c>
       <c r="AR180" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="AS180" t="n">
@@ -37472,7 +37504,7 @@
       </c>
       <c r="AR181" t="inlineStr">
         <is>
-          <t>14.2</t>
+          <t>13.7</t>
         </is>
       </c>
       <c r="AS181" t="n">
@@ -37659,11 +37691,11 @@
       </c>
       <c r="AR182" t="inlineStr">
         <is>
-          <t>17.8</t>
+          <t>16.5</t>
         </is>
       </c>
       <c r="AS182" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="183">
@@ -37846,11 +37878,11 @@
       </c>
       <c r="AR183" t="inlineStr">
         <is>
-          <t>20.5</t>
+          <t>21.0</t>
         </is>
       </c>
       <c r="AS183" t="n">
-        <v>0.39</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="184">
@@ -38028,11 +38060,11 @@
       </c>
       <c r="AR184" t="inlineStr">
         <is>
-          <t>17.8</t>
+          <t>16.5</t>
         </is>
       </c>
       <c r="AS184" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="185">
@@ -38216,7 +38248,7 @@
       </c>
       <c r="AR185" t="inlineStr">
         <is>
-          <t>14.2</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="AS185" t="n">
@@ -38404,7 +38436,7 @@
       </c>
       <c r="AR186" t="inlineStr">
         <is>
-          <t>13.1</t>
+          <t>13.8</t>
         </is>
       </c>
       <c r="AS186" t="n">
@@ -38572,7 +38604,7 @@
       </c>
       <c r="AR187" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS187" t="n">
@@ -38764,7 +38796,7 @@
       </c>
       <c r="AR188" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS188" t="n">
@@ -38941,11 +38973,11 @@
       </c>
       <c r="AR189" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS189" t="n">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="190">
@@ -39123,7 +39155,7 @@
       </c>
       <c r="AR190" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS190" t="n">
@@ -39284,11 +39316,11 @@
       </c>
       <c r="AR191" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS191" t="n">
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="192">
@@ -39467,7 +39499,7 @@
       </c>
       <c r="AR192" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.3</t>
         </is>
       </c>
       <c r="AS192" t="n">
@@ -39650,7 +39682,7 @@
       </c>
       <c r="AR193" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS193" t="n">
@@ -39812,11 +39844,11 @@
       </c>
       <c r="AR194" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>8.9</t>
         </is>
       </c>
       <c r="AS194" t="n">
-        <v>0.49</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="195">
@@ -39974,11 +40006,11 @@
       </c>
       <c r="AR195" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>8.9</t>
         </is>
       </c>
       <c r="AS195" t="n">
-        <v>0.49</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="196">
@@ -40141,11 +40173,11 @@
       </c>
       <c r="AR196" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS196" t="n">
-        <v>0.43</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="197">
@@ -40303,7 +40335,7 @@
       </c>
       <c r="AR197" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="AS197" t="n">
@@ -40465,11 +40497,11 @@
       </c>
       <c r="AR198" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS198" t="n">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="199">
@@ -40632,11 +40664,11 @@
       </c>
       <c r="AR199" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS199" t="n">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="200">
@@ -40815,7 +40847,7 @@
       </c>
       <c r="AR200" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS200" t="n">
@@ -40998,7 +41030,7 @@
       </c>
       <c r="AR201" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS201" t="n">
@@ -41181,7 +41213,7 @@
       </c>
       <c r="AR202" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS202" t="n">
@@ -41364,7 +41396,7 @@
       </c>
       <c r="AR203" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS203" t="n">
@@ -41542,7 +41574,7 @@
       </c>
       <c r="AR204" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS204" t="n">
@@ -41720,7 +41752,7 @@
       </c>
       <c r="AR205" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS205" t="n">
@@ -41895,7 +41927,7 @@
       </c>
       <c r="AR206" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="AS206" t="n">
@@ -42078,7 +42110,7 @@
       </c>
       <c r="AR207" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS207" t="n">
@@ -42260,11 +42292,11 @@
       </c>
       <c r="AR208" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="AS208" t="n">
-        <v>0.38</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="209">
@@ -42442,11 +42474,11 @@
       </c>
       <c r="AR209" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS209" t="n">
-        <v>0.3</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="210">
@@ -42619,11 +42651,11 @@
       </c>
       <c r="AR210" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS210" t="n">
-        <v>0.61</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="211">
@@ -42801,7 +42833,7 @@
       </c>
       <c r="AR211" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS211" t="n">
@@ -42988,11 +43020,11 @@
       </c>
       <c r="AR212" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS212" t="n">
-        <v>0.51</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="213">
@@ -43171,7 +43203,7 @@
       </c>
       <c r="AR213" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS213" t="n">
@@ -43537,7 +43569,7 @@
       </c>
       <c r="AR215" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS215" t="n">
@@ -43721,7 +43753,7 @@
       </c>
       <c r="AR216" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS216" t="n">
@@ -43888,11 +43920,11 @@
       </c>
       <c r="AR217" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS217" t="n">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="218">
@@ -44056,7 +44088,7 @@
       </c>
       <c r="AR218" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS218" t="n">
@@ -44233,7 +44265,7 @@
       </c>
       <c r="AR219" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS219" t="n">
@@ -44371,7 +44403,7 @@
         <v>1280</v>
       </c>
       <c r="AL220" t="n">
-        <v>0.86</v>
+        <v>0.85</v>
       </c>
       <c r="AM220" t="inlineStr">
         <is>
@@ -44400,11 +44432,11 @@
       </c>
       <c r="AR220" t="inlineStr">
         <is>
-          <t>10.3</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS220" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="221">
@@ -44582,7 +44614,7 @@
       </c>
       <c r="AR221" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS221" t="n">
@@ -44759,7 +44791,7 @@
       </c>
       <c r="AR222" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS222" t="n">
@@ -44941,7 +44973,7 @@
       </c>
       <c r="AR223" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS223" t="n">
@@ -45301,7 +45333,7 @@
       </c>
       <c r="AR225" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS225" t="n">
@@ -45468,7 +45500,7 @@
       </c>
       <c r="AR226" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS226" t="n">
@@ -45636,11 +45668,11 @@
       </c>
       <c r="AR227" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS227" t="n">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="228">
@@ -45819,7 +45851,7 @@
       </c>
       <c r="AR228" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS228" t="n">
@@ -45987,7 +46019,7 @@
       </c>
       <c r="AR229" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS229" t="n">
@@ -46174,11 +46206,11 @@
       </c>
       <c r="AR230" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="AS230" t="n">
-        <v>0.42</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="231">
@@ -46357,7 +46389,7 @@
       </c>
       <c r="AR231" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS231" t="n">
@@ -46539,7 +46571,7 @@
       </c>
       <c r="AR232" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS232" t="n">
@@ -46711,7 +46743,7 @@
       </c>
       <c r="AR233" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS233" t="n">
@@ -46893,7 +46925,7 @@
       </c>
       <c r="AR234" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS234" t="n">
@@ -47075,7 +47107,7 @@
       </c>
       <c r="AR235" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS235" t="n">
@@ -47257,7 +47289,7 @@
       </c>
       <c r="AR236" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS236" t="n">
@@ -47439,7 +47471,7 @@
       </c>
       <c r="AR237" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS237" t="n">
@@ -47621,7 +47653,7 @@
       </c>
       <c r="AR238" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS238" t="n">
@@ -47803,7 +47835,7 @@
       </c>
       <c r="AR239" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="AS239" t="n">
@@ -47980,7 +48012,7 @@
       </c>
       <c r="AR240" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS240" t="n">
@@ -48147,11 +48179,11 @@
       </c>
       <c r="AR241" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS241" t="n">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="242">
@@ -48324,7 +48356,7 @@
       </c>
       <c r="AR242" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS242" t="n">
@@ -48506,7 +48538,7 @@
       </c>
       <c r="AR243" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS243" t="n">
@@ -48688,7 +48720,7 @@
       </c>
       <c r="AR244" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS244" t="n">
@@ -48865,7 +48897,7 @@
       </c>
       <c r="AR245" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS245" t="n">
@@ -49047,7 +49079,7 @@
       </c>
       <c r="AR246" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS246" t="n">
@@ -49214,7 +49246,7 @@
       </c>
       <c r="AR247" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS247" t="n">
@@ -49371,11 +49403,11 @@
       </c>
       <c r="AR248" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS248" t="n">
-        <v>0.42</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="249">
@@ -49540,11 +49572,11 @@
       </c>
       <c r="AR249" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS249" t="n">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="250">
@@ -49708,11 +49740,11 @@
       </c>
       <c r="AR250" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS250" t="n">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="251">
@@ -49876,11 +49908,11 @@
       </c>
       <c r="AR251" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS251" t="n">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="252">
@@ -50073,7 +50105,7 @@
       </c>
       <c r="AR252" t="inlineStr">
         <is>
-          <t>2.4</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="AS252" t="n">
@@ -50240,11 +50272,11 @@
       </c>
       <c r="AR253" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS253" t="n">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="254">
@@ -50422,11 +50454,11 @@
       </c>
       <c r="AR254" t="inlineStr">
         <is>
-          <t>17.0</t>
+          <t>16.2</t>
         </is>
       </c>
       <c r="AS254" t="n">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="255">
@@ -50599,11 +50631,11 @@
       </c>
       <c r="AR255" t="inlineStr">
         <is>
-          <t>10.7</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS255" t="n">
-        <v>0.43</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="256">
@@ -50781,7 +50813,7 @@
       </c>
       <c r="AR256" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS256" t="n">
@@ -50968,7 +51000,7 @@
       </c>
       <c r="AR257" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS257" t="n">
@@ -51155,7 +51187,7 @@
       </c>
       <c r="AR258" t="inlineStr">
         <is>
-          <t>8.5</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS258" t="n">
@@ -51342,7 +51374,7 @@
       </c>
       <c r="AR259" t="inlineStr">
         <is>
-          <t>21.1</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS259" t="n">
@@ -51530,7 +51562,7 @@
       </c>
       <c r="AR260" t="inlineStr">
         <is>
-          <t>10.9</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS260" t="n">
@@ -51717,7 +51749,7 @@
       </c>
       <c r="AR261" t="inlineStr">
         <is>
-          <t>14.2</t>
+          <t>13.4</t>
         </is>
       </c>
       <c r="AS261" t="n">
@@ -51899,11 +51931,11 @@
       </c>
       <c r="AR262" t="inlineStr">
         <is>
-          <t>17.0</t>
+          <t>16.4</t>
         </is>
       </c>
       <c r="AS262" t="n">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="263">
@@ -52076,11 +52108,11 @@
       </c>
       <c r="AR263" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS263" t="n">
-        <v>0.42</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="264">
@@ -52258,7 +52290,7 @@
       </c>
       <c r="AR264" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.3</t>
         </is>
       </c>
       <c r="AS264" t="n">
@@ -52445,7 +52477,7 @@
       </c>
       <c r="AR265" t="inlineStr">
         <is>
-          <t>14.2</t>
+          <t>13.4</t>
         </is>
       </c>
       <c r="AS265" t="n">
@@ -52633,7 +52665,7 @@
       </c>
       <c r="AR266" t="inlineStr">
         <is>
-          <t>21.1</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS266" t="n">
@@ -52815,11 +52847,11 @@
       </c>
       <c r="AR267" t="inlineStr">
         <is>
-          <t>4.1</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="AS267" t="n">
-        <v>0.3</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="268">
@@ -52992,11 +53024,11 @@
       </c>
       <c r="AR268" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS268" t="n">
-        <v>0.61</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="269">
@@ -53170,7 +53202,7 @@
       </c>
       <c r="AR269" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS269" t="n">
@@ -53348,7 +53380,7 @@
       </c>
       <c r="AR270" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS270" t="n">
@@ -53531,7 +53563,7 @@
       </c>
       <c r="AR271" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS271" t="n">
@@ -53714,7 +53746,7 @@
       </c>
       <c r="AR272" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS272" t="n">
@@ -53897,7 +53929,7 @@
       </c>
       <c r="AR273" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS273" t="n">
@@ -54075,7 +54107,7 @@
       </c>
       <c r="AR274" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS274" t="n">
@@ -54262,7 +54294,7 @@
       </c>
       <c r="AR275" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="AS275" t="n">
@@ -54627,7 +54659,7 @@
       </c>
       <c r="AR277" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS277" t="n">
@@ -54804,7 +54836,7 @@
       </c>
       <c r="AR278" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS278" t="n">
@@ -54986,7 +55018,7 @@
       </c>
       <c r="AR279" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS279" t="n">
@@ -55164,7 +55196,7 @@
       </c>
       <c r="AR280" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="AS280" t="n">
@@ -55346,7 +55378,7 @@
       </c>
       <c r="AR281" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS281" t="n">
@@ -55528,7 +55560,7 @@
       </c>
       <c r="AR282" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS282" t="n">
@@ -55710,7 +55742,7 @@
       </c>
       <c r="AR283" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS283" t="n">
@@ -55887,7 +55919,7 @@
       </c>
       <c r="AR284" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS284" t="n">
@@ -56064,7 +56096,7 @@
       </c>
       <c r="AR285" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS285" t="n">
@@ -56246,7 +56278,7 @@
       </c>
       <c r="AR286" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS286" t="n">
@@ -56423,7 +56455,7 @@
       </c>
       <c r="AR287" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS287" t="n">
@@ -56602,7 +56634,7 @@
       </c>
       <c r="AR288" t="inlineStr">
         <is>
-          <t>21.1</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS288" t="n">
@@ -56784,7 +56816,7 @@
       </c>
       <c r="AR289" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="AS289" t="n">
@@ -56961,11 +56993,11 @@
       </c>
       <c r="AR290" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS290" t="n">
-        <v>0.36</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="291">
@@ -57138,7 +57170,7 @@
       </c>
       <c r="AR291" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS291" t="n">
@@ -57316,11 +57348,11 @@
       </c>
       <c r="AR292" t="inlineStr">
         <is>
-          <t>9.8</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="AS292" t="n">
-        <v>0.53</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="293">
@@ -57493,7 +57525,7 @@
       </c>
       <c r="AR293" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="AS293" t="n">
@@ -57650,7 +57682,7 @@
       </c>
       <c r="AR294" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS294" t="n">
@@ -57833,7 +57865,7 @@
       </c>
       <c r="AR295" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS295" t="n">
@@ -58012,11 +58044,11 @@
       </c>
       <c r="AR296" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS296" t="n">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="297">
@@ -58195,7 +58227,7 @@
       </c>
       <c r="AR297" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.4</t>
         </is>
       </c>
       <c r="AS297" t="n">
@@ -58373,7 +58405,7 @@
       </c>
       <c r="AR298" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.1</t>
         </is>
       </c>
       <c r="AS298" t="n">
@@ -58535,11 +58567,11 @@
       </c>
       <c r="AR299" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS299" t="n">
-        <v>0.52</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="300">
@@ -58692,11 +58724,11 @@
       </c>
       <c r="AR300" t="inlineStr">
         <is>
-          <t>17.0</t>
+          <t>16.4</t>
         </is>
       </c>
       <c r="AS300" t="n">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="301">
@@ -58854,7 +58886,7 @@
       </c>
       <c r="AR301" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS301" t="n">
@@ -59016,7 +59048,7 @@
       </c>
       <c r="AR302" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS302" t="n">
@@ -59173,11 +59205,11 @@
       </c>
       <c r="AR303" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="AS303" t="n">
-        <v>0.63</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="304">
@@ -59330,11 +59362,11 @@
       </c>
       <c r="AR304" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="AS304" t="n">
-        <v>0.63</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="305">
@@ -59487,11 +59519,11 @@
       </c>
       <c r="AR305" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS305" t="n">
-        <v>0.47</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="306">
@@ -59664,7 +59696,7 @@
       </c>
       <c r="AR306" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS306" t="n">
@@ -59841,7 +59873,7 @@
       </c>
       <c r="AR307" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS307" t="n">
@@ -60018,7 +60050,7 @@
       </c>
       <c r="AR308" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS308" t="n">
@@ -60195,7 +60227,7 @@
       </c>
       <c r="AR309" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS309" t="n">
@@ -60382,7 +60414,7 @@
       </c>
       <c r="AR310" t="inlineStr">
         <is>
-          <t>9.0</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="AS310" t="n">
@@ -60569,7 +60601,7 @@
       </c>
       <c r="AR311" t="inlineStr">
         <is>
-          <t>8.8</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS311" t="n">
@@ -60731,11 +60763,11 @@
       </c>
       <c r="AR312" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS312" t="n">
-        <v>0.3</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="313">
@@ -60898,7 +60930,7 @@
       </c>
       <c r="AR313" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS313" t="n">
@@ -61065,11 +61097,11 @@
       </c>
       <c r="AR314" t="inlineStr">
         <is>
-          <t>11.4</t>
+          <t>11.2</t>
         </is>
       </c>
       <c r="AS314" t="n">
-        <v>0.46</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="315">
@@ -61234,7 +61266,7 @@
       </c>
       <c r="AR315" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS315" t="n">
@@ -61585,7 +61617,7 @@
       </c>
       <c r="AR317" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="AS317" t="n">
@@ -61768,11 +61800,11 @@
       </c>
       <c r="AR318" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS318" t="n">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="319">
@@ -62137,7 +62169,7 @@
       </c>
       <c r="AR320" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.8</t>
         </is>
       </c>
       <c r="AS320" t="n">
@@ -62324,7 +62356,7 @@
       </c>
       <c r="AR321" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS321" t="n">
@@ -62472,7 +62504,7 @@
         <v>1680</v>
       </c>
       <c r="AL322" t="n">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
       <c r="AM322" t="inlineStr">
         <is>
@@ -62501,7 +62533,7 @@
       </c>
       <c r="AR322" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS322" t="n">
@@ -62688,7 +62720,7 @@
       </c>
       <c r="AR323" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS323" t="n">
@@ -62870,11 +62902,11 @@
       </c>
       <c r="AR324" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS324" t="n">
-        <v>0.52</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="325">
@@ -63053,7 +63085,7 @@
       </c>
       <c r="AR325" t="inlineStr">
         <is>
-          <t>2.8</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS325" t="n">
@@ -63186,7 +63218,7 @@
         <v>1280</v>
       </c>
       <c r="AL326" t="n">
-        <v>0.32</v>
+        <v>0.31</v>
       </c>
       <c r="AM326" t="inlineStr">
         <is>
@@ -63210,11 +63242,11 @@
       </c>
       <c r="AR326" t="inlineStr">
         <is>
-          <t>11.3</t>
+          <t>8.0</t>
         </is>
       </c>
       <c r="AS326" t="n">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="327">
@@ -63392,7 +63424,7 @@
       </c>
       <c r="AR327" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>7.1</t>
         </is>
       </c>
       <c r="AS327" t="n">
@@ -63578,7 +63610,7 @@
       </c>
       <c r="AR328" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>8.6</t>
         </is>
       </c>
       <c r="AS328" t="n">
@@ -63756,7 +63788,7 @@
       </c>
       <c r="AR329" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS329" t="n">
@@ -63938,7 +63970,7 @@
       </c>
       <c r="AR330" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS330" t="n">
@@ -64099,7 +64131,7 @@
         <v>680</v>
       </c>
       <c r="AL331" t="n">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="AM331" t="inlineStr">
         <is>
@@ -64128,11 +64160,11 @@
       </c>
       <c r="AR331" t="inlineStr">
         <is>
-          <t>20.5</t>
+          <t>20.8</t>
         </is>
       </c>
       <c r="AS331" t="n">
-        <v>0.39</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="332">
@@ -64312,7 +64344,7 @@
       </c>
       <c r="AR332" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS332" t="n">
@@ -64474,7 +64506,7 @@
       </c>
       <c r="AR333" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS333" t="n">
@@ -64631,7 +64663,7 @@
       </c>
       <c r="AR334" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS334" t="n">
@@ -64788,7 +64820,7 @@
       </c>
       <c r="AR335" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS335" t="n">
@@ -64965,7 +64997,7 @@
       </c>
       <c r="AR336" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS336" t="n">
@@ -65142,11 +65174,11 @@
       </c>
       <c r="AR337" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS337" t="n">
-        <v>0.44</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="338">
@@ -65319,7 +65351,7 @@
       </c>
       <c r="AR338" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS338" t="n">
@@ -65497,7 +65529,7 @@
       </c>
       <c r="AR339" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS339" t="n">
@@ -65669,7 +65701,7 @@
       </c>
       <c r="AR340" t="inlineStr">
         <is>
-          <t>1.9</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS340" t="n">
@@ -65847,7 +65879,7 @@
       </c>
       <c r="AR341" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS341" t="n">
@@ -66007,7 +66039,7 @@
         <v>850</v>
       </c>
       <c r="AL342" t="n">
-        <v>0.91</v>
+        <v>0.9</v>
       </c>
       <c r="AM342" t="inlineStr">
         <is>
@@ -66036,7 +66068,7 @@
       </c>
       <c r="AR342" t="inlineStr">
         <is>
-          <t>8.9</t>
+          <t>6.0</t>
         </is>
       </c>
       <c r="AS342" t="n">
@@ -66226,7 +66258,7 @@
       </c>
       <c r="AR343" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS343" t="n">
@@ -66382,7 +66414,7 @@
       </c>
       <c r="AR344" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="AS344" t="n">
@@ -66561,7 +66593,7 @@
       </c>
       <c r="AR345" t="inlineStr">
         <is>
-          <t>11.1</t>
+          <t>13.1</t>
         </is>
       </c>
       <c r="AS345" t="n">
@@ -66739,7 +66771,7 @@
       </c>
       <c r="AR346" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS346" t="n">
@@ -66917,7 +66949,7 @@
       </c>
       <c r="AR347" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS347" t="n">
@@ -67074,11 +67106,11 @@
       </c>
       <c r="AR348" t="inlineStr">
         <is>
-          <t>9.2</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="AS348" t="n">
-        <v>0.63</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="349">
@@ -67231,7 +67263,7 @@
       </c>
       <c r="AR349" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="AS349" t="n">
@@ -67388,11 +67420,11 @@
       </c>
       <c r="AR350" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="AS350" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="351">
@@ -67545,11 +67577,11 @@
       </c>
       <c r="AR351" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>6.2</t>
         </is>
       </c>
       <c r="AS351" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="352">
@@ -67702,7 +67734,7 @@
       </c>
       <c r="AR352" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS352" t="n">
@@ -67835,7 +67867,7 @@
         <v>1680</v>
       </c>
       <c r="AL353" t="n">
-        <v>0.2</v>
+        <v>0.21</v>
       </c>
       <c r="AM353" t="inlineStr">
         <is>
@@ -67844,7 +67876,7 @@
       </c>
       <c r="AN353" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="AO353" t="inlineStr">
@@ -67859,11 +67891,11 @@
       </c>
       <c r="AR353" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS353" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="354">
@@ -68041,7 +68073,7 @@
       </c>
       <c r="AR354" t="inlineStr">
         <is>
-          <t>2.9</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS354" t="n">
@@ -68208,7 +68240,7 @@
       </c>
       <c r="AR355" t="inlineStr">
         <is>
-          <t>8.2</t>
+          <t>9.6</t>
         </is>
       </c>
       <c r="AS355" t="n">
@@ -68386,7 +68418,7 @@
       </c>
       <c r="AR356" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS356" t="n">
@@ -68554,7 +68586,7 @@
       </c>
       <c r="AR357" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS357" t="n">
@@ -68900,7 +68932,7 @@
       </c>
       <c r="AR359" t="inlineStr">
         <is>
-          <t>2.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS359" t="n">
@@ -69077,7 +69109,7 @@
       </c>
       <c r="AR360" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS360" t="n">
@@ -69238,11 +69270,11 @@
       </c>
       <c r="AR361" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS361" t="n">
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="362">
@@ -69405,11 +69437,11 @@
       </c>
       <c r="AR362" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="AS362" t="n">
-        <v>0.38</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="363">
@@ -69573,7 +69605,7 @@
       </c>
       <c r="AR363" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS363" t="n">
@@ -69751,7 +69783,7 @@
       </c>
       <c r="AR364" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS364" t="n">
@@ -69938,7 +69970,7 @@
       </c>
       <c r="AR365" t="inlineStr">
         <is>
-          <t>12.7</t>
+          <t>11.3</t>
         </is>
       </c>
       <c r="AS365" t="n">
@@ -70125,7 +70157,7 @@
       </c>
       <c r="AR366" t="inlineStr">
         <is>
-          <t>12.7</t>
+          <t>11.3</t>
         </is>
       </c>
       <c r="AS366" t="n">
@@ -70312,7 +70344,7 @@
       </c>
       <c r="AR367" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>13.5</t>
         </is>
       </c>
       <c r="AS367" t="n">
@@ -70479,7 +70511,7 @@
       </c>
       <c r="AR368" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS368" t="n">
@@ -70816,7 +70848,7 @@
       </c>
       <c r="AR370" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS370" t="n">
@@ -70983,7 +71015,7 @@
       </c>
       <c r="AR371" t="inlineStr">
         <is>
-          <t>14.2</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="AS371" t="n">
@@ -71151,7 +71183,7 @@
       </c>
       <c r="AR372" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS372" t="n">
@@ -71339,7 +71371,7 @@
       </c>
       <c r="AR373" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS373" t="n">
@@ -71509,11 +71541,11 @@
       </c>
       <c r="AR374" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS374" t="n">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="375">
@@ -71679,11 +71711,11 @@
       </c>
       <c r="AR375" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS375" t="n">
-        <v>0.36</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="376">
@@ -72048,7 +72080,7 @@
       </c>
       <c r="AR377" t="inlineStr">
         <is>
-          <t>2.3</t>
+          <t>2.5</t>
         </is>
       </c>
       <c r="AS377" t="n">
@@ -72394,11 +72426,11 @@
       </c>
       <c r="AR379" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS379" t="n">
-        <v>0.49</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="380">
@@ -72561,7 +72593,7 @@
       </c>
       <c r="AR380" t="inlineStr">
         <is>
-          <t>12.7</t>
+          <t>11.3</t>
         </is>
       </c>
       <c r="AS380" t="n">
@@ -72728,7 +72760,7 @@
       </c>
       <c r="AR381" t="inlineStr">
         <is>
-          <t>12.7</t>
+          <t>11.3</t>
         </is>
       </c>
       <c r="AS381" t="n">
@@ -72895,7 +72927,7 @@
       </c>
       <c r="AR382" t="inlineStr">
         <is>
-          <t>12.7</t>
+          <t>11.3</t>
         </is>
       </c>
       <c r="AS382" t="n">
@@ -73062,7 +73094,7 @@
       </c>
       <c r="AR383" t="inlineStr">
         <is>
-          <t>14.2</t>
+          <t>13.3</t>
         </is>
       </c>
       <c r="AS383" t="n">
@@ -73229,7 +73261,7 @@
       </c>
       <c r="AR384" t="inlineStr">
         <is>
-          <t>12.9</t>
+          <t>13.0</t>
         </is>
       </c>
       <c r="AS384" t="n">
@@ -73396,7 +73428,7 @@
       </c>
       <c r="AR385" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS385" t="n">
@@ -73564,11 +73596,11 @@
       </c>
       <c r="AR386" t="inlineStr">
         <is>
-          <t>10.9</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS386" t="n">
-        <v>0.43</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="387">
@@ -73731,7 +73763,7 @@
       </c>
       <c r="AR387" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS387" t="n">
@@ -73898,11 +73930,11 @@
       </c>
       <c r="AR388" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="AS388" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="389">
@@ -74056,11 +74088,11 @@
       </c>
       <c r="AR389" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS389" t="n">
-        <v>0.41</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="390">
@@ -74224,7 +74256,7 @@
       </c>
       <c r="AR390" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS390" t="n">
@@ -74402,11 +74434,11 @@
       </c>
       <c r="AR391" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS391" t="n">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="392">
@@ -74570,7 +74602,7 @@
       </c>
       <c r="AR392" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS392" t="n">
@@ -74748,7 +74780,7 @@
       </c>
       <c r="AR393" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="AS393" t="n">
@@ -74915,7 +74947,7 @@
       </c>
       <c r="AR394" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS394" t="n">
@@ -75082,7 +75114,7 @@
       </c>
       <c r="AR395" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS395" t="n">
@@ -75269,7 +75301,7 @@
       </c>
       <c r="AR396" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS396" t="n">
@@ -75436,7 +75468,7 @@
       </c>
       <c r="AR397" t="inlineStr">
         <is>
-          <t>2.7</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS397" t="n">
@@ -75514,36 +75546,36 @@
     <row r="7" ht="90" customHeight="1">
       <c r="A7" s="111" t="inlineStr">
         <is>
-          <t>The chart illustrates the Friction Pareto Analysis of an 80/20 Rule Application, showcasing the distribution of friction points across various categories. | Key: The top two categories, Scheduling &amp; Planning and Configuration &amp; Data, account for a significant proportion of friction points, with 7230 and 6130 points, respectively. | Action: Focusing on optimizing the top two categories, Scheduling &amp; Planning and Configuration &amp; Data, could lead to substantial reductions in overall friction points. By addressing these high-impact areas, significant improvements can be made to the overall process.</t>
+          <t>This chart presents a Friction Pareto Analysis of an 80/20 Rule Application, illustrating the distribution of friction points across various categories. | Key: The top two categories, Scheduling &amp; Planning and Configuration &amp; Data, account for the majority of friction points, with 7,230 and 6,130 points, respectively. | Action: Focusing on optimizing the top two categories, Scheduling &amp; Planning and Configuration &amp; Data, would likely yield the most significant reductions in friction points.</t>
         </is>
       </c>
       <c r="N7" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the Risk Origin Distribution for an Escalation Source Analysis, with a focus on Internal and External sources. | Key: The Internal source is the largest contributor to risk, accounting for 89.9% of the total. | Action: To mitigate risk, it is recommended to focus on addressing Internal sources, which are the primary drivers of risk in this analysis.</t>
+          <t>The chart is a pie chart illustrating the distribution of risk origin sources, with a focus on internal and external factors. | Key: The majority of risk origin sources are internal, accounting for 89.9% of the total, while external sources make up a smaller proportion of 10.1%. | Action: To mitigate risk, it is essential to prioritize internal risk management strategies and address the underlying causes of internal risk sources. This may involve implementing internal controls, improving processes, and enhancing employee training to reduce the likelihood of internal risk events. By a</t>
         </is>
       </c>
     </row>
     <row r="29" ht="90" customHeight="1">
       <c r="A29" s="111" t="inlineStr">
         <is>
-          <t>The chart illustrates the risk trend of a company over a period of time, with a historical perspective and a target score. | Key: The risk score has been consistently above the target score, indicating a high-risk environment. | Action: The company should focus on reducing its risk score to below the target score, as it has been above the target for an extended period. This can be achieved by implementing risk-reducing strategies and monitoring progress regularly.</t>
+          <t>The chart displays a risk trend analysis for a 3-month moving average (MA) and a target score, with a historical perspective. | Key: The risk score has been consistently below the target score for the entire period, indicating a stable and controlled risk environment. | Action: Given the stable and controlled risk environment, it is recommended to maintain the current risk management strategy and continue to monitor the risk score to ensure it remains below the target score.</t>
         </is>
       </c>
       <c r="N29" s="111" t="inlineStr">
         <is>
-          <t>The chart is a Severity-Impact Matrix Escalation Distribution Analysis, illustrating the relationship between the severity of an event and its impact on business operations. | Key: The chart reveals that the majority of events (30) have a significant impact on business operations, while only a few (1) have a critical impact. | Action: To mitigate the impact of events on business operations, it is recommended to focus on addressing the most critical events (1) and developing strategies to manage the significant impact events (30).</t>
+          <t>The chart is a severity-impact matrix for an escalation distribution analysis, showing the relationship between business impact and ticket count. | Key: The chart shows that the majority of tickets have a significant business impact, with 25 tickets having a high impact and 18 tickets having a severe impact. | Action: Based on the chart, it appears that the company should focus on addressing the most critical tickets first, as they have the most significant business impact. This could involve prioritizing resources and attention on these tickets to minimize their impact on the business.</t>
         </is>
       </c>
     </row>
-    <row r="51" ht="84" customHeight="1">
+    <row r="51" ht="90" customHeight="1">
       <c r="A51" s="111" t="inlineStr">
         <is>
-          <t>The chart displays a daily escalation count for breaches, with a focus on the impact of Smart Alert Thresholds. | Key: The chart shows a significant reduction in breaches when Smart Alert Thresholds are used, with a notable decrease in the number of breaches from 38 to 119. | Action: Based on the chart, it is recommended to implement Smart Alert Thresholds to reduce the number of breaches.</t>
+          <t>The chart illustrates the daily escalation count for breaches over a period of time, with a focus on the impact of Smart Alert Thresholds. | Key: The chart shows that the number of breaches has decreased significantly after the implementation of Smart Alert Thresholds, with a notable drop in the number of breaches from 38 to 119 to 0-2. | Action: Based on the chart, it is recommended to continue using Smart Alert Thresholds to maintain the low number of breaches and further improve breach management.</t>
         </is>
       </c>
       <c r="N51" s="111" t="inlineStr">
         <is>
-          <t>The chart displays a daily friction score with smart alert thresholds, indicating the number of breaches and daily friction score over time. | Key: The chart shows a significant increase in daily friction score from 2025-09 to 2025-11, with a peak of approximately 800 in 2025-11. | Action: Given the increasing trend and peak in 2025-11, it is recommended to closely monitor the daily friction score and consider implementing additional measures to address the potential breach.</t>
+          <t>The chart shows a daily friction score with smart alert thresholds, indicating the level of friction or resistance experienced by a system or process over time. | Key: The chart shows a significant spike in daily friction score in 2025-11, with a value of approximately 800, which is much higher than the normal range of 0-400. | Action: Based on the chart, it appears that the system or process is experiencing increasing levels of friction or resistance over time, which may be due to various factors such as increased demand, changes in the system or process, or other external factors. It may be worth investigating these factors to i</t>
         </is>
       </c>
     </row>
@@ -75557,12 +75589,12 @@
     <row r="77" ht="90" customHeight="1">
       <c r="A77" s="111" t="inlineStr">
         <is>
-          <t>The chart presents a bar graph illustrating the performance of engineers in a friction analysis, with scores ranging from 150 to 225. | Key: The top-scoring engineers, Manos Antonopoulos and Ankush Juneja, both achieved a perfect score of 281, indicating their exceptional performance in the analysis. | Action: Given the high scores across the board, it may be beneficial to focus on further improving the analysis by introducing more challenging or complex scenarios to better challenge the engineers' skills.</t>
+          <t>The chart displays the Engineer Friction Analysis Performance Risk Assessment, showcasing the performance of various engineers in a friction analysis. | Key: The chart reveals that Manos Antonopoulos and Ankush Juneja have the highest performance scores, both achieving a score of 281, while Milind Desai has the lowest score of 225. | Action: To improve performance, engineers should focus on identifying and addressing any areas of low performance, such as Milind Desai's score of 225, and work on improving their skills to achieve higher scores.</t>
         </is>
       </c>
       <c r="N77" s="111" t="inlineStr">
         <is>
-          <t>The chart illustrates the Engineer Learning Progress, comparing issue resolution (green) and repeat patterns (yellow) across various engineers. | Key: Yashpal Hans has the highest number of issues resolved (11), while Daniel Lamas has the most repeat patterns (31). | Action: To improve engineer learning progress, focus on addressing repeat patterns, as they are more prevalent than issues resolved. This could involve providing more resources or training to address these patterns.</t>
+          <t>The chart illustrates the Engineer Learning Progress, comparing issue resolution (green) and repeat patterns (yellow) across various engineers. | Key: Yashpal Hans has the highest number of issues resolved (11), while Daniel Lamas has the most repeat patterns (31). | Action: To improve overall performance, it is essential to focus on addressing repeat patterns and ensuring that all engineers have a similar number of issues resolved. This can be achieved by providing additional training or resources to those with high repeat patterns.</t>
         </is>
       </c>
     </row>
@@ -75576,19 +75608,19 @@
     <row r="103" ht="90" customHeight="1">
       <c r="A103" s="111" t="inlineStr">
         <is>
-          <t>The chart displays the LOB Friction Distribution Business Unit Performance, showcasing the average score of 62.3 and the average friction score of 56.1. | Key: The PAG business unit has the highest average score of 129.5, while the PM business unit has the lowest average score of 56.1. | Action: To improve overall performance, it is recommended to focus on the PM business unit, which needs to address its low scores and improve its performance to catch up with other business units.</t>
+          <t>The chart displays the LOB Friction Distribution Business Unit Performance, showcasing the average score of 62.3 and the average score of 62.3 for each business unit. | Key: The PAG business unit has the highest score at 129.5, while the Optimization business unit has the lowest score at 29.0. | Action: The PAG business unit's high score suggests that it is performing well and may be worth further investigation to understand its success.</t>
         </is>
       </c>
       <c r="N103" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the performance of three metrics - Volume, Friction Score, and Resolution Time - across different business lines. | Key: The Friction Score metric has the highest value across all business lines, with PAG having the highest score at 129. | Action: The Friction Score metric should be further investigated to understand the reasons behind its high score in PAG and its overall performance across all business lines.</t>
+          <t>The chart compares the performance of various business processes across three metrics: Volume (normalized), Friction Score, and Resolution Time (normalized). | Key: The Friction Score is the most critical metric, with PAG scoring 129, while PM scores 56, indicating a significant difference in the ease of use or user experience. | Action: Based on the chart, it appears that PAG is performing better than PM in all three metrics. Therefore, it is recommended to focus on improving the performance of PM to match or even surpass PAG.</t>
         </is>
       </c>
     </row>
     <row r="125" ht="90" customHeight="1">
       <c r="A125" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the distribution of issues across various categories in a business unit, with a focus on the number of issues per category. | Key: The category with the highest number of issues is PM, with over 150 issues, while others like Field, Design, and PM have fewer than 20 issues. | Action: The business unit should focus on addressing the PM category issues first, as they are the most numerous and may be causing the most significant impact on the business. This could involve prioritizing resources and resources to address these issues.</t>
+          <t>The chart shows the distribution of issues across various categories in a business unit, with a focus on the number of issues per category. | Key: The category with the highest number of issues is PM (Project Management), with over 150 issues, while others like Design, PAG, and Field have fewer than 10 issues. | Action: Based on the chart, it appears that PM is a critical area that requires more resources and attention to address the high number of issues. This could be due to various factors such as project management challenges, project scope, or project management process. It is recommended to review and address</t>
         </is>
       </c>
     </row>
@@ -75602,36 +75634,36 @@
     <row r="151" ht="90" customHeight="1">
       <c r="A151" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the root cause analysis of top escalation drivers, highlighting the most frequently occurring causes of escalations. | Key: The most common root cause of escalations is Scheduling &amp; Planning, accounting for 136 occurrences. | Action: To address the most frequent cause of escalations, Scheduling &amp; Planning, it is recommended to focus on improving planning and scheduling processes to reduce the number of escalations. This could involve implementing more efficient planning tools, training staff on better planning practices, or incr</t>
+          <t>The chart shows the Root Cause Analysis of Top Escalation Drivers, highlighting the most frequent causes of escalations. | Key: Scheduling &amp; Planning is the leading cause of escalations, accounting for 136 occurrences. | Action: Addressing Scheduling &amp; Planning issues should be a priority to reduce the number of escalations. This could involve improving communication, increasing resource allocation, or streamlining processes to reduce the frequency of these issues.</t>
         </is>
       </c>
       <c r="N151" s="111" t="inlineStr">
         <is>
-          <t>The chart presents four pie charts that display various metrics for a learning system, including data quality, model accuracy, model feedback, and learning system health. | Key: The learning system health metric has the lowest value at 78%, indicating room for improvement. | Action: To improve overall system health, focus on addressing the low health metric by identifying and addressing any issues that may be contributing to this metric. This could involve reviewing system logs, identifying and addressing any system errors, and ensuring that all system components are working pr</t>
+          <t xml:space="preserve">The chart presents four pie charts, each representing a different aspect of a system's performance: Data Quality, Learning System Integrity, Health Metrics Dashboard, and Feedback Loop. | Key: The Learning System Integrity Health Metrics Dashboard has the highest percentage of model accuracy at 87%, indicating a strong foundation for health metrics. | Action: To further improve model accuracy, focus on enhancing data quality by addressing any data-related issues that may be affecting model performance. This could involve data cleaning, data transformation, or data quality checks to ensure that data is accurate and reliable. By improving data quality, it </t>
         </is>
       </c>
     </row>
     <row r="173" ht="90" customHeight="1">
       <c r="A173" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a distribution of escalations across various categories, with Scheduling &amp; Planning having the highest number of escalations. | Key: The top three categories with the most escalations are Scheduling &amp; Planning, Documentation &amp; Reporting, and Configuration &amp; Data Mismatch. | Action: Based on the chart, it appears that Scheduling &amp; Planning is the most critical area that needs attention and resources to reduce the number of escalations. It is recommended to focus on this category to improve the overall performance.</t>
+          <t>The chart illustrates the distribution of escalations across various categories, providing a visual representation of the frequency of each category. | Key: Scheduling and Planning is the most frequent category, accounting for 85% of all escalations. | Action: Given the high frequency of Scheduling and Planning-related escalations, it may be beneficial to focus on improving processes and resources in this area to reduce the number of escalations.</t>
         </is>
       </c>
       <c r="N173" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the distribution of ticket volumes between categories and sub-categories, providing a comprehensive overview of ticket volume patterns. | Key: The chart highlights the significant difference in ticket volume between categories, with Scheduling &amp; Planning having the highest volume (43) and Site Readiness having the lowest (7). | Action: To better understand and address the underlying causes of these patterns, it is recommended to conduct further analysis on each category and sub-category to identify specific trends and patterns. This could involve exploring the causes of the high volume in Scheduling &amp; Planning and the low volume i</t>
+          <t xml:space="preserve">The chart compares the distribution of ticket volumes across categories and subcategories, providing insights into the relative popularity of each. | Key: The category "Scheduling &amp; Planning" has the highest ticket volume, with 43 tickets across all subcategories, while "Nesting &amp; Tool Error" has the lowest, with only 42 tickets. | Action: Based on the chart, it appears that Scheduling &amp; Planning is a high-priority category, while Nesting &amp; Tool Error is a low-priority category. It may be worth exploring why Scheduling &amp; Planning has such a high ticket volume, and whether there are any opportunities to reduce the number of tickets in </t>
         </is>
       </c>
     </row>
     <row r="195" ht="90" customHeight="1">
       <c r="A195" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the performance of various categories between the Baseline and Recent periods, highlighting changes in performance. | Key: The category with the most significant improvement is Nesting &amp; Tool Errors, which has seen a 198% increase. | Action: The chart suggests that focusing on categories with significant improvement, such as Nesting &amp; Tool Errors, could be a strategic move to further improve performance.</t>
+          <t>The chart compares the performance of categories in the "Emerging" and "Declining" periods, with a focus on changes from baseline. | Key: The chart highlights significant changes in categories such as "Scheduling &amp; Planning" (-58%), "Process Compliance" (-50%), and "Communication &amp; Response" (-17%), indicating a decline in performance. | Action: Based on the chart, it appears that the "Emerging" period has experienced a significant decline in performance, suggesting that the company should focus on improving these categories to maintain or improve performance.</t>
         </is>
       </c>
       <c r="N195" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the distribution of categories between a baseline (60%) and a recent (40%) period, highlighting the differences in category distribution. | Key: The most significant difference is in the "Scheduling &amp; Planning" category, which has increased from 58% to 158%, indicating a substantial shift in focus or priority. | Action: Given the significant increase in "Scheduling &amp; Planning" and the decrease in "Nestings &amp; Tool Errors", it may be beneficial to re-evaluate and adjust resources or resources to better align with current priorities. This could involve re-assigning resources or re-prioritizing projects to focus on Sch</t>
+          <t>The chart compares the distribution of categories between a baseline (60%) and a recent (40%) period. | Key: The category with the highest distribution in both periods is "Scheduling &amp; Planning" with 58% and 40% respectively. | Action: It is recommended to focus on improving the "Scheduling &amp; Planning" category to further increase its distribution in the recent period.</t>
         </is>
       </c>
     </row>
@@ -75642,22 +75674,22 @@
         </is>
       </c>
     </row>
-    <row r="221" ht="90" customHeight="1">
+    <row r="221" ht="84" customHeight="1">
       <c r="A221" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a comparison of predictive model accuracy and model performance trend analysis over a six-week period. | Key: The predictive model accuracy is consistently above 80%, with a peak of 85% in week 3. | Action: Based on the stable performance and high accuracy, it is recommended to continue using the current model with minor adjustments to further improve its performance.</t>
+          <t>The chart shows a comparison of model performance over six weeks, with scores for predictive model accuracy, model performance trend analysis, and model performance trend analysis. | Key: The chart shows that week 3 has the highest score for predictive model accuracy. | Action: Based on the chart, it appears that week 3 is a good time to evaluate and potentially improve the model's performance.</t>
         </is>
       </c>
       <c r="N221" s="111" t="inlineStr">
         <is>
-          <t>The chart compares AI Recurrence Prediction Predicted vs. Actual Rates across various categories. | Key: The chart shows that AI Recurrence Prediction Predicted rates are generally higher than actual rates, with Process Complia. having the highest predicted rate at 96% and Nesting &amp; Tool. having the lowest actual rate at 64%. | Action: Based on the chart, it appears that there is room for improvement in actual rates, especially in categories like Nesting &amp; Tool. and Process Complia. where actual rates are below predicted rates. This could be due to various factors such as data quality, model training, or data … [rest of the respon</t>
+          <t>The chart compares AI Recurrence Prediction Predicted vs. Actual Rates across various categories. | Key: The actual rates are generally higher than the predicted rates, with the largest difference being in the "Nesting &amp; Tool" category. | Action: To improve accuracy, consider retraining or adjusting the AI Recurrence Prediction model to account for these differences, particularly in categories with significant prediction-actual rate gaps.</t>
         </is>
       </c>
     </row>
     <row r="243" ht="90" customHeight="1">
       <c r="A243" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a box-and-whisker plot comparing the distribution of resolution time for different categories. | Key: The target resolution time is 2.5 days, but most categories have a much longer average resolution time, with some categories having a much longer average resolution time. | Action: It appears that there is room for improvement in most categories, as most categories have a much longer average resolution time than the target. This suggests that there may be opportunities to improve the efficiency of these categories.</t>
+          <t>The chart shows a box plot of resolution time distribution for various categories, with a target resolution time of 3 days. | Key: The actual resolution times for most categories are below the target, with most categories having a median resolution time of around 5-6 days. | Action: Based on the chart, it appears that most categories are meeting or even exceeding the target resolution time of 3 days, suggesting that the current process or resources are sufficient to meet the target. However, it's worth noting that some categories have a longer tail of slower resolution times, w</t>
         </is>
       </c>
     </row>
@@ -75671,12 +75703,12 @@
     <row r="269" ht="90" customHeight="1">
       <c r="A269" s="111" t="inlineStr">
         <is>
-          <t>The chart provides a financial impact analysis of various categories, including direct and indirect costs, with a total potential savings of $463,000. | Key: The category with the highest potential savings is Scheduling &amp; Planning, with a direct cost of $193,000 and an indirect cost of $97,000, resulting in a potential saving of $135,000. | Action: Based on the chart, it is recommended that Scheduling &amp; Planning should be given priority in the project planning and resource allocation, as it has the highest direct and indirect costs. Additionally, it is recommended that the project manager should focus on reducing the indirect costs of Scheduli</t>
+          <t>The chart shows a financial impact analysis of various categories, with direct and indirect costs, and potential savings. | Key: The category with the highest potential savings is Scheduling &amp; Planning, with a potential saving of $135,000. | Action: Based on the chart, it is recommended to focus on Scheduling &amp; Planning, as it has the highest potential savings, and explore ways to further reduce costs in this category.</t>
         </is>
       </c>
       <c r="N269" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the sub-category financial impact of top cost drivers, with a total impact of $810,000. | Key: Backhaul issues have the most significant financial impact, with a cost of $180,000, followed by MW/Transmission issues at $160,000. | Action: Based on the chart, it is recommended to focus on addressing Backhaul issues and MW/Transmission issues to reduce the financial impact of these sub- categories.</t>
+          <t>The chart displays the financial impact of various subcategories of cost drivers, with a total financial impact of $810,000. | Key: The chart reveals that Backhaul Issues have the most significant financial impact, accounting for $180,000 of the total, while Backhaul Issues and MW/Transmission Issues account for the majority of the financial impact. | Action: To address the financial impact of these subcategories, it is recommended that resources be allocated to address Backhaul Issues and MW/Transmission Issues, which account for the majority of the financial impact. This could involve investing in infrastructure or training to improve these areas.</t>
         </is>
       </c>
     </row>
@@ -75690,31 +75722,31 @@
     <row r="295" ht="90" customHeight="1">
       <c r="A295" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the distribution of similar ticket counts for 396 tickets analyzed, with an average of 3.4 matches per ticket. | Key: The distribution is skewed towards tickets with few matches, with a mean of 3.4 matches per ticket. | Action: Given the skew towards few matches, it may be worth exploring why this is the case, and whether it's due to factors such as ticket quality, or whether it’s due to other factors.</t>
+          <t>The chart shows the distribution of similar ticket counts for 396 tickets analyzed, with an average of 3.4 matches per ticket. | Key: The chart reveals that most tickets have 0-1 similar matches, with a significant spike in tickets having 5 similar matches. | Action: Based on the chart, it appears that tickets with 5 similar matches are more common than expected, suggesting that there may be a need to re-evaluate the matching algorithm or review the data for any potential errors or anomalies.</t>
         </is>
       </c>
       <c r="N295" s="111" t="inlineStr">
         <is>
-          <t>The chart presents a resolution consistency analysis based on similar ticket patterns, providing insights into the performance of various categories. | Key: The chart reveals that Scheduling &amp; Planning has the highest number of Inconsistencies (122), while Scheduling &amp; Planning also has the highest number of Inconsistencies per Category (122/7 = 17.3). | Action: Based on the chart, it is recommended to focus on improving Scheduling &amp; Planning, as it has the highest number of Incons… (122/7 = 17.3) while S… (122/7 = 17.3). This could involve… (122/7 = 17.3) while S… (122/7 = 17.3). This could involve… (122/7 = 17.3) while S… (122/7 = 17.3). This could involv</t>
+          <t>The chart provides a resolution consistency analysis based on similar ticket patterns, offering insights into the performance of various categories. | Key: The chart reveals that Scheduling &amp; Planning has the highest number of Inconsistencies (122), while Scheduling &amp; Planning also has the highest number of Inconsistencies per category (122/8 = 15.25). | Action: Based on the chart, it appears that Scheduling &amp; Planning is the most critical category for resolution consistency. Therefore, it is recommended that Scheduling &amp; Planning be given priority in  .</t>
         </is>
       </c>
     </row>
     <row r="317" ht="90" customHeight="1">
       <c r="A317" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a distribution of similarity scores for 321 matches analyzed, with a focus on high and medium confidence scores. | Key: The distribution of scores is heavily skewed towards high confidence scores, with a significant majority of scores above 0.8. | Action: Given the high concentration of high- and medium- confidence scores, it may be worth exploring ways to further increase the number of high- and medium- confidence matches, potentially through improved match- or … *   ___________________________________________________________________________________</t>
+          <t>The chart shows a distribution of similarity scores for 321 matches analyzed, with a focus on high and medium confidence scores. | Key: The chart highlights a significant difference in distribution between high and medium confidence scores, with high confidence scores having a much lower distribution. | Action: Given the difference in distribution, it may be worth exploring why high confidence scores are so low, and whether there are any specific factors or conditions that lead to this phenomenon.</t>
         </is>
       </c>
       <c r="N317" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the mean absolute differences in resolution times between expected and AI-predicted values for various categories. | Key: The mean absolute difference for "Nesting &amp; Tool" is notably higher at 40.5, while most categories have a mean absolute difference below 10. | Action: Further investigation is needed to understand why "Nestings &amp; Tool" has such a high mean absolute difference, and to explore ways to improve its accuracy.</t>
+          <t>The chart compares the mean difference in resolution time between expected (similar) tickets and AI-predicted tickets across various categories. | Key: The mean difference in resolution time is 8.3 days, with AI-predicted tickets generally taking longer to resolve. | Action: Consider investing in AI-prediction training or improving processes for categories with larger differences (e.g., Process Complia.) to reduce mean difference in resolution time.</t>
         </is>
       </c>
     </row>
     <row r="339" ht="90" customHeight="1">
       <c r="A339" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a comparison of similarity search effectiveness across various categories and origins, with a focus on match effectiveness. | Key: The chart reveals that Site Readiness and Site Readiness Readiness have the highest match effectiveness, with 100% and 92% respectively. | Action: Based on the chart, it appears that Site Readiness and Site Readiness Readiness are the most effective categories for similarity search, and should be prioritized for further investigation.</t>
+          <t>The chart shows a comparison of similarity search effectiveness across various categories and sources, with a focus on origin and external sources. | Key: The chart highlights that Site Readiness and Site Readiness-related categories have the highest match effectiveness, with Site Readiness itself having a 100% match effectiveness. | Action: Based on the chart, it appears that internal sources are more effective for similarity searches, and therefore, it may be worth considering using internal sources for future searches.</t>
         </is>
       </c>
     </row>
@@ -75728,31 +75760,31 @@
     <row r="365" ht="90" customHeight="1">
       <c r="A365" s="111" t="inlineStr">
         <is>
-          <t>The chart displays learning effectiveness scores for various categories based on recurrence, lesson completion, and consistency. | Key: The category with the highest learning effectiveness score is "Nesting &amp; Tool Error" with a score of 12, while "Process Compliance" has the lowest score of 1. | Action: Based on the chart, it appears that there is room for improvement in many categories, particularly "Nesting &amp; Tool Error" and "Communication &amp; Response" which both have high scores. It may be worth exploring ways to improve these areas to further enhance learning effectiveness.</t>
+          <t>The chart shows a bar chart of learning effectiveness scores for various categories based on 100% learning effectiveness. | Key: The category with the lowest learning effectiveness score is Process Compliancy at F (2), while Nesting &amp; Tool Error has the highest at F (12). | Action: Given that most categories have F (4) or F (6) scores, it is recommended to focus on improving these categories to achieve better learning effectiveness scores. This could involve re-assigning resources, training, or other resources to these categories.</t>
         </is>
       </c>
       <c r="N365" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the lesson documentation and completion rate by category, with a focus on the percentage of lessons completed. | Key: The chart reveals that all categories have a completion rate of 0%, indicating that no lessons have been completed in any category. | Action: Given the lack of progress in any category, it is recommended to review and adjust the lesson documentation and completion process to improve the overall rate of completion. This could involve identifying and addressing any issues or challenges that are preventing progress in each category.</t>
+          <t>The chart shows the lesson documentation and completion rate for different categories. | Key: The chart shows that all categories have a completion rate of 0%, indicating that no lessons were completed. | Action: Based on the chart, it appears that there is a need to improve the completion rate of lessons in all categories. This could be achieved by increasing the number of lessons completed or improving the process of documenting and completing lessons.</t>
         </is>
       </c>
     </row>
     <row r="387" ht="90" customHeight="1">
       <c r="A387" s="111" t="inlineStr">
         <is>
-          <t xml:space="preserve">The chart compares the Recurrence Rate (RR) of lessons and their corresponding Recurrence Rate (RR) of the lessons' completion. It shows that lessons with higher Recurrence Rates (RR) tend to have lower completion rates. | Key: The chart highlights a negative correlation between Recurrence Rate (RR) and lesson completion rates. Lessons with higher Recurrence Rates (RR) tend to have lower completion rates. | Action: Based on the chart, it is recommended to focus on improving the Recorrrer (a software tool) to reduce its Recorrrer Rate (RR) and improve lesson completion rates. This can be achieved by implementing *   A : [Action] to [Desire] by [Means] *   B : [Action] to [Desire] by [Means] *   C : [Action] to </t>
+          <t>The chart compares the Recurrence Rate of Bottom-Right (Low Recurrence, High Completion) and Lesson-Only (Low Recurrence, Low Completion) approaches. | Key: The chart shows that both approaches have similar Recurrence Rates, with both being around 90-95%. | Action: Given that both approaches have similar Recurrence Rates, it may be worth considering other factors such as resource allocation, cost, and resource management when making decisions.</t>
         </is>
       </c>
       <c r="N387" s="111" t="inlineStr">
         <is>
-          <t>The chart displays a heat map of learning effectiveness for various categories, with green indicating good learning and red indicating needs attention. | Key: The category with the highest learning score is "Communication &amp;." with 77, while "Nesting &amp; Tool" has the lowest score at 13. | Action: Based on the chart, it appears that "Communication &amp;." is a category that requires less attention, while "Nesting &amp; Tool" needs more attention. Therefore, it is recommended to focus on improving the latter category.</t>
+          <t>The chart illustrates the learning effectiveness of various categories across different business lines, with each category represented by a bar and each business line represented by a different color. | Key: The category with the highest learning effectiveness is "Communication &amp;...," with a score of 77. | Action: Based on the chart, it appears that investing in categories with lower learning effectiveness, such as "Nesting &amp; Tool..." and "Scheduling &amp; PI...", could lead to significant improvements in overall learning effectiveness.</t>
         </is>
       </c>
     </row>
     <row r="409" ht="90" customHeight="1">
       <c r="A409" s="111" t="inlineStr">
         <is>
-          <t>The chart presents AI-generated improvement recommendations for various aspects of an organization's processes, including Process Compliance, Scheduling &amp; Planning, Site Readiness, Documentation &amp; Reporting, and Validation &amp; Quality (Val &amp; Q). | Key: The chart highlights that all five areas have a critical (C) rating, indicating that all areas need improvement. The areas with the most critical need for improvement are Process Compliance (96% recurrence) and Scheduling &amp; Planning (93% recurrence).</t>
+          <t xml:space="preserve">The chart presents an AI-generated improvement recommendations chart for various AI-generated improvement recommendations. | Key: The chart shows that all categories have a critical (C) rating, indicating that all categories are critical and need improvement. | Action: Based on the chart, it is recommended to focus on improving all categories as they all have a critical (C) rating, indicating that all categories need improvement. This can be done by focusing on improving process compliance, scheduling and planning, site readiness, documentation and reporting, and </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Overhaul financial calculations: rework cost only, remove delay fabrication
Formula change:
  OLD: (Material + Labor + Delay) × Severity × (1 + Origin)
  NEW: (Material + Labor_Hours × Hourly_Rate) × Severity × (1 + Origin)

Removed delay_cost entirely - no data exists to support delay duration
estimates. Financial_Impact now represents pure rework cost.

Fixes from comprehensive review:
- Remove delay_cost from price_catalog.py, dashboard, and all fallbacks
- Fix preventable categories to match actual 8-category AI classification
  (was using old category names that matched nothing)
- Replace silent fallback (Score × 15) with visible st.error() warning
- If price_catalog fails, use existing Excel values or show $0 (not fake numbers)

Impact: Total Financial_Impact $478K → $36K (pure rework cost, defensible)

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Strategic_Report.xlsx
+++ b/Strategic_Report.xlsx
@@ -5069,7 +5069,7 @@
         </is>
       </c>
       <c r="AK2" t="n">
-        <v>35</v>
+        <v>17.5</v>
       </c>
       <c r="AL2" t="n">
         <v>0.91</v>
@@ -5267,7 +5267,7 @@
         </is>
       </c>
       <c r="AK3" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL3" t="n">
         <v>0.92</v>
@@ -5455,7 +5455,7 @@
         </is>
       </c>
       <c r="AK4" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL4" t="n">
         <v>1</v>
@@ -5634,7 +5634,7 @@
         </is>
       </c>
       <c r="AK5" t="n">
-        <v>816</v>
+        <v>168</v>
       </c>
       <c r="AL5" t="n">
         <v>0.98</v>
@@ -5819,7 +5819,7 @@
         </is>
       </c>
       <c r="AK6" t="n">
-        <v>2040</v>
+        <v>240</v>
       </c>
       <c r="AL6" t="n">
         <v>0.93</v>
@@ -6012,7 +6012,7 @@
         </is>
       </c>
       <c r="AK7" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL7" t="n">
         <v>1</v>
@@ -6210,7 +6210,7 @@
         </is>
       </c>
       <c r="AK8" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL8" t="n">
         <v>1</v>
@@ -6398,7 +6398,7 @@
         </is>
       </c>
       <c r="AK9" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL9" t="n">
         <v>0.97</v>
@@ -6591,7 +6591,7 @@
         </is>
       </c>
       <c r="AK10" t="n">
-        <v>816</v>
+        <v>168</v>
       </c>
       <c r="AL10" t="n">
         <v>0.95</v>
@@ -6769,7 +6769,7 @@
         </is>
       </c>
       <c r="AK11" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL11" t="n">
         <v>1</v>
@@ -6946,7 +6946,7 @@
         </is>
       </c>
       <c r="AK12" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL12" t="n">
         <v>0.97</v>
@@ -7144,7 +7144,7 @@
         </is>
       </c>
       <c r="AK13" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL13" t="n">
         <v>0.97</v>
@@ -7337,7 +7337,7 @@
         </is>
       </c>
       <c r="AK14" t="n">
-        <v>4992</v>
+        <v>336</v>
       </c>
       <c r="AL14" t="n">
         <v>0.97</v>
@@ -7530,7 +7530,7 @@
         </is>
       </c>
       <c r="AK15" t="n">
-        <v>5040</v>
+        <v>240</v>
       </c>
       <c r="AL15" t="n">
         <v>0.36</v>
@@ -7715,7 +7715,7 @@
         </is>
       </c>
       <c r="AK16" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL16" t="n">
         <v>0.95</v>
@@ -7887,7 +7887,7 @@
         </is>
       </c>
       <c r="AK17" t="n">
-        <v>2016</v>
+        <v>168</v>
       </c>
       <c r="AL17" t="n">
         <v>0.95</v>
@@ -8075,7 +8075,7 @@
         </is>
       </c>
       <c r="AK18" t="n">
-        <v>2040</v>
+        <v>240</v>
       </c>
       <c r="AL18" t="n">
         <v>0.96</v>
@@ -8258,7 +8258,7 @@
         </is>
       </c>
       <c r="AK19" t="n">
-        <v>2040</v>
+        <v>240</v>
       </c>
       <c r="AL19" t="n">
         <v>0.96</v>
@@ -8432,7 +8432,7 @@
         </is>
       </c>
       <c r="AK20" t="n">
-        <v>2040</v>
+        <v>240</v>
       </c>
       <c r="AL20" t="n">
         <v>0.24</v>
@@ -8610,7 +8610,7 @@
         </is>
       </c>
       <c r="AK21" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL21" t="n">
         <v>0.96</v>
@@ -8793,7 +8793,7 @@
         </is>
       </c>
       <c r="AK22" t="n">
-        <v>2016</v>
+        <v>168</v>
       </c>
       <c r="AL22" t="n">
         <v>0.92</v>
@@ -8986,7 +8986,7 @@
         </is>
       </c>
       <c r="AK23" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL23" t="n">
         <v>1</v>
@@ -9185,7 +9185,7 @@
         </is>
       </c>
       <c r="AK24" t="n">
-        <v>168</v>
+        <v>84</v>
       </c>
       <c r="AL24" t="n">
         <v>0.95</v>
@@ -9373,7 +9373,7 @@
         </is>
       </c>
       <c r="AK25" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL25" t="n">
         <v>0.9399999999999999</v>
@@ -9555,7 +9555,7 @@
         </is>
       </c>
       <c r="AK26" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL26" t="n">
         <v>0.9399999999999999</v>
@@ -9743,7 +9743,7 @@
         </is>
       </c>
       <c r="AK27" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL27" t="n">
         <v>1</v>
@@ -9930,7 +9930,7 @@
         </is>
       </c>
       <c r="AK28" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL28" t="n">
         <v>0.89</v>
@@ -10119,7 +10119,7 @@
         </is>
       </c>
       <c r="AK29" t="n">
-        <v>168</v>
+        <v>84</v>
       </c>
       <c r="AL29" t="n">
         <v>0.9399999999999999</v>
@@ -10314,7 +10314,7 @@
         </is>
       </c>
       <c r="AK30" t="n">
-        <v>816</v>
+        <v>168</v>
       </c>
       <c r="AL30" t="n">
         <v>0.9399999999999999</v>
@@ -10512,7 +10512,7 @@
         </is>
       </c>
       <c r="AK31" t="n">
-        <v>816</v>
+        <v>168</v>
       </c>
       <c r="AL31" t="n">
         <v>0.98</v>
@@ -10700,7 +10700,7 @@
         </is>
       </c>
       <c r="AK32" t="n">
-        <v>1280</v>
+        <v>80</v>
       </c>
       <c r="AL32" t="n">
         <v>0.97</v>
@@ -10893,7 +10893,7 @@
         </is>
       </c>
       <c r="AK33" t="n">
-        <v>1280</v>
+        <v>80</v>
       </c>
       <c r="AL33" t="n">
         <v>0.97</v>
@@ -11091,7 +11091,7 @@
         </is>
       </c>
       <c r="AK34" t="n">
-        <v>816</v>
+        <v>168</v>
       </c>
       <c r="AL34" t="n">
         <v>0.98</v>
@@ -11288,7 +11288,7 @@
         </is>
       </c>
       <c r="AK35" t="n">
-        <v>1536</v>
+        <v>96</v>
       </c>
       <c r="AL35" t="n">
         <v>0.1</v>
@@ -11466,7 +11466,7 @@
         </is>
       </c>
       <c r="AK36" t="n">
-        <v>168</v>
+        <v>84</v>
       </c>
       <c r="AL36" t="n">
         <v>0.93</v>
@@ -11649,7 +11649,7 @@
         </is>
       </c>
       <c r="AK37" t="n">
-        <v>1280</v>
+        <v>80</v>
       </c>
       <c r="AL37" t="n">
         <v>0.96</v>
@@ -11836,7 +11836,7 @@
         </is>
       </c>
       <c r="AK38" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL38" t="n">
         <v>0.93</v>
@@ -12027,7 +12027,7 @@
         </is>
       </c>
       <c r="AK39" t="n">
-        <v>2496</v>
+        <v>168</v>
       </c>
       <c r="AL39" t="n">
         <v>0.99</v>
@@ -12223,7 +12223,7 @@
         </is>
       </c>
       <c r="AK40" t="n">
-        <v>816</v>
+        <v>168</v>
       </c>
       <c r="AL40" t="n">
         <v>0.95</v>
@@ -12410,7 +12410,7 @@
         </is>
       </c>
       <c r="AK41" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL41" t="n">
         <v>1</v>
@@ -12598,7 +12598,7 @@
         </is>
       </c>
       <c r="AK42" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL42" t="n">
         <v>1</v>
@@ -12786,7 +12786,7 @@
         </is>
       </c>
       <c r="AK43" t="n">
-        <v>1280</v>
+        <v>80</v>
       </c>
       <c r="AL43" t="n">
         <v>0.99</v>
@@ -12969,7 +12969,7 @@
         </is>
       </c>
       <c r="AK44" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL44" t="n">
         <v>0.37</v>
@@ -13158,7 +13158,7 @@
         </is>
       </c>
       <c r="AK45" t="n">
-        <v>5040</v>
+        <v>240</v>
       </c>
       <c r="AL45" t="n">
         <v>0.92</v>
@@ -13360,7 +13360,7 @@
         </is>
       </c>
       <c r="AK46" t="n">
-        <v>2016</v>
+        <v>96</v>
       </c>
       <c r="AL46" t="n">
         <v>0.12</v>
@@ -13538,7 +13538,7 @@
         </is>
       </c>
       <c r="AK47" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL47" t="n">
         <v>0.95</v>
@@ -13737,7 +13737,7 @@
         </is>
       </c>
       <c r="AK48" t="n">
-        <v>816</v>
+        <v>168</v>
       </c>
       <c r="AL48" t="n">
         <v>0.9399999999999999</v>
@@ -13927,7 +13927,7 @@
         </is>
       </c>
       <c r="AK49" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL49" t="n">
         <v>0.99</v>
@@ -14127,7 +14127,7 @@
         </is>
       </c>
       <c r="AK50" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL50" t="n">
         <v>0.11</v>
@@ -14325,7 +14325,7 @@
         </is>
       </c>
       <c r="AK51" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL51" t="n">
         <v>0.12</v>
@@ -14497,7 +14497,7 @@
         </is>
       </c>
       <c r="AK52" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL52" t="n">
         <v>0.99</v>
@@ -14685,7 +14685,7 @@
         </is>
       </c>
       <c r="AK53" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL53" t="n">
         <v>0.92</v>
@@ -14878,7 +14878,7 @@
         </is>
       </c>
       <c r="AK54" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL54" t="n">
         <v>0.96</v>
@@ -15055,7 +15055,7 @@
         </is>
       </c>
       <c r="AK55" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL55" t="n">
         <v>0.97</v>
@@ -15243,7 +15243,7 @@
         </is>
       </c>
       <c r="AK56" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL56" t="n">
         <v>0.92</v>
@@ -15411,7 +15411,7 @@
         </is>
       </c>
       <c r="AK57" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL57" t="n">
         <v>0.92</v>
@@ -15568,7 +15568,7 @@
         </is>
       </c>
       <c r="AK58" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL58" t="n">
         <v>0.93</v>
@@ -15740,7 +15740,7 @@
         </is>
       </c>
       <c r="AK59" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL59" t="n">
         <v>0.93</v>
@@ -15898,7 +15898,7 @@
         </is>
       </c>
       <c r="AK60" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL60" t="n">
         <v>0.85</v>
@@ -16075,7 +16075,7 @@
         </is>
       </c>
       <c r="AK61" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL61" t="n">
         <v>0.92</v>
@@ -16252,7 +16252,7 @@
         </is>
       </c>
       <c r="AK62" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL62" t="n">
         <v>0.92</v>
@@ -16430,7 +16430,7 @@
         </is>
       </c>
       <c r="AK63" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL63" t="n">
         <v>0.9</v>
@@ -16607,7 +16607,7 @@
         </is>
       </c>
       <c r="AK64" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL64" t="n">
         <v>0.89</v>
@@ -16774,7 +16774,7 @@
         </is>
       </c>
       <c r="AK65" t="n">
-        <v>4160</v>
+        <v>160</v>
       </c>
       <c r="AL65" t="n">
         <v>0.91</v>
@@ -16956,7 +16956,7 @@
         </is>
       </c>
       <c r="AK66" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL66" t="n">
         <v>0.95</v>
@@ -17134,7 +17134,7 @@
         </is>
       </c>
       <c r="AK67" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL67" t="n">
         <v>0.95</v>
@@ -17316,7 +17316,7 @@
         </is>
       </c>
       <c r="AK68" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL68" t="n">
         <v>0.93</v>
@@ -17493,7 +17493,7 @@
         </is>
       </c>
       <c r="AK69" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL69" t="n">
         <v>0.95</v>
@@ -17677,7 +17677,7 @@
         </is>
       </c>
       <c r="AK70" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL70" t="n">
         <v>0.9399999999999999</v>
@@ -17854,7 +17854,7 @@
         </is>
       </c>
       <c r="AK71" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL71" t="n">
         <v>0.9399999999999999</v>
@@ -18026,7 +18026,7 @@
         </is>
       </c>
       <c r="AK72" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL72" t="n">
         <v>0.93</v>
@@ -18213,7 +18213,7 @@
         </is>
       </c>
       <c r="AK73" t="n">
-        <v>680</v>
+        <v>80</v>
       </c>
       <c r="AL73" t="n">
         <v>0.93</v>
@@ -18380,7 +18380,7 @@
         </is>
       </c>
       <c r="AK74" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL74" t="n">
         <v>0.96</v>
@@ -18547,7 +18547,7 @@
         </is>
       </c>
       <c r="AK75" t="n">
-        <v>4160</v>
+        <v>160</v>
       </c>
       <c r="AL75" t="n">
         <v>0.96</v>
@@ -18724,7 +18724,7 @@
         </is>
       </c>
       <c r="AK76" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL76" t="n">
         <v>0.95</v>
@@ -18901,7 +18901,7 @@
         </is>
       </c>
       <c r="AK77" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL77" t="n">
         <v>0.95</v>
@@ -19073,7 +19073,7 @@
         </is>
       </c>
       <c r="AK78" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL78" t="n">
         <v>0.9399999999999999</v>
@@ -19245,7 +19245,7 @@
         </is>
       </c>
       <c r="AK79" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL79" t="n">
         <v>0.95</v>
@@ -19427,7 +19427,7 @@
         </is>
       </c>
       <c r="AK80" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL80" t="n">
         <v>0.96</v>
@@ -19604,7 +19604,7 @@
         </is>
       </c>
       <c r="AK81" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL81" t="n">
         <v>0.95</v>
@@ -19781,7 +19781,7 @@
         </is>
       </c>
       <c r="AK82" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL82" t="n">
         <v>0.9399999999999999</v>
@@ -19958,7 +19958,7 @@
         </is>
       </c>
       <c r="AK83" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL83" t="n">
         <v>0.9399999999999999</v>
@@ -20136,7 +20136,7 @@
         </is>
       </c>
       <c r="AK84" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL84" t="n">
         <v>0.93</v>
@@ -20313,7 +20313,7 @@
         </is>
       </c>
       <c r="AK85" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL85" t="n">
         <v>0.9399999999999999</v>
@@ -20490,7 +20490,7 @@
         </is>
       </c>
       <c r="AK86" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL86" t="n">
         <v>0.95</v>
@@ -20673,7 +20673,7 @@
         </is>
       </c>
       <c r="AK87" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL87" t="n">
         <v>0.95</v>
@@ -20850,7 +20850,7 @@
         </is>
       </c>
       <c r="AK88" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL88" t="n">
         <v>0.96</v>
@@ -21027,7 +21027,7 @@
         </is>
       </c>
       <c r="AK89" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL89" t="n">
         <v>0.92</v>
@@ -21210,7 +21210,7 @@
         </is>
       </c>
       <c r="AK90" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL90" t="n">
         <v>0.93</v>
@@ -21388,7 +21388,7 @@
         </is>
       </c>
       <c r="AK91" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL91" t="n">
         <v>0.93</v>
@@ -21570,7 +21570,7 @@
         </is>
       </c>
       <c r="AK92" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL92" t="n">
         <v>0.98</v>
@@ -21737,7 +21737,7 @@
         </is>
       </c>
       <c r="AK93" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL93" t="n">
         <v>0.91</v>
@@ -21920,7 +21920,7 @@
         </is>
       </c>
       <c r="AK94" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL94" t="n">
         <v>0.97</v>
@@ -22097,7 +22097,7 @@
         </is>
       </c>
       <c r="AK95" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL95" t="n">
         <v>0.9399999999999999</v>
@@ -22280,7 +22280,7 @@
         </is>
       </c>
       <c r="AK96" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL96" t="n">
         <v>0.97</v>
@@ -22448,7 +22448,7 @@
         </is>
       </c>
       <c r="AK97" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL97" t="n">
         <v>0.97</v>
@@ -22617,7 +22617,7 @@
         </is>
       </c>
       <c r="AK98" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL98" t="n">
         <v>0.9399999999999999</v>
@@ -22775,7 +22775,7 @@
         </is>
       </c>
       <c r="AK99" t="n">
-        <v>340</v>
+        <v>70</v>
       </c>
       <c r="AL99" t="n">
         <v>0.96</v>
@@ -22944,7 +22944,7 @@
         </is>
       </c>
       <c r="AK100" t="n">
-        <v>340</v>
+        <v>70</v>
       </c>
       <c r="AL100" t="n">
         <v>0.95</v>
@@ -23121,7 +23121,7 @@
         </is>
       </c>
       <c r="AK101" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL101" t="n">
         <v>0.92</v>
@@ -23305,7 +23305,7 @@
         </is>
       </c>
       <c r="AK102" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL102" t="n">
         <v>0.9399999999999999</v>
@@ -23467,7 +23467,7 @@
         </is>
       </c>
       <c r="AK103" t="n">
-        <v>1280</v>
+        <v>80</v>
       </c>
       <c r="AL103" t="n">
         <v>0.91</v>
@@ -23634,7 +23634,7 @@
         </is>
       </c>
       <c r="AK104" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL104" t="n">
         <v>0.9399999999999999</v>
@@ -23804,7 +23804,7 @@
         </is>
       </c>
       <c r="AK105" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL105" t="n">
         <v>0.9399999999999999</v>
@@ -24015,7 +24015,7 @@
         </is>
       </c>
       <c r="AK106" t="n">
-        <v>10400</v>
+        <v>400</v>
       </c>
       <c r="AL106" t="n">
         <v>0.93</v>
@@ -24202,7 +24202,7 @@
         </is>
       </c>
       <c r="AK107" t="n">
-        <v>4200</v>
+        <v>200</v>
       </c>
       <c r="AL107" t="n">
         <v>0.92</v>
@@ -24382,7 +24382,7 @@
         </is>
       </c>
       <c r="AK108" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL108" t="n">
         <v>0.9399999999999999</v>
@@ -24564,7 +24564,7 @@
         </is>
       </c>
       <c r="AK109" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL109" t="n">
         <v>0.9399999999999999</v>
@@ -24749,7 +24749,7 @@
         </is>
       </c>
       <c r="AK110" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL110" t="n">
         <v>0.97</v>
@@ -24926,7 +24926,7 @@
         </is>
       </c>
       <c r="AK111" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL111" t="n">
         <v>0.97</v>
@@ -25110,7 +25110,7 @@
         </is>
       </c>
       <c r="AK112" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL112" t="n">
         <v>0.96</v>
@@ -25287,7 +25287,7 @@
         </is>
       </c>
       <c r="AK113" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL113" t="n">
         <v>0.95</v>
@@ -25464,7 +25464,7 @@
         </is>
       </c>
       <c r="AK114" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL114" t="n">
         <v>0.96</v>
@@ -25641,7 +25641,7 @@
         </is>
       </c>
       <c r="AK115" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL115" t="n">
         <v>0.96</v>
@@ -25823,7 +25823,7 @@
         </is>
       </c>
       <c r="AK116" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL116" t="n">
         <v>0.96</v>
@@ -26000,7 +26000,7 @@
         </is>
       </c>
       <c r="AK117" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL117" t="n">
         <v>0.9399999999999999</v>
@@ -26167,7 +26167,7 @@
         </is>
       </c>
       <c r="AK118" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL118" t="n">
         <v>0.99</v>
@@ -26344,7 +26344,7 @@
         </is>
       </c>
       <c r="AK119" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL119" t="n">
         <v>0.92</v>
@@ -26513,7 +26513,7 @@
         </is>
       </c>
       <c r="AK120" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL120" t="n">
         <v>0.93</v>
@@ -26685,7 +26685,7 @@
         </is>
       </c>
       <c r="AK121" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL121" t="n">
         <v>0.95</v>
@@ -26868,7 +26868,7 @@
         </is>
       </c>
       <c r="AK122" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL122" t="n">
         <v>0.98</v>
@@ -27050,7 +27050,7 @@
         </is>
       </c>
       <c r="AK123" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL123" t="n">
         <v>0.95</v>
@@ -27227,7 +27227,7 @@
         </is>
       </c>
       <c r="AK124" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL124" t="n">
         <v>0.96</v>
@@ -27404,7 +27404,7 @@
         </is>
       </c>
       <c r="AK125" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL125" t="n">
         <v>0.9399999999999999</v>
@@ -27587,7 +27587,7 @@
         </is>
       </c>
       <c r="AK126" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL126" t="n">
         <v>0.97</v>
@@ -27764,7 +27764,7 @@
         </is>
       </c>
       <c r="AK127" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL127" t="n">
         <v>0.95</v>
@@ -27951,7 +27951,7 @@
         </is>
       </c>
       <c r="AK128" t="n">
-        <v>5200</v>
+        <v>200</v>
       </c>
       <c r="AL128" t="n">
         <v>0.9399999999999999</v>
@@ -28148,7 +28148,7 @@
         </is>
       </c>
       <c r="AK129" t="n">
-        <v>10400</v>
+        <v>400</v>
       </c>
       <c r="AL129" t="n">
         <v>0.95</v>
@@ -28335,7 +28335,7 @@
         </is>
       </c>
       <c r="AK130" t="n">
-        <v>10400</v>
+        <v>400</v>
       </c>
       <c r="AL130" t="n">
         <v>0.91</v>
@@ -28527,7 +28527,7 @@
         </is>
       </c>
       <c r="AK131" t="n">
-        <v>10400</v>
+        <v>400</v>
       </c>
       <c r="AL131" t="n">
         <v>0.9399999999999999</v>
@@ -28720,7 +28720,7 @@
         </is>
       </c>
       <c r="AK132" t="n">
-        <v>340</v>
+        <v>70</v>
       </c>
       <c r="AL132" t="n">
         <v>0.96</v>
@@ -28902,7 +28902,7 @@
         </is>
       </c>
       <c r="AK133" t="n">
-        <v>340</v>
+        <v>70</v>
       </c>
       <c r="AL133" t="n">
         <v>0.96</v>
@@ -29079,7 +29079,7 @@
         </is>
       </c>
       <c r="AK134" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL134" t="n">
         <v>0.95</v>
@@ -29256,7 +29256,7 @@
         </is>
       </c>
       <c r="AK135" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL135" t="n">
         <v>0.95</v>
@@ -29438,7 +29438,7 @@
         </is>
       </c>
       <c r="AK136" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL136" t="n">
         <v>0.96</v>
@@ -29615,7 +29615,7 @@
         </is>
       </c>
       <c r="AK137" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL137" t="n">
         <v>0.97</v>
@@ -29777,7 +29777,7 @@
         </is>
       </c>
       <c r="AK138" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL138" t="n">
         <v>0.89</v>
@@ -29944,7 +29944,7 @@
         </is>
       </c>
       <c r="AK139" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL139" t="n">
         <v>0.9</v>
@@ -30130,7 +30130,7 @@
         </is>
       </c>
       <c r="AK140" t="n">
-        <v>4160</v>
+        <v>160</v>
       </c>
       <c r="AL140" t="n">
         <v>0.9399999999999999</v>
@@ -30308,7 +30308,7 @@
         </is>
       </c>
       <c r="AK141" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL141" t="n">
         <v>0.99</v>
@@ -30486,7 +30486,7 @@
         </is>
       </c>
       <c r="AK142" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL142" t="n">
         <v>0.98</v>
@@ -30664,7 +30664,7 @@
         </is>
       </c>
       <c r="AK143" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL143" t="n">
         <v>0.99</v>
@@ -30847,7 +30847,7 @@
         </is>
       </c>
       <c r="AK144" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL144" t="n">
         <v>0.9399999999999999</v>
@@ -31019,7 +31019,7 @@
         </is>
       </c>
       <c r="AK145" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL145" t="n">
         <v>0.95</v>
@@ -31201,7 +31201,7 @@
         </is>
       </c>
       <c r="AK146" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL146" t="n">
         <v>0.93</v>
@@ -31378,7 +31378,7 @@
         </is>
       </c>
       <c r="AK147" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL147" t="n">
         <v>0.95</v>
@@ -31555,7 +31555,7 @@
         </is>
       </c>
       <c r="AK148" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL148" t="n">
         <v>0.97</v>
@@ -31732,7 +31732,7 @@
         </is>
       </c>
       <c r="AK149" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL149" t="n">
         <v>0.93</v>
@@ -31920,7 +31920,7 @@
         </is>
       </c>
       <c r="AK150" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL150" t="n">
         <v>0.9399999999999999</v>
@@ -32116,7 +32116,7 @@
         </is>
       </c>
       <c r="AK151" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL151" t="n">
         <v>0.23</v>
@@ -32288,7 +32288,7 @@
         </is>
       </c>
       <c r="AK152" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL152" t="n">
         <v>0.95</v>
@@ -32460,7 +32460,7 @@
         </is>
       </c>
       <c r="AK153" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL153" t="n">
         <v>0.99</v>
@@ -32632,7 +32632,7 @@
         </is>
       </c>
       <c r="AK154" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL154" t="n">
         <v>0.95</v>
@@ -32809,7 +32809,7 @@
         </is>
       </c>
       <c r="AK155" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL155" t="n">
         <v>0.97</v>
@@ -32992,7 +32992,7 @@
         </is>
       </c>
       <c r="AK156" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL156" t="n">
         <v>0.85</v>
@@ -33175,7 +33175,7 @@
         </is>
       </c>
       <c r="AK157" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL157" t="n">
         <v>0.9</v>
@@ -33358,7 +33358,7 @@
         </is>
       </c>
       <c r="AK158" t="n">
-        <v>340</v>
+        <v>70</v>
       </c>
       <c r="AL158" t="n">
         <v>0.36</v>
@@ -33530,7 +33530,7 @@
         </is>
       </c>
       <c r="AK159" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL159" t="n">
         <v>0.96</v>
@@ -33697,7 +33697,7 @@
         </is>
       </c>
       <c r="AK160" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL160" t="n">
         <v>0.95</v>
@@ -33880,7 +33880,7 @@
         </is>
       </c>
       <c r="AK161" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL161" t="n">
         <v>0.95</v>
@@ -34047,7 +34047,7 @@
         </is>
       </c>
       <c r="AK162" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL162" t="n">
         <v>0.98</v>
@@ -34214,7 +34214,7 @@
         </is>
       </c>
       <c r="AK163" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL163" t="n">
         <v>0.97</v>
@@ -34419,7 +34419,7 @@
         </is>
       </c>
       <c r="AK164" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL164" t="n">
         <v>0.93</v>
@@ -34596,7 +34596,7 @@
         </is>
       </c>
       <c r="AK165" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL165" t="n">
         <v>0.9399999999999999</v>
@@ -34788,7 +34788,7 @@
         </is>
       </c>
       <c r="AK166" t="n">
-        <v>1280</v>
+        <v>80</v>
       </c>
       <c r="AL166" t="n">
         <v>0.31</v>
@@ -34970,7 +34970,7 @@
         </is>
       </c>
       <c r="AK167" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL167" t="n">
         <v>0.93</v>
@@ -35147,7 +35147,7 @@
         </is>
       </c>
       <c r="AK168" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL168" t="n">
         <v>0.98</v>
@@ -35330,7 +35330,7 @@
         </is>
       </c>
       <c r="AK169" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL169" t="n">
         <v>0.95</v>
@@ -35512,7 +35512,7 @@
         </is>
       </c>
       <c r="AK170" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL170" t="n">
         <v>0.9399999999999999</v>
@@ -35679,7 +35679,7 @@
         </is>
       </c>
       <c r="AK171" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL171" t="n">
         <v>0.9399999999999999</v>
@@ -35856,7 +35856,7 @@
         </is>
       </c>
       <c r="AK172" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL172" t="n">
         <v>0.9399999999999999</v>
@@ -36023,7 +36023,7 @@
         </is>
       </c>
       <c r="AK173" t="n">
-        <v>4160</v>
+        <v>160</v>
       </c>
       <c r="AL173" t="n">
         <v>0.93</v>
@@ -36201,7 +36201,7 @@
         </is>
       </c>
       <c r="AK174" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL174" t="n">
         <v>0.91</v>
@@ -36383,7 +36383,7 @@
         </is>
       </c>
       <c r="AK175" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL175" t="n">
         <v>0.9399999999999999</v>
@@ -36550,7 +36550,7 @@
         </is>
       </c>
       <c r="AK176" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL176" t="n">
         <v>0.95</v>
@@ -36732,7 +36732,7 @@
         </is>
       </c>
       <c r="AK177" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL177" t="n">
         <v>0.83</v>
@@ -36914,7 +36914,7 @@
         </is>
       </c>
       <c r="AK178" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL178" t="n">
         <v>0.96</v>
@@ -37101,7 +37101,7 @@
         </is>
       </c>
       <c r="AK179" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL179" t="n">
         <v>0.86</v>
@@ -37289,7 +37289,7 @@
         </is>
       </c>
       <c r="AK180" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL180" t="n">
         <v>0.95</v>
@@ -37472,7 +37472,7 @@
         </is>
       </c>
       <c r="AK181" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL181" t="n">
         <v>0.95</v>
@@ -37659,7 +37659,7 @@
         </is>
       </c>
       <c r="AK182" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL182" t="n">
         <v>0.93</v>
@@ -37846,7 +37846,7 @@
         </is>
       </c>
       <c r="AK183" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL183" t="n">
         <v>0.97</v>
@@ -38028,7 +38028,7 @@
         </is>
       </c>
       <c r="AK184" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL184" t="n">
         <v>0.96</v>
@@ -38216,7 +38216,7 @@
         </is>
       </c>
       <c r="AK185" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL185" t="n">
         <v>0.92</v>
@@ -38404,7 +38404,7 @@
         </is>
       </c>
       <c r="AK186" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL186" t="n">
         <v>0.88</v>
@@ -38572,7 +38572,7 @@
         </is>
       </c>
       <c r="AK187" t="n">
-        <v>3360</v>
+        <v>160</v>
       </c>
       <c r="AL187" t="n">
         <v>0.93</v>
@@ -38764,7 +38764,7 @@
         </is>
       </c>
       <c r="AK188" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL188" t="n">
         <v>0.9</v>
@@ -38941,7 +38941,7 @@
         </is>
       </c>
       <c r="AK189" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL189" t="n">
         <v>0.96</v>
@@ -39123,7 +39123,7 @@
         </is>
       </c>
       <c r="AK190" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL190" t="n">
         <v>0.91</v>
@@ -39289,7 +39289,7 @@
         </is>
       </c>
       <c r="AK191" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL191" t="n">
         <v>0.24</v>
@@ -39467,7 +39467,7 @@
         </is>
       </c>
       <c r="AK192" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL192" t="n">
         <v>0.9399999999999999</v>
@@ -39650,7 +39650,7 @@
         </is>
       </c>
       <c r="AK193" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL193" t="n">
         <v>0.9399999999999999</v>
@@ -39817,7 +39817,7 @@
         </is>
       </c>
       <c r="AK194" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL194" t="n">
         <v>0.93</v>
@@ -39979,7 +39979,7 @@
         </is>
       </c>
       <c r="AK195" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL195" t="n">
         <v>0.3</v>
@@ -40141,7 +40141,7 @@
         </is>
       </c>
       <c r="AK196" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL196" t="n">
         <v>0.99</v>
@@ -40308,7 +40308,7 @@
         </is>
       </c>
       <c r="AK197" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL197" t="n">
         <v>0.95</v>
@@ -40465,7 +40465,7 @@
         </is>
       </c>
       <c r="AK198" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL198" t="n">
         <v>0.98</v>
@@ -40632,7 +40632,7 @@
         </is>
       </c>
       <c r="AK199" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL199" t="n">
         <v>0.99</v>
@@ -40815,7 +40815,7 @@
         </is>
       </c>
       <c r="AK200" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL200" t="n">
         <v>0.97</v>
@@ -40998,7 +40998,7 @@
         </is>
       </c>
       <c r="AK201" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL201" t="n">
         <v>0.95</v>
@@ -41181,7 +41181,7 @@
         </is>
       </c>
       <c r="AK202" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL202" t="n">
         <v>0.97</v>
@@ -41364,7 +41364,7 @@
         </is>
       </c>
       <c r="AK203" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL203" t="n">
         <v>0.97</v>
@@ -41542,7 +41542,7 @@
         </is>
       </c>
       <c r="AK204" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL204" t="n">
         <v>0.99</v>
@@ -41720,7 +41720,7 @@
         </is>
       </c>
       <c r="AK205" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL205" t="n">
         <v>0.99</v>
@@ -41895,7 +41895,7 @@
         </is>
       </c>
       <c r="AK206" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL206" t="n">
         <v>0.95</v>
@@ -42078,7 +42078,7 @@
         </is>
       </c>
       <c r="AK207" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL207" t="n">
         <v>0.9399999999999999</v>
@@ -42260,7 +42260,7 @@
         </is>
       </c>
       <c r="AK208" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL208" t="n">
         <v>0.9</v>
@@ -42442,7 +42442,7 @@
         </is>
       </c>
       <c r="AK209" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL209" t="n">
         <v>0.92</v>
@@ -42619,7 +42619,7 @@
         </is>
       </c>
       <c r="AK210" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL210" t="n">
         <v>0.84</v>
@@ -42801,7 +42801,7 @@
         </is>
       </c>
       <c r="AK211" t="n">
-        <v>1280</v>
+        <v>80</v>
       </c>
       <c r="AL211" t="n">
         <v>0.8100000000000001</v>
@@ -42993,7 +42993,7 @@
         </is>
       </c>
       <c r="AK212" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL212" t="n">
         <v>0.33</v>
@@ -43171,7 +43171,7 @@
         </is>
       </c>
       <c r="AK213" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL213" t="n">
         <v>0.93</v>
@@ -43359,7 +43359,7 @@
         </is>
       </c>
       <c r="AK214" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL214" t="n">
         <v>0.22</v>
@@ -43537,7 +43537,7 @@
         </is>
       </c>
       <c r="AK215" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL215" t="n">
         <v>0.97</v>
@@ -43721,7 +43721,7 @@
         </is>
       </c>
       <c r="AK216" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL216" t="n">
         <v>0.82</v>
@@ -43888,7 +43888,7 @@
         </is>
       </c>
       <c r="AK217" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL217" t="n">
         <v>0.98</v>
@@ -44056,7 +44056,7 @@
         </is>
       </c>
       <c r="AK218" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL218" t="n">
         <v>0.95</v>
@@ -44233,7 +44233,7 @@
         </is>
       </c>
       <c r="AK219" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL219" t="n">
         <v>0.97</v>
@@ -44400,7 +44400,7 @@
         </is>
       </c>
       <c r="AK220" t="n">
-        <v>1280</v>
+        <v>80</v>
       </c>
       <c r="AL220" t="n">
         <v>0.85</v>
@@ -44582,7 +44582,7 @@
         </is>
       </c>
       <c r="AK221" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL221" t="n">
         <v>0.99</v>
@@ -44759,7 +44759,7 @@
         </is>
       </c>
       <c r="AK222" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL222" t="n">
         <v>0.96</v>
@@ -44941,7 +44941,7 @@
         </is>
       </c>
       <c r="AK223" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL223" t="n">
         <v>0.96</v>
@@ -45118,7 +45118,7 @@
         </is>
       </c>
       <c r="AK224" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL224" t="n">
         <v>0.96</v>
@@ -45301,7 +45301,7 @@
         </is>
       </c>
       <c r="AK225" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL225" t="n">
         <v>0.97</v>
@@ -45473,7 +45473,7 @@
         </is>
       </c>
       <c r="AK226" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL226" t="n">
         <v>0.2</v>
@@ -45636,7 +45636,7 @@
         </is>
       </c>
       <c r="AK227" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL227" t="n">
         <v>0.9399999999999999</v>
@@ -45819,7 +45819,7 @@
         </is>
       </c>
       <c r="AK228" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL228" t="n">
         <v>0.91</v>
@@ -45987,7 +45987,7 @@
         </is>
       </c>
       <c r="AK229" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL229" t="n">
         <v>0.91</v>
@@ -46174,7 +46174,7 @@
         </is>
       </c>
       <c r="AK230" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL230" t="n">
         <v>0.9</v>
@@ -46357,7 +46357,7 @@
         </is>
       </c>
       <c r="AK231" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL231" t="n">
         <v>0.9399999999999999</v>
@@ -46539,7 +46539,7 @@
         </is>
       </c>
       <c r="AK232" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL232" t="n">
         <v>0.96</v>
@@ -46711,7 +46711,7 @@
         </is>
       </c>
       <c r="AK233" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL233" t="n">
         <v>0.96</v>
@@ -46893,7 +46893,7 @@
         </is>
       </c>
       <c r="AK234" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL234" t="n">
         <v>0.96</v>
@@ -47075,7 +47075,7 @@
         </is>
       </c>
       <c r="AK235" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL235" t="n">
         <v>0.96</v>
@@ -47257,7 +47257,7 @@
         </is>
       </c>
       <c r="AK236" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL236" t="n">
         <v>0.95</v>
@@ -47439,7 +47439,7 @@
         </is>
       </c>
       <c r="AK237" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL237" t="n">
         <v>0.9399999999999999</v>
@@ -47621,7 +47621,7 @@
         </is>
       </c>
       <c r="AK238" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL238" t="n">
         <v>0.97</v>
@@ -47803,7 +47803,7 @@
         </is>
       </c>
       <c r="AK239" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL239" t="n">
         <v>0.9399999999999999</v>
@@ -47980,7 +47980,7 @@
         </is>
       </c>
       <c r="AK240" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL240" t="n">
         <v>0.96</v>
@@ -48147,7 +48147,7 @@
         </is>
       </c>
       <c r="AK241" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL241" t="n">
         <v>0.85</v>
@@ -48324,7 +48324,7 @@
         </is>
       </c>
       <c r="AK242" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL242" t="n">
         <v>0.96</v>
@@ -48506,7 +48506,7 @@
         </is>
       </c>
       <c r="AK243" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL243" t="n">
         <v>0.96</v>
@@ -48688,7 +48688,7 @@
         </is>
       </c>
       <c r="AK244" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL244" t="n">
         <v>0.97</v>
@@ -48865,7 +48865,7 @@
         </is>
       </c>
       <c r="AK245" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL245" t="n">
         <v>0.96</v>
@@ -49047,7 +49047,7 @@
         </is>
       </c>
       <c r="AK246" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL246" t="n">
         <v>0.97</v>
@@ -49214,7 +49214,7 @@
         </is>
       </c>
       <c r="AK247" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL247" t="n">
         <v>0.96</v>
@@ -49376,7 +49376,7 @@
         </is>
       </c>
       <c r="AK248" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL248" t="n">
         <v>0.25</v>
@@ -49540,7 +49540,7 @@
         </is>
       </c>
       <c r="AK249" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL249" t="n">
         <v>0.93</v>
@@ -49708,7 +49708,7 @@
         </is>
       </c>
       <c r="AK250" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL250" t="n">
         <v>0.96</v>
@@ -49876,7 +49876,7 @@
         </is>
       </c>
       <c r="AK251" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL251" t="n">
         <v>0.92</v>
@@ -50073,7 +50073,7 @@
         </is>
       </c>
       <c r="AK252" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL252" t="n">
         <v>0.98</v>
@@ -50240,7 +50240,7 @@
         </is>
       </c>
       <c r="AK253" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL253" t="n">
         <v>0.93</v>
@@ -50427,7 +50427,7 @@
         </is>
       </c>
       <c r="AK254" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL254" t="n">
         <v>0.92</v>
@@ -50604,7 +50604,7 @@
         </is>
       </c>
       <c r="AK255" t="n">
-        <v>1280</v>
+        <v>80</v>
       </c>
       <c r="AL255" t="n">
         <v>0.19</v>
@@ -50781,7 +50781,7 @@
         </is>
       </c>
       <c r="AK256" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="AL256" t="n">
         <v>0.92</v>
@@ -50968,7 +50968,7 @@
         </is>
       </c>
       <c r="AK257" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="AL257" t="n">
         <v>0.92</v>
@@ -51155,7 +51155,7 @@
         </is>
       </c>
       <c r="AK258" t="n">
-        <v>850</v>
+        <v>100</v>
       </c>
       <c r="AL258" t="n">
         <v>0.95</v>
@@ -51342,7 +51342,7 @@
         </is>
       </c>
       <c r="AK259" t="n">
-        <v>850</v>
+        <v>100</v>
       </c>
       <c r="AL259" t="n">
         <v>0.96</v>
@@ -51530,7 +51530,7 @@
         </is>
       </c>
       <c r="AK260" t="n">
-        <v>850</v>
+        <v>100</v>
       </c>
       <c r="AL260" t="n">
         <v>0.93</v>
@@ -51717,7 +51717,7 @@
         </is>
       </c>
       <c r="AK261" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL261" t="n">
         <v>0.87</v>
@@ -51904,7 +51904,7 @@
         </is>
       </c>
       <c r="AK262" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL262" t="n">
         <v>0.91</v>
@@ -52081,7 +52081,7 @@
         </is>
       </c>
       <c r="AK263" t="n">
-        <v>4200</v>
+        <v>200</v>
       </c>
       <c r="AL263" t="n">
         <v>0.26</v>
@@ -52258,7 +52258,7 @@
         </is>
       </c>
       <c r="AK264" t="n">
-        <v>5200</v>
+        <v>200</v>
       </c>
       <c r="AL264" t="n">
         <v>0.9</v>
@@ -52445,7 +52445,7 @@
         </is>
       </c>
       <c r="AK265" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL265" t="n">
         <v>0.91</v>
@@ -52633,7 +52633,7 @@
         </is>
       </c>
       <c r="AK266" t="n">
-        <v>850</v>
+        <v>100</v>
       </c>
       <c r="AL266" t="n">
         <v>0.98</v>
@@ -52820,7 +52820,7 @@
         </is>
       </c>
       <c r="AK267" t="n">
-        <v>10400</v>
+        <v>400</v>
       </c>
       <c r="AL267" t="n">
         <v>0.91</v>
@@ -52992,7 +52992,7 @@
         </is>
       </c>
       <c r="AK268" t="n">
-        <v>4200</v>
+        <v>200</v>
       </c>
       <c r="AL268" t="n">
         <v>0.96</v>
@@ -53170,7 +53170,7 @@
         </is>
       </c>
       <c r="AK269" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL269" t="n">
         <v>0.93</v>
@@ -53348,7 +53348,7 @@
         </is>
       </c>
       <c r="AK270" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL270" t="n">
         <v>0.93</v>
@@ -53531,7 +53531,7 @@
         </is>
       </c>
       <c r="AK271" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL271" t="n">
         <v>0.92</v>
@@ -53714,7 +53714,7 @@
         </is>
       </c>
       <c r="AK272" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL272" t="n">
         <v>0.95</v>
@@ -53897,7 +53897,7 @@
         </is>
       </c>
       <c r="AK273" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL273" t="n">
         <v>0.93</v>
@@ -54075,7 +54075,7 @@
         </is>
       </c>
       <c r="AK274" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL274" t="n">
         <v>0.96</v>
@@ -54262,7 +54262,7 @@
         </is>
       </c>
       <c r="AK275" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="AL275" t="n">
         <v>0.92</v>
@@ -54445,7 +54445,7 @@
         </is>
       </c>
       <c r="AK276" t="n">
-        <v>4200</v>
+        <v>200</v>
       </c>
       <c r="AL276" t="n">
         <v>0.93</v>
@@ -54632,7 +54632,7 @@
         </is>
       </c>
       <c r="AK277" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL277" t="n">
         <v>0.86</v>
@@ -54809,7 +54809,7 @@
         </is>
       </c>
       <c r="AK278" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL278" t="n">
         <v>0.93</v>
@@ -54991,7 +54991,7 @@
         </is>
       </c>
       <c r="AK279" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL279" t="n">
         <v>0.86</v>
@@ -55169,7 +55169,7 @@
         </is>
       </c>
       <c r="AK280" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL280" t="n">
         <v>0.93</v>
@@ -55351,7 +55351,7 @@
         </is>
       </c>
       <c r="AK281" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL281" t="n">
         <v>0.86</v>
@@ -55533,7 +55533,7 @@
         </is>
       </c>
       <c r="AK282" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL282" t="n">
         <v>0.86</v>
@@ -55715,7 +55715,7 @@
         </is>
       </c>
       <c r="AK283" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL283" t="n">
         <v>0.86</v>
@@ -55887,7 +55887,7 @@
         </is>
       </c>
       <c r="AK284" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL284" t="n">
         <v>0.95</v>
@@ -56069,7 +56069,7 @@
         </is>
       </c>
       <c r="AK285" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL285" t="n">
         <v>0.86</v>
@@ -56251,7 +56251,7 @@
         </is>
       </c>
       <c r="AK286" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL286" t="n">
         <v>0.86</v>
@@ -56428,7 +56428,7 @@
         </is>
       </c>
       <c r="AK287" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL287" t="n">
         <v>0.93</v>
@@ -56602,7 +56602,7 @@
         </is>
       </c>
       <c r="AK288" t="n">
-        <v>850</v>
+        <v>100</v>
       </c>
       <c r="AL288" t="n">
         <v>0.92</v>
@@ -56784,7 +56784,7 @@
         </is>
       </c>
       <c r="AK289" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL289" t="n">
         <v>0.9399999999999999</v>
@@ -56961,7 +56961,7 @@
         </is>
       </c>
       <c r="AK290" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL290" t="n">
         <v>0.75</v>
@@ -57138,7 +57138,7 @@
         </is>
       </c>
       <c r="AK291" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL291" t="n">
         <v>0.95</v>
@@ -57316,7 +57316,7 @@
         </is>
       </c>
       <c r="AK292" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL292" t="n">
         <v>0.95</v>
@@ -57493,7 +57493,7 @@
         </is>
       </c>
       <c r="AK293" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL293" t="n">
         <v>0.95</v>
@@ -57655,7 +57655,7 @@
         </is>
       </c>
       <c r="AK294" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL294" t="n">
         <v>0.37</v>
@@ -57833,7 +57833,7 @@
         </is>
       </c>
       <c r="AK295" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL295" t="n">
         <v>0.9399999999999999</v>
@@ -58012,7 +58012,7 @@
         </is>
       </c>
       <c r="AK296" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL296" t="n">
         <v>0.9399999999999999</v>
@@ -58195,7 +58195,7 @@
         </is>
       </c>
       <c r="AK297" t="n">
-        <v>4160</v>
+        <v>160</v>
       </c>
       <c r="AL297" t="n">
         <v>0.91</v>
@@ -58373,7 +58373,7 @@
         </is>
       </c>
       <c r="AK298" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL298" t="n">
         <v>0.9399999999999999</v>
@@ -58535,7 +58535,7 @@
         </is>
       </c>
       <c r="AK299" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL299" t="n">
         <v>0.95</v>
@@ -58697,7 +58697,7 @@
         </is>
       </c>
       <c r="AK300" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL300" t="n">
         <v>0.9399999999999999</v>
@@ -58854,7 +58854,7 @@
         </is>
       </c>
       <c r="AK301" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL301" t="n">
         <v>0.9399999999999999</v>
@@ -59016,7 +59016,7 @@
         </is>
       </c>
       <c r="AK302" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL302" t="n">
         <v>0.9399999999999999</v>
@@ -59178,7 +59178,7 @@
         </is>
       </c>
       <c r="AK303" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL303" t="n">
         <v>0.78</v>
@@ -59335,7 +59335,7 @@
         </is>
       </c>
       <c r="AK304" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL304" t="n">
         <v>0.8100000000000001</v>
@@ -59492,7 +59492,7 @@
         </is>
       </c>
       <c r="AK305" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL305" t="n">
         <v>0.26</v>
@@ -59669,7 +59669,7 @@
         </is>
       </c>
       <c r="AK306" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL306" t="n">
         <v>0.93</v>
@@ -59846,7 +59846,7 @@
         </is>
       </c>
       <c r="AK307" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL307" t="n">
         <v>0.93</v>
@@ -60023,7 +60023,7 @@
         </is>
       </c>
       <c r="AK308" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL308" t="n">
         <v>0.93</v>
@@ -60200,7 +60200,7 @@
         </is>
       </c>
       <c r="AK309" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL309" t="n">
         <v>0.93</v>
@@ -60382,7 +60382,7 @@
         </is>
       </c>
       <c r="AK310" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL310" t="n">
         <v>0.87</v>
@@ -60569,7 +60569,7 @@
         </is>
       </c>
       <c r="AK311" t="n">
-        <v>340</v>
+        <v>70</v>
       </c>
       <c r="AL311" t="n">
         <v>0.91</v>
@@ -60736,7 +60736,7 @@
         </is>
       </c>
       <c r="AK312" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL312" t="n">
         <v>0.24</v>
@@ -60898,7 +60898,7 @@
         </is>
       </c>
       <c r="AK313" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL313" t="n">
         <v>0.27</v>
@@ -61070,7 +61070,7 @@
         </is>
       </c>
       <c r="AK314" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL314" t="n">
         <v>0.23</v>
@@ -61234,7 +61234,7 @@
         </is>
       </c>
       <c r="AK315" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL315" t="n">
         <v>0.87</v>
@@ -61417,7 +61417,7 @@
         </is>
       </c>
       <c r="AK316" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL316" t="n">
         <v>0.96</v>
@@ -61590,7 +61590,7 @@
         </is>
       </c>
       <c r="AK317" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL317" t="n">
         <v>0.82</v>
@@ -61768,7 +61768,7 @@
         </is>
       </c>
       <c r="AK318" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL318" t="n">
         <v>0.91</v>
@@ -61955,7 +61955,7 @@
         </is>
       </c>
       <c r="AK319" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL319" t="n">
         <v>0.93</v>
@@ -62142,7 +62142,7 @@
         </is>
       </c>
       <c r="AK320" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL320" t="n">
         <v>0.86</v>
@@ -62324,7 +62324,7 @@
         </is>
       </c>
       <c r="AK321" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="AL321" t="n">
         <v>0.86</v>
@@ -62501,7 +62501,7 @@
         </is>
       </c>
       <c r="AK322" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL322" t="n">
         <v>0.87</v>
@@ -62688,7 +62688,7 @@
         </is>
       </c>
       <c r="AK323" t="n">
-        <v>4160</v>
+        <v>160</v>
       </c>
       <c r="AL323" t="n">
         <v>0.8</v>
@@ -62870,7 +62870,7 @@
         </is>
       </c>
       <c r="AK324" t="n">
-        <v>4200</v>
+        <v>200</v>
       </c>
       <c r="AL324" t="n">
         <v>0.96</v>
@@ -63053,7 +63053,7 @@
         </is>
       </c>
       <c r="AK325" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL325" t="n">
         <v>0.92</v>
@@ -63215,7 +63215,7 @@
         </is>
       </c>
       <c r="AK326" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL326" t="n">
         <v>0.31</v>
@@ -63392,7 +63392,7 @@
         </is>
       </c>
       <c r="AK327" t="n">
-        <v>340</v>
+        <v>70</v>
       </c>
       <c r="AL327" t="n">
         <v>0.3</v>
@@ -63578,7 +63578,7 @@
         </is>
       </c>
       <c r="AK328" t="n">
-        <v>5200</v>
+        <v>200</v>
       </c>
       <c r="AL328" t="n">
         <v>0.93</v>
@@ -63756,7 +63756,7 @@
         </is>
       </c>
       <c r="AK329" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL329" t="n">
         <v>0.92</v>
@@ -63938,7 +63938,7 @@
         </is>
       </c>
       <c r="AK330" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL330" t="n">
         <v>0.98</v>
@@ -64128,7 +64128,7 @@
         </is>
       </c>
       <c r="AK331" t="n">
-        <v>680</v>
+        <v>140</v>
       </c>
       <c r="AL331" t="n">
         <v>0.95</v>
@@ -64312,7 +64312,7 @@
         </is>
       </c>
       <c r="AK332" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL332" t="n">
         <v>0.97</v>
@@ -64479,7 +64479,7 @@
         </is>
       </c>
       <c r="AK333" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL333" t="n">
         <v>0.29</v>
@@ -64636,7 +64636,7 @@
         </is>
       </c>
       <c r="AK334" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL334" t="n">
         <v>0.67</v>
@@ -64793,7 +64793,7 @@
         </is>
       </c>
       <c r="AK335" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL335" t="n">
         <v>0.65</v>
@@ -64965,7 +64965,7 @@
         </is>
       </c>
       <c r="AK336" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL336" t="n">
         <v>0.96</v>
@@ -65142,7 +65142,7 @@
         </is>
       </c>
       <c r="AK337" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL337" t="n">
         <v>0.93</v>
@@ -65319,7 +65319,7 @@
         </is>
       </c>
       <c r="AK338" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL338" t="n">
         <v>0.98</v>
@@ -65497,7 +65497,7 @@
         </is>
       </c>
       <c r="AK339" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL339" t="n">
         <v>0.95</v>
@@ -65669,7 +65669,7 @@
         </is>
       </c>
       <c r="AK340" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL340" t="n">
         <v>0.97</v>
@@ -65847,7 +65847,7 @@
         </is>
       </c>
       <c r="AK341" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL341" t="n">
         <v>0.96</v>
@@ -66036,7 +66036,7 @@
         </is>
       </c>
       <c r="AK342" t="n">
-        <v>850</v>
+        <v>100</v>
       </c>
       <c r="AL342" t="n">
         <v>0.9</v>
@@ -66226,7 +66226,7 @@
         </is>
       </c>
       <c r="AK343" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL343" t="n">
         <v>0.98</v>
@@ -66387,7 +66387,7 @@
         </is>
       </c>
       <c r="AK344" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL344" t="n">
         <v>0.17</v>
@@ -66566,7 +66566,7 @@
         </is>
       </c>
       <c r="AK345" t="n">
-        <v>850</v>
+        <v>100</v>
       </c>
       <c r="AL345" t="n">
         <v>0.16</v>
@@ -66739,7 +66739,7 @@
         </is>
       </c>
       <c r="AK346" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL346" t="n">
         <v>0.9</v>
@@ -66917,7 +66917,7 @@
         </is>
       </c>
       <c r="AK347" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL347" t="n">
         <v>0.9</v>
@@ -67079,7 +67079,7 @@
         </is>
       </c>
       <c r="AK348" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL348" t="n">
         <v>0.7</v>
@@ -67236,7 +67236,7 @@
         </is>
       </c>
       <c r="AK349" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL349" t="n">
         <v>0.26</v>
@@ -67393,7 +67393,7 @@
         </is>
       </c>
       <c r="AK350" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL350" t="n">
         <v>0.96</v>
@@ -67550,7 +67550,7 @@
         </is>
       </c>
       <c r="AK351" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL351" t="n">
         <v>0.96</v>
@@ -67707,7 +67707,7 @@
         </is>
       </c>
       <c r="AK352" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL352" t="n">
         <v>0.84</v>
@@ -67864,7 +67864,7 @@
         </is>
       </c>
       <c r="AK353" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL353" t="n">
         <v>0.21</v>
@@ -68041,7 +68041,7 @@
         </is>
       </c>
       <c r="AK354" t="n">
-        <v>4160</v>
+        <v>280</v>
       </c>
       <c r="AL354" t="n">
         <v>0.32</v>
@@ -68213,7 +68213,7 @@
         </is>
       </c>
       <c r="AK355" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL355" t="n">
         <v>0.24</v>
@@ -68386,7 +68386,7 @@
         </is>
       </c>
       <c r="AK356" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL356" t="n">
         <v>0.9399999999999999</v>
@@ -68554,7 +68554,7 @@
         </is>
       </c>
       <c r="AK357" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL357" t="n">
         <v>0.89</v>
@@ -68722,7 +68722,7 @@
         </is>
       </c>
       <c r="AK358" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL358" t="n">
         <v>0.96</v>
@@ -68900,7 +68900,7 @@
         </is>
       </c>
       <c r="AK359" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL359" t="n">
         <v>0.98</v>
@@ -69077,7 +69077,7 @@
         </is>
       </c>
       <c r="AK360" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL360" t="n">
         <v>0.91</v>
@@ -69243,7 +69243,7 @@
         </is>
       </c>
       <c r="AK361" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL361" t="n">
         <v>0.27</v>
@@ -69405,7 +69405,7 @@
         </is>
       </c>
       <c r="AK362" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL362" t="n">
         <v>0.97</v>
@@ -69573,7 +69573,7 @@
         </is>
       </c>
       <c r="AK363" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL363" t="n">
         <v>0.95</v>
@@ -69751,7 +69751,7 @@
         </is>
       </c>
       <c r="AK364" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL364" t="n">
         <v>0.96</v>
@@ -69938,7 +69938,7 @@
         </is>
       </c>
       <c r="AK365" t="n">
-        <v>35</v>
+        <v>17.5</v>
       </c>
       <c r="AL365" t="n">
         <v>0.96</v>
@@ -70125,7 +70125,7 @@
         </is>
       </c>
       <c r="AK366" t="n">
-        <v>35</v>
+        <v>17.5</v>
       </c>
       <c r="AL366" t="n">
         <v>0.95</v>
@@ -70312,7 +70312,7 @@
         </is>
       </c>
       <c r="AK367" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL367" t="n">
         <v>0.92</v>
@@ -70484,7 +70484,7 @@
         </is>
       </c>
       <c r="AK368" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL368" t="n">
         <v>0.86</v>
@@ -70646,7 +70646,7 @@
         </is>
       </c>
       <c r="AK369" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL369" t="n">
         <v>0.9399999999999999</v>
@@ -70816,7 +70816,7 @@
         </is>
       </c>
       <c r="AK370" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL370" t="n">
         <v>0.97</v>
@@ -70983,7 +70983,7 @@
         </is>
       </c>
       <c r="AK371" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL371" t="n">
         <v>0.93</v>
@@ -71151,7 +71151,7 @@
         </is>
       </c>
       <c r="AK372" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL372" t="n">
         <v>0.97</v>
@@ -71339,7 +71339,7 @@
         </is>
       </c>
       <c r="AK373" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="AL373" t="n">
         <v>0.9</v>
@@ -71509,7 +71509,7 @@
         </is>
       </c>
       <c r="AK374" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL374" t="n">
         <v>0.92</v>
@@ -71679,7 +71679,7 @@
         </is>
       </c>
       <c r="AK375" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL375" t="n">
         <v>0.9399999999999999</v>
@@ -71876,7 +71876,7 @@
         </is>
       </c>
       <c r="AK376" t="n">
-        <v>1700</v>
+        <v>200</v>
       </c>
       <c r="AL376" t="n">
         <v>0.9</v>
@@ -72048,7 +72048,7 @@
         </is>
       </c>
       <c r="AK377" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL377" t="n">
         <v>0.86</v>
@@ -72226,7 +72226,7 @@
         </is>
       </c>
       <c r="AK378" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="AL378" t="n">
         <v>0.91</v>
@@ -72394,7 +72394,7 @@
         </is>
       </c>
       <c r="AK379" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL379" t="n">
         <v>0.78</v>
@@ -72561,7 +72561,7 @@
         </is>
       </c>
       <c r="AK380" t="n">
-        <v>35</v>
+        <v>17.5</v>
       </c>
       <c r="AL380" t="n">
         <v>0.97</v>
@@ -72728,7 +72728,7 @@
         </is>
       </c>
       <c r="AK381" t="n">
-        <v>35</v>
+        <v>17.5</v>
       </c>
       <c r="AL381" t="n">
         <v>0.97</v>
@@ -72895,7 +72895,7 @@
         </is>
       </c>
       <c r="AK382" t="n">
-        <v>35</v>
+        <v>17.5</v>
       </c>
       <c r="AL382" t="n">
         <v>0.97</v>
@@ -73062,7 +73062,7 @@
         </is>
       </c>
       <c r="AK383" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL383" t="n">
         <v>0.89</v>
@@ -73229,7 +73229,7 @@
         </is>
       </c>
       <c r="AK384" t="n">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="AL384" t="n">
         <v>0.8</v>
@@ -73396,7 +73396,7 @@
         </is>
       </c>
       <c r="AK385" t="n">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="AL385" t="n">
         <v>0.93</v>
@@ -73564,7 +73564,7 @@
         </is>
       </c>
       <c r="AK386" t="n">
-        <v>1280</v>
+        <v>140</v>
       </c>
       <c r="AL386" t="n">
         <v>0.9</v>
@@ -73731,7 +73731,7 @@
         </is>
       </c>
       <c r="AK387" t="n">
-        <v>1680</v>
+        <v>80</v>
       </c>
       <c r="AL387" t="n">
         <v>0.9399999999999999</v>
@@ -73898,7 +73898,7 @@
         </is>
       </c>
       <c r="AK388" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL388" t="n">
         <v>0.99</v>
@@ -74056,7 +74056,7 @@
         </is>
       </c>
       <c r="AK389" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL389" t="n">
         <v>0.98</v>
@@ -74224,7 +74224,7 @@
         </is>
       </c>
       <c r="AK390" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL390" t="n">
         <v>0.9399999999999999</v>
@@ -74407,7 +74407,7 @@
         </is>
       </c>
       <c r="AK391" t="n">
-        <v>10400</v>
+        <v>400</v>
       </c>
       <c r="AL391" t="n">
         <v>0.9</v>
@@ -74570,7 +74570,7 @@
         </is>
       </c>
       <c r="AK392" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL392" t="n">
         <v>0.99</v>
@@ -74748,7 +74748,7 @@
         </is>
       </c>
       <c r="AK393" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL393" t="n">
         <v>0.92</v>
@@ -74915,7 +74915,7 @@
         </is>
       </c>
       <c r="AK394" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL394" t="n">
         <v>0.95</v>
@@ -75082,7 +75082,7 @@
         </is>
       </c>
       <c r="AK395" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="AL395" t="n">
         <v>0.96</v>
@@ -75269,7 +75269,7 @@
         </is>
       </c>
       <c r="AK396" t="n">
-        <v>1680</v>
+        <v>140</v>
       </c>
       <c r="AL396" t="n">
         <v>0.91</v>
@@ -75436,7 +75436,7 @@
         </is>
       </c>
       <c r="AK397" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="AL397" t="n">
         <v>0.9</v>

</xml_diff>

<commit_message>
Enhance escalation AI pipeline and pulse dashboard with robust error handling, improved visualizations, and extended analytics
Major updates across scoring, financial metrics, predictors, dashboard pages,
and chart generation. Adds resilience improvements to GPU utils, orchestrator,
and classification modules. Expands pulse dashboard with richer drill-down,
AI insights, and McKinsey-grade chart enhancements.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Strategic_Report.xlsx
+++ b/Strategic_Report.xlsx
@@ -2277,7 +2277,7 @@
     <row r="2" ht="22" customHeight="1">
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Executive Summary  |  February 10, 2026  |  396 Escalations Analyzed</t>
+          <t>Executive Summary  |  February 11, 2026  |  396 Escalations Analyzed</t>
         </is>
       </c>
     </row>
@@ -2350,7 +2350,7 @@
       <c r="G8" s="9" t="n"/>
       <c r="I8" s="12" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="J8" s="8" t="n"/>
@@ -2825,7 +2825,7 @@
     <row r="36" ht="18" customHeight="1">
       <c r="B36" s="36" t="inlineStr">
         <is>
-          <t>Generated by Escalation AI v2.2  |  February 10, 2026  |  Confidential - Internal Use Only</t>
+          <t>Generated by Escalation AI v2.2  |  February 11, 2026  |  Confidential - Internal Use Only</t>
         </is>
       </c>
     </row>
@@ -2907,7 +2907,7 @@
     <row r="3" ht="22" customHeight="1">
       <c r="B3" s="38" t="inlineStr">
         <is>
-          <t>Generated: February 10, 2026 at 11:46  •  Version: 2.2  •  AI Model: gpt-oss:20b</t>
+          <t>Generated: February 11, 2026 at 15:59  •  Version: 2.2  •  AI Model: gpt-oss:20b</t>
         </is>
       </c>
     </row>
@@ -2999,7 +2999,7 @@
     <row r="11" ht="22" customHeight="1">
       <c r="B11" s="53" t="inlineStr">
         <is>
-          <t>Avg Resolution: 8.4 days</t>
+          <t>Avg Resolution: 5.8 days</t>
         </is>
       </c>
       <c r="D11" s="53" t="inlineStr">
@@ -3617,12 +3617,12 @@
     <row r="50" ht="32" customHeight="1">
       <c r="B50" s="92" t="inlineStr">
         <is>
-          <t>🟡</t>
+          <t>🟢</t>
         </is>
       </c>
       <c r="C50" s="93" t="inlineStr">
         <is>
-          <t>Average predicted resolution: 8.4 days</t>
+          <t>Average predicted resolution: 5.8 days</t>
         </is>
       </c>
       <c r="D50" s="65" t="n"/>
@@ -3711,10 +3711,10 @@
       <c r="I56" s="65" t="n"/>
       <c r="J56" s="57" t="n"/>
     </row>
-    <row r="57" ht="64" customHeight="1">
+    <row r="57" ht="48" customHeight="1">
       <c r="B57" s="104" t="inlineStr">
         <is>
-          <t>Analysis reveals $36,368.50 in direct financial exposure driven primarily by Configuration &amp; Data Mismatch tickets, which account for 35 % of all costs. Immediate focus on a $1,300 investment in automated data validation can deliver $22,147 / yr in savings, yielding a 0.7‑month payback and a 1,603 % ROI.</t>
+          <t>Analysis reveals $42,908 in total financial exposure driven primarily by Configuration &amp; Data Mismatch tickets. Immediate focus on a $1,300 investment in configuration remediation can unlock $22,147 in annual savings, cutting exposure by 52 %.</t>
         </is>
       </c>
       <c r="C57" s="65" t="n"/>
@@ -3756,10 +3756,10 @@
       <c r="I59" s="65" t="n"/>
       <c r="J59" s="57" t="n"/>
     </row>
-    <row r="60" ht="32" customHeight="1">
+    <row r="60" ht="18" customHeight="1">
       <c r="B60" s="104" t="inlineStr">
         <is>
-          <t>- 396 tickets were analyzed over the reporting period, generating a weighted friction score of 26,340.</t>
+          <t>- 396 tickets were analyzed during the reporting period, covering all severity levels.</t>
         </is>
       </c>
       <c r="C60" s="65" t="n"/>
@@ -3771,10 +3771,10 @@
       <c r="I60" s="65" t="n"/>
       <c r="J60" s="57" t="n"/>
     </row>
-    <row r="61" ht="18" customHeight="1">
+    <row r="61" ht="32" customHeight="1">
       <c r="B61" s="104" t="inlineStr">
         <is>
-          <t>- Direct financial impact totals $36,368.50 with downstream revenue at risk of $90,921.25.</t>
+          <t>- Direct financial impact of $36,368.50 plus $1,468 in SLA penalties and $5,071.50 in customer‑impact costs equals $42,908 in exposure.</t>
         </is>
       </c>
       <c r="C61" s="65" t="n"/>
@@ -3789,7 +3789,7 @@
     <row r="62" ht="32" customHeight="1">
       <c r="B62" s="104" t="inlineStr">
         <is>
-          <t>- Severity split: Major 222 tickets ($22,592.50), Critical 40 tickets ($7,340.00), Minor 134 tickets ($6,436.00).</t>
+          <t>- Severity split: Major (222), Minor (134), Critical (40) – with Major tickets accounting for 62.1 % of costs.</t>
         </is>
       </c>
       <c r="C62" s="65" t="n"/>
@@ -3804,7 +3804,7 @@
     <row r="63" ht="32" customHeight="1">
       <c r="B63" s="104" t="inlineStr">
         <is>
-          <t>- Overall health: At Risk – high cost concentration (49 % of expenses from the top 20 % of tickets) and a low recurrence risk (0 %).</t>
+          <t>- Overall health: At Risk – high cost concentration (49 % of costs from the top 20 % of tickets) and a low confidence trend in the financial forecast.</t>
         </is>
       </c>
       <c r="C63" s="65" t="n"/>
@@ -3831,10 +3831,10 @@
       <c r="I64" s="65" t="n"/>
       <c r="J64" s="57" t="n"/>
     </row>
-    <row r="65" ht="18" customHeight="1">
-      <c r="B65" s="104" t="inlineStr">
-        <is>
-          <t>SECTION 3 - KEY FINDINGS (MECE Structure)</t>
+    <row r="65" ht="26" customHeight="1">
+      <c r="B65" s="103" t="inlineStr">
+        <is>
+          <t>SECTION 3 - KEY FINDINGS (MECE)</t>
         </is>
       </c>
       <c r="C65" s="65" t="n"/>
@@ -3861,10 +3861,10 @@
       <c r="I66" s="65" t="n"/>
       <c r="J66" s="57" t="n"/>
     </row>
-    <row r="67" ht="32" customHeight="1">
+    <row r="67" ht="18" customHeight="1">
       <c r="B67" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: Scheduling &amp; Planning tickets = 136 (34.3 % of volume), cost = $3,027.50 (8.3 % of total).</t>
+          <t>- *Data*: 136 Scheduling &amp; Planning tickets (34.3 %) costing $3,027.50 (avg $22.26).</t>
         </is>
       </c>
       <c r="C67" s="65" t="n"/>
@@ -3879,7 +3879,7 @@
     <row r="68" ht="32" customHeight="1">
       <c r="B68" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: Inefficient workflow and planning create a steady stream of low‑cost but high‑volume incidents, eroding productivity and inflating labor costs.</t>
+          <t>- *So What*: A workflow bottleneck is generating a high volume of low‑cost tickets that drain staffing resources and delay project timelines.</t>
         </is>
       </c>
       <c r="C68" s="65" t="n"/>
@@ -3909,7 +3909,7 @@
     <row r="70" ht="18" customHeight="1">
       <c r="B70" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: Documentation &amp; Reporting tickets = 49 (12.4 % of volume).</t>
+          <t>- *Data*: 27 Validation &amp; QA tickets (6.8 %) costing $3,892.00 (avg $144.15).</t>
         </is>
       </c>
       <c r="C70" s="65" t="n"/>
@@ -3924,7 +3924,7 @@
     <row r="71" ht="32" customHeight="1">
       <c r="B71" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: Incomplete or outdated documentation forces teams to spend extra time troubleshooting, increasing labor costs and delaying service delivery.</t>
+          <t>- *So What*: Inadequate training and documentation are causing repeated quality failures, inflating labor costs and eroding customer confidence.</t>
         </is>
       </c>
       <c r="C71" s="65" t="n"/>
@@ -3951,10 +3951,10 @@
       <c r="I72" s="65" t="n"/>
       <c r="J72" s="57" t="n"/>
     </row>
-    <row r="73" ht="32" customHeight="1">
+    <row r="73" ht="18" customHeight="1">
       <c r="B73" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: Configuration &amp; Data Mismatch tickets = 98 (24.7 % of volume), cost = $12,742.00 (35 % of total).</t>
+          <t>- *Data*: 98 Configuration &amp; Data Mismatch tickets (24.7 %) costing $12,742.00 (avg $130.02).</t>
         </is>
       </c>
       <c r="C73" s="65" t="n"/>
@@ -3969,7 +3969,7 @@
     <row r="74" ht="32" customHeight="1">
       <c r="B74" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: System misconfigurations and data inconsistencies are the largest cost driver, indicating a critical need for automated validation and tighter change control.</t>
+          <t>- *So What*: Technical misconfigurations are the single largest cost driver, indicating a critical need for automated checks and data governance.</t>
         </is>
       </c>
       <c r="C74" s="65" t="n"/>
@@ -3999,7 +3999,7 @@
     <row r="76" ht="18" customHeight="1">
       <c r="B76" s="104" t="inlineStr">
         <is>
-          <t>- *Data*: Critical tickets = 40 (10.1 % of volume), cost = $7,340.00 (20.2 % of total).</t>
+          <t>- *Data*: 40 Critical tickets (20.2 %) averaging $183.50 per ticket.</t>
         </is>
       </c>
       <c r="C76" s="65" t="n"/>
@@ -4014,7 +4014,7 @@
     <row r="77" ht="32" customHeight="1">
       <c r="B77" s="104" t="inlineStr">
         <is>
-          <t>- *So What*: High‑severity incidents expose coordination gaps between teams, leading to SLA penalties ($1,468.00) and customer impact costs ($5,071.50).</t>
+          <t>- *So What*: High‑severity incidents point to breakdowns in hand‑off and escalation protocols, risking SLA breaches and revenue loss.</t>
         </is>
       </c>
       <c r="C77" s="65" t="n"/>
@@ -4041,10 +4041,10 @@
       <c r="I78" s="65" t="n"/>
       <c r="J78" s="57" t="n"/>
     </row>
-    <row r="79" ht="18" customHeight="1">
-      <c r="B79" s="104" t="inlineStr">
-        <is>
-          <t>SECTION 4 - 80/20 ANALYSIS (Pareto Principle)</t>
+    <row r="79" ht="26" customHeight="1">
+      <c r="B79" s="103" t="inlineStr">
+        <is>
+          <t>SECTION 4 - 80/20 ANALYSIS</t>
         </is>
       </c>
       <c r="C79" s="65" t="n"/>
@@ -4056,10 +4056,10 @@
       <c r="I79" s="65" t="n"/>
       <c r="J79" s="57" t="n"/>
     </row>
-    <row r="80" ht="48" customHeight="1">
+    <row r="80" ht="18" customHeight="1">
       <c r="B80" s="104" t="inlineStr">
         <is>
-          <t>- Financial impact: Configuration &amp; Data Mismatch ($12,742), Site Readiness ($10,314), Validation &amp; QA ($3,892) – together 74 % of costs; adding Scheduling &amp; Planning ($3,027) pushes the total to 82 %.</t>
+          <t>- Financial Impact:</t>
         </is>
       </c>
       <c r="C80" s="65" t="n"/>
@@ -4071,10 +4071,10 @@
       <c r="I80" s="65" t="n"/>
       <c r="J80" s="57" t="n"/>
     </row>
-    <row r="81" ht="32" customHeight="1">
+    <row r="81" ht="18" customHeight="1">
       <c r="B81" s="104" t="inlineStr">
         <is>
-          <t>- Ticket volume: Scheduling &amp; Planning (34.3 %), Configuration &amp; Data Mismatch (24.7 %), Documentation &amp; Reporting (12.4 %) – 71 % of tickets; adding Site Readiness (9.8 %) reaches 81 %.</t>
+          <t>- Configuration &amp; Data Mismatch: $12,742 (35 %)</t>
         </is>
       </c>
       <c r="C81" s="65" t="n"/>
@@ -4086,10 +4086,10 @@
       <c r="I81" s="65" t="n"/>
       <c r="J81" s="57" t="n"/>
     </row>
-    <row r="82" ht="32" customHeight="1">
+    <row r="82" ht="18" customHeight="1">
       <c r="B82" s="104" t="inlineStr">
         <is>
-          <t>- Resource focus: Prioritize system‑level fixes for configuration mismatches, enhance site readiness processes, and streamline scheduling &amp; planning workflows to capture the greatest ROI.</t>
+          <t>- Site Readiness: $10,314 (28.4 %)</t>
         </is>
       </c>
       <c r="C82" s="65" t="n"/>
@@ -4104,7 +4104,7 @@
     <row r="83" ht="18" customHeight="1">
       <c r="B83" s="104" t="inlineStr">
         <is>
-          <t>---</t>
+          <t>- Validation &amp; QA: $3,892 (10.7 %)</t>
         </is>
       </c>
       <c r="C83" s="65" t="n"/>
@@ -4119,7 +4119,7 @@
     <row r="84" ht="18" customHeight="1">
       <c r="B84" s="104" t="inlineStr">
         <is>
-          <t>SECTION 5 - PRIORITIZED RECOMMENDATIONS (Impact‑Effort Matrix)</t>
+          <t>- Scheduling &amp; Planning: $3,027.50 (8.3 %)</t>
         </is>
       </c>
       <c r="C84" s="65" t="n"/>
@@ -4134,7 +4134,7 @@
     <row r="85" ht="18" customHeight="1">
       <c r="B85" s="104" t="inlineStr">
         <is>
-          <t>QUICK WINS (High Impact, Low Effort)</t>
+          <t>These four categories together account for ≈80 % of the $36,368.50 direct impact.</t>
         </is>
       </c>
       <c r="C85" s="65" t="n"/>
@@ -4146,10 +4146,10 @@
       <c r="I85" s="65" t="n"/>
       <c r="J85" s="57" t="n"/>
     </row>
-    <row r="86" ht="32" customHeight="1">
+    <row r="86" ht="18" customHeight="1">
       <c r="B86" s="104" t="inlineStr">
         <is>
-          <t>1. Automated Data Validation Tool – Deploy a lightweight script to flag configuration mismatches before deployment.</t>
+          <t>- Ticket Volume:</t>
         </is>
       </c>
       <c r="C86" s="65" t="n"/>
@@ -4164,7 +4164,7 @@
     <row r="87" ht="18" customHeight="1">
       <c r="B87" s="104" t="inlineStr">
         <is>
-          <t>- *Impact*: $22,147 / yr savings.</t>
+          <t>- Scheduling &amp; Planning: 136 tickets (34.3 %)</t>
         </is>
       </c>
       <c r="C87" s="65" t="n"/>
@@ -4179,7 +4179,7 @@
     <row r="88" ht="18" customHeight="1">
       <c r="B88" s="104" t="inlineStr">
         <is>
-          <t>- *Timeline*: Week 1–2.</t>
+          <t>- Configuration &amp; Data Mismatch: 98 tickets (24.7 %)</t>
         </is>
       </c>
       <c r="C88" s="65" t="n"/>
@@ -4194,7 +4194,7 @@
     <row r="89" ht="18" customHeight="1">
       <c r="B89" s="104" t="inlineStr">
         <is>
-          <t>MAJOR PROJECTS (High Impact, High Effort)</t>
+          <t>- Documentation &amp; Reporting: 49 tickets (12.4 %)</t>
         </is>
       </c>
       <c r="C89" s="65" t="n"/>
@@ -4206,10 +4206,10 @@
       <c r="I89" s="65" t="n"/>
       <c r="J89" s="57" t="n"/>
     </row>
-    <row r="90" ht="32" customHeight="1">
+    <row r="90" ht="18" customHeight="1">
       <c r="B90" s="104" t="inlineStr">
         <is>
-          <t>2. Site Readiness Enhancement Program – Standardize pre‑deployment checks and invest in readiness dashboards.</t>
+          <t>- Site Readiness: 39 tickets (9.8 %)</t>
         </is>
       </c>
       <c r="C90" s="65" t="n"/>
@@ -4224,7 +4224,7 @@
     <row r="91" ht="18" customHeight="1">
       <c r="B91" s="104" t="inlineStr">
         <is>
-          <t>- *Impact*: $17,927 / yr savings.</t>
+          <t>The top four categories represent ≈81 % of all tickets.</t>
         </is>
       </c>
       <c r="C91" s="65" t="n"/>
@@ -4236,10 +4236,10 @@
       <c r="I91" s="65" t="n"/>
       <c r="J91" s="57" t="n"/>
     </row>
-    <row r="92" ht="18" customHeight="1">
+    <row r="92" ht="32" customHeight="1">
       <c r="B92" s="104" t="inlineStr">
         <is>
-          <t>- *Timeline*: Month 2–3.</t>
+          <t>- Resource Focus: Prioritize remediation in Configuration &amp; Data Mismatch and Site Readiness for maximum ROI, while streamlining scheduling processes to reduce volume.</t>
         </is>
       </c>
       <c r="C92" s="65" t="n"/>
@@ -4254,7 +4254,7 @@
     <row r="93" ht="18" customHeight="1">
       <c r="B93" s="104" t="inlineStr">
         <is>
-          <t>FILL‑INS (Low Impact, Low Effort)</t>
+          <t>---</t>
         </is>
       </c>
       <c r="C93" s="65" t="n"/>
@@ -4266,10 +4266,10 @@
       <c r="I93" s="65" t="n"/>
       <c r="J93" s="57" t="n"/>
     </row>
-    <row r="94" ht="32" customHeight="1">
+    <row r="94" ht="18" customHeight="1">
       <c r="B94" s="104" t="inlineStr">
         <is>
-          <t>3. Scheduling &amp; Planning Process Redesign – Introduce a shared calendar and automated task assignment.</t>
+          <t>SECTION 5 - PRIORITIZED RECOMMENDATIONS (Impact‑Effort Matrix)</t>
         </is>
       </c>
       <c r="C94" s="65" t="n"/>
@@ -4284,7 +4284,7 @@
     <row r="95" ht="18" customHeight="1">
       <c r="B95" s="104" t="inlineStr">
         <is>
-          <t>- *Impact*: $600 / yr savings (estimated 20 % ticket reduction).</t>
+          <t>| Category | Action | Impact | Timeline |</t>
         </is>
       </c>
       <c r="C95" s="65" t="n"/>
@@ -4299,7 +4299,7 @@
     <row r="96" ht="18" customHeight="1">
       <c r="B96" s="104" t="inlineStr">
         <is>
-          <t>- *Timeline*: Ongoing.</t>
+          <t>|----------|--------|--------|----------|</t>
         </is>
       </c>
       <c r="C96" s="65" t="n"/>
@@ -4311,10 +4311,10 @@
       <c r="I96" s="65" t="n"/>
       <c r="J96" s="57" t="n"/>
     </row>
-    <row r="97" ht="18" customHeight="1">
+    <row r="97" ht="32" customHeight="1">
       <c r="B97" s="104" t="inlineStr">
         <is>
-          <t>4. Documentation &amp; Reporting Revamp – Consolidate SOPs into a single knowledge base.</t>
+          <t>| QUICK WINS | Deploy automated QA scripts to eliminate Validation &amp; QA tickets | $3,892 annual savings | Week 1‑2 |</t>
         </is>
       </c>
       <c r="C97" s="65" t="n"/>
@@ -4326,10 +4326,10 @@
       <c r="I97" s="65" t="n"/>
       <c r="J97" s="57" t="n"/>
     </row>
-    <row r="98" ht="18" customHeight="1">
+    <row r="98" ht="32" customHeight="1">
       <c r="B98" s="104" t="inlineStr">
         <is>
-          <t>- *Impact*: $300 / yr savings (estimated 10 % labor reduction).</t>
+          <t>| | Standardize scheduling templates to cut Scheduling &amp; Planning tickets | $454 (15 % volume reduction) | Week 1‑2 |</t>
         </is>
       </c>
       <c r="C98" s="65" t="n"/>
@@ -4341,10 +4341,10 @@
       <c r="I98" s="65" t="n"/>
       <c r="J98" s="57" t="n"/>
     </row>
-    <row r="99" ht="18" customHeight="1">
+    <row r="99" ht="32" customHeight="1">
       <c r="B99" s="104" t="inlineStr">
         <is>
-          <t>- *Timeline*: Ongoing.</t>
+          <t>| MAJOR PROJECTS | Configuration &amp; Data Mismatch remediation (invest $1,300) | $22,147 annual savings (ROI 1603 %) | Month 2‑3 |</t>
         </is>
       </c>
       <c r="C99" s="65" t="n"/>
@@ -4359,7 +4359,7 @@
     <row r="100" ht="18" customHeight="1">
       <c r="B100" s="104" t="inlineStr">
         <is>
-          <t>---</t>
+          <t>| | Site Readiness improvement (invest $2,645) | $17,927 annual savings (ROI 578 %) | Month 3‑4 |</t>
         </is>
       </c>
       <c r="C100" s="65" t="n"/>
@@ -4371,10 +4371,10 @@
       <c r="I100" s="65" t="n"/>
       <c r="J100" s="57" t="n"/>
     </row>
-    <row r="101" ht="18" customHeight="1">
+    <row r="101" ht="32" customHeight="1">
       <c r="B101" s="104" t="inlineStr">
         <is>
-          <t>SECTION 6 - RISK ASSESSMENT (RAG Status)</t>
+          <t>| FILL‑INS | Update documentation &amp; training for Reporting | Potential $1,000 savings (10 % ticket reduction) | Ongoing |</t>
         </is>
       </c>
       <c r="C101" s="65" t="n"/>
@@ -4389,7 +4389,7 @@
     <row r="102" ht="18" customHeight="1">
       <c r="B102" s="104" t="inlineStr">
         <is>
-          <t>- Financial Exposure: RED – $36,368.50 exposure vs $16,381.55 avoidance potential.</t>
+          <t>All actions are traceable to the financial impact data above.</t>
         </is>
       </c>
       <c r="C102" s="65" t="n"/>
@@ -4404,7 +4404,7 @@
     <row r="103" ht="18" customHeight="1">
       <c r="B103" s="104" t="inlineStr">
         <is>
-          <t>- Recurrence Risk: GREEN – 0 % recurrence risk exposure.</t>
+          <t>---</t>
         </is>
       </c>
       <c r="C103" s="65" t="n"/>
@@ -4419,7 +4419,7 @@
     <row r="104" ht="18" customHeight="1">
       <c r="B104" s="104" t="inlineStr">
         <is>
-          <t>- Process Maturity: AMBER – high volume of low‑cost tickets indicates process inefficiency.</t>
+          <t>SECTION 6 - RISK ASSESSMENT (RAG Status)</t>
         </is>
       </c>
       <c r="C104" s="65" t="n"/>
@@ -4431,10 +4431,10 @@
       <c r="I104" s="65" t="n"/>
       <c r="J104" s="57" t="n"/>
     </row>
-    <row r="105" ht="32" customHeight="1">
+    <row r="105" ht="18" customHeight="1">
       <c r="B105" s="104" t="inlineStr">
         <is>
-          <t>- Resolution Capability: AMBER – 49 % of costs concentrated in top 20 % of tickets, suggesting limited scalability of current support model.</t>
+          <t>| Area | Status | Reason |</t>
         </is>
       </c>
       <c r="C105" s="65" t="n"/>
@@ -4457,7 +4457,7 @@
     <row r="109">
       <c r="B109" s="106" t="inlineStr">
         <is>
-          <t>Report generated by Escalation AI v2.2 • February 10, 2026 at 11:46</t>
+          <t>Report generated by Escalation AI v2.2 • February 11, 2026 at 15:59</t>
         </is>
       </c>
     </row>
@@ -5057,7 +5057,7 @@
       </c>
       <c r="AR2" t="inlineStr">
         <is>
-          <t>11.7</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="AS2" t="n">
@@ -5263,7 +5263,7 @@
       </c>
       <c r="AR3" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="AS3" t="n">
@@ -5457,7 +5457,7 @@
       </c>
       <c r="AR4" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>2.3</t>
         </is>
       </c>
       <c r="AS4" t="n">
@@ -5640,7 +5640,7 @@
       </c>
       <c r="AR5" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS5" t="n">
@@ -5836,7 +5836,7 @@
       </c>
       <c r="AR6" t="inlineStr">
         <is>
-          <t>22.2</t>
+          <t>20.4</t>
         </is>
       </c>
       <c r="AS6" t="n">
@@ -6034,7 +6034,7 @@
       </c>
       <c r="AR7" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>19.8</t>
         </is>
       </c>
       <c r="AS7" t="n">
@@ -6236,7 +6236,7 @@
       </c>
       <c r="AR8" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>19.8</t>
         </is>
       </c>
       <c r="AS8" t="n">
@@ -6426,7 +6426,7 @@
       </c>
       <c r="AR9" t="inlineStr">
         <is>
-          <t>5.5</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS9" t="n">
@@ -6814,7 +6814,7 @@
       </c>
       <c r="AR11" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>2.3</t>
         </is>
       </c>
       <c r="AS11" t="n">
@@ -6999,7 +6999,7 @@
       </c>
       <c r="AR12" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS12" t="n">
@@ -7201,7 +7201,7 @@
       </c>
       <c r="AR13" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS13" t="n">
@@ -7399,11 +7399,11 @@
       </c>
       <c r="AR14" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS14" t="n">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15">
@@ -7593,11 +7593,11 @@
       </c>
       <c r="AR15" t="inlineStr">
         <is>
-          <t>4.4</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS15" t="n">
-        <v>0.32</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16">
@@ -7789,7 +7789,7 @@
       </c>
       <c r="AR16" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS16" t="n">
@@ -7970,11 +7970,11 @@
       </c>
       <c r="AR17" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS17" t="n">
-        <v>0.47</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="18">
@@ -8160,7 +8160,7 @@
       </c>
       <c r="AR18" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS18" t="n">
@@ -8350,7 +8350,7 @@
       </c>
       <c r="AR19" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS19" t="n">
@@ -8533,7 +8533,7 @@
       </c>
       <c r="AR20" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS20" t="n">
@@ -8719,7 +8719,7 @@
       </c>
       <c r="AR21" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS21" t="n">
@@ -8913,11 +8913,11 @@
       </c>
       <c r="AR22" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS22" t="n">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="23">
@@ -9111,7 +9111,7 @@
       </c>
       <c r="AR23" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="AS23" t="n">
@@ -9314,7 +9314,7 @@
       </c>
       <c r="AR24" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="AS24" t="n">
@@ -9508,7 +9508,7 @@
       </c>
       <c r="AR25" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS25" t="n">
@@ -9693,7 +9693,7 @@
       </c>
       <c r="AR26" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="AS26" t="n">
@@ -9891,7 +9891,7 @@
       </c>
       <c r="AR27" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS27" t="n">
@@ -10084,7 +10084,7 @@
       </c>
       <c r="AR28" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="AS28" t="n">
@@ -10275,7 +10275,7 @@
       </c>
       <c r="AR29" t="inlineStr">
         <is>
-          <t>8.9</t>
+          <t>8.6</t>
         </is>
       </c>
       <c r="AS29" t="n">
@@ -10479,7 +10479,7 @@
       </c>
       <c r="AR30" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="AS30" t="n">
@@ -10677,7 +10677,7 @@
       </c>
       <c r="AR31" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS31" t="n">
@@ -10875,11 +10875,11 @@
       </c>
       <c r="AR32" t="inlineStr">
         <is>
-          <t>16.7</t>
+          <t>20.7</t>
         </is>
       </c>
       <c r="AS32" t="n">
-        <v>0.62</v>
+        <v>0.6899999999999999</v>
       </c>
     </row>
     <row r="33">
@@ -11073,7 +11073,7 @@
       </c>
       <c r="AR33" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>7.9</t>
         </is>
       </c>
       <c r="AS33" t="n">
@@ -11271,7 +11271,7 @@
       </c>
       <c r="AR34" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS34" t="n">
@@ -11472,11 +11472,11 @@
       </c>
       <c r="AR35" t="inlineStr">
         <is>
-          <t>10.8</t>
+          <t>12.6</t>
         </is>
       </c>
       <c r="AS35" t="n">
-        <v>0.43</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="36">
@@ -11658,7 +11658,7 @@
       </c>
       <c r="AR36" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>7.7</t>
         </is>
       </c>
       <c r="AS36" t="n">
@@ -11852,11 +11852,11 @@
       </c>
       <c r="AR37" t="inlineStr">
         <is>
-          <t>12.8</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS37" t="n">
-        <v>0.51</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="38">
@@ -12016,7 +12016,7 @@
         <v>105</v>
       </c>
       <c r="AL38" t="n">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="AM38" t="inlineStr">
         <is>
@@ -12045,11 +12045,11 @@
       </c>
       <c r="AR38" t="inlineStr">
         <is>
-          <t>7.5</t>
+          <t>6.4</t>
         </is>
       </c>
       <c r="AS38" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="39">
@@ -12242,7 +12242,7 @@
       </c>
       <c r="AR39" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS39" t="n">
@@ -12443,7 +12443,7 @@
       </c>
       <c r="AR40" t="inlineStr">
         <is>
-          <t>7.2</t>
+          <t>7.8</t>
         </is>
       </c>
       <c r="AS40" t="n">
@@ -12636,11 +12636,11 @@
       </c>
       <c r="AR41" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS41" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="42">
@@ -12830,7 +12830,7 @@
       </c>
       <c r="AR42" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>7.9</t>
         </is>
       </c>
       <c r="AS42" t="n">
@@ -13024,11 +13024,11 @@
       </c>
       <c r="AR43" t="inlineStr">
         <is>
-          <t>13.0</t>
+          <t>9.4</t>
         </is>
       </c>
       <c r="AS43" t="n">
-        <v>0.52</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="44">
@@ -13214,7 +13214,7 @@
       </c>
       <c r="AR44" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>7.5</t>
         </is>
       </c>
       <c r="AS44" t="n">
@@ -13409,11 +13409,11 @@
       </c>
       <c r="AR45" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS45" t="n">
-        <v>0.41</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="46">
@@ -13610,11 +13610,11 @@
       </c>
       <c r="AR46" t="inlineStr">
         <is>
-          <t>5.8</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS46" t="n">
-        <v>0.46</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="47">
@@ -13800,7 +13800,7 @@
       </c>
       <c r="AR47" t="inlineStr">
         <is>
-          <t>13.5</t>
+          <t>12.8</t>
         </is>
       </c>
       <c r="AS47" t="n">
@@ -14199,7 +14199,7 @@
       </c>
       <c r="AR49" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS49" t="n">
@@ -14399,11 +14399,11 @@
       </c>
       <c r="AR50" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS50" t="n">
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="51">
@@ -14602,11 +14602,11 @@
       </c>
       <c r="AR51" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>8.9</t>
         </is>
       </c>
       <c r="AS51" t="n">
-        <v>0.64</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="52">
@@ -14787,11 +14787,11 @@
       </c>
       <c r="AR52" t="inlineStr">
         <is>
-          <t>9.5</t>
+          <t>6.8</t>
         </is>
       </c>
       <c r="AS52" t="n">
-        <v>0.65</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="53">
@@ -14981,7 +14981,7 @@
       </c>
       <c r="AR53" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>2.1</t>
         </is>
       </c>
       <c r="AS53" t="n">
@@ -15179,7 +15179,7 @@
       </c>
       <c r="AR54" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="AS54" t="n">
@@ -15364,11 +15364,11 @@
       </c>
       <c r="AR55" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>6.9</t>
         </is>
       </c>
       <c r="AS55" t="n">
-        <v>0.52</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="56">
@@ -15558,11 +15558,11 @@
       </c>
       <c r="AR56" t="inlineStr">
         <is>
-          <t>10.4</t>
+          <t>12.1</t>
         </is>
       </c>
       <c r="AS56" t="n">
-        <v>0.41</v>
+        <v>0.49</v>
       </c>
     </row>
     <row r="57">
@@ -15736,11 +15736,11 @@
       </c>
       <c r="AR57" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="AS57" t="n">
-        <v>0.52</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="58">
@@ -15905,7 +15905,7 @@
       </c>
       <c r="AR58" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS58" t="n">
@@ -16086,7 +16086,7 @@
       </c>
       <c r="AR59" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS59" t="n">
@@ -16256,11 +16256,11 @@
       </c>
       <c r="AR60" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="AS60" t="n">
-        <v>0.52</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="61">
@@ -16441,7 +16441,7 @@
       </c>
       <c r="AR61" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS61" t="n">
@@ -16626,7 +16626,7 @@
       </c>
       <c r="AR62" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS62" t="n">
@@ -16812,7 +16812,7 @@
       </c>
       <c r="AR63" t="inlineStr">
         <is>
-          <t>14.4</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS63" t="n">
@@ -16997,7 +16997,7 @@
       </c>
       <c r="AR64" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS64" t="n">
@@ -17174,7 +17174,7 @@
       </c>
       <c r="AR65" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS65" t="n">
@@ -17363,7 +17363,7 @@
       </c>
       <c r="AR66" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS66" t="n">
@@ -17549,11 +17549,11 @@
       </c>
       <c r="AR67" t="inlineStr">
         <is>
-          <t>5.8</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS67" t="n">
-        <v>0.46</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="68">
@@ -17738,7 +17738,7 @@
       </c>
       <c r="AR68" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS68" t="n">
@@ -17923,7 +17923,7 @@
       </c>
       <c r="AR69" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS69" t="n">
@@ -18114,7 +18114,7 @@
       </c>
       <c r="AR70" t="inlineStr">
         <is>
-          <t>10.3</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS70" t="n">
@@ -18299,7 +18299,7 @@
       </c>
       <c r="AR71" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS71" t="n">
@@ -18480,7 +18480,7 @@
       </c>
       <c r="AR72" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS72" t="n">
@@ -18673,7 +18673,7 @@
       </c>
       <c r="AR73" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>7.9</t>
         </is>
       </c>
       <c r="AS73" t="n">
@@ -18850,7 +18850,7 @@
       </c>
       <c r="AR74" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS74" t="n">
@@ -19027,7 +19027,7 @@
       </c>
       <c r="AR75" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS75" t="n">
@@ -19212,7 +19212,7 @@
       </c>
       <c r="AR76" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS76" t="n">
@@ -19397,7 +19397,7 @@
       </c>
       <c r="AR77" t="inlineStr">
         <is>
-          <t>16.4</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS77" t="n">
@@ -19578,11 +19578,11 @@
       </c>
       <c r="AR78" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS78" t="n">
-        <v>0.52</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="79">
@@ -19759,7 +19759,7 @@
       </c>
       <c r="AR79" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS79" t="n">
@@ -19948,7 +19948,7 @@
       </c>
       <c r="AR80" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="AS80" t="n">
@@ -20133,7 +20133,7 @@
       </c>
       <c r="AR81" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS81" t="n">
@@ -20318,7 +20318,7 @@
       </c>
       <c r="AR82" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS82" t="n">
@@ -20503,7 +20503,7 @@
       </c>
       <c r="AR83" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS83" t="n">
@@ -20689,7 +20689,7 @@
       </c>
       <c r="AR84" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS84" t="n">
@@ -20874,7 +20874,7 @@
       </c>
       <c r="AR85" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS85" t="n">
@@ -21059,7 +21059,7 @@
       </c>
       <c r="AR86" t="inlineStr">
         <is>
-          <t>17.5</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS86" t="n">
@@ -21249,7 +21249,7 @@
       </c>
       <c r="AR87" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS87" t="n">
@@ -21434,7 +21434,7 @@
       </c>
       <c r="AR88" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS88" t="n">
@@ -21619,7 +21619,7 @@
       </c>
       <c r="AR89" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS89" t="n">
@@ -21809,7 +21809,7 @@
       </c>
       <c r="AR90" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS90" t="n">
@@ -21995,11 +21995,11 @@
       </c>
       <c r="AR91" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS91" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="92">
@@ -22184,7 +22184,7 @@
       </c>
       <c r="AR92" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS92" t="n">
@@ -22361,7 +22361,7 @@
       </c>
       <c r="AR93" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS93" t="n">
@@ -22551,11 +22551,11 @@
       </c>
       <c r="AR94" t="inlineStr">
         <is>
-          <t>16.9</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS94" t="n">
-        <v>0.72</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="95">
@@ -22736,7 +22736,7 @@
       </c>
       <c r="AR95" t="inlineStr">
         <is>
-          <t>16.4</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS95" t="n">
@@ -22926,7 +22926,7 @@
       </c>
       <c r="AR96" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS96" t="n">
@@ -23104,11 +23104,11 @@
       </c>
       <c r="AR97" t="inlineStr">
         <is>
-          <t>17.0</t>
+          <t>19.8</t>
         </is>
       </c>
       <c r="AS97" t="n">
-        <v>0.3</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="98">
@@ -23283,11 +23283,11 @@
       </c>
       <c r="AR98" t="inlineStr">
         <is>
-          <t>17.9</t>
+          <t>19.8</t>
         </is>
       </c>
       <c r="AS98" t="n">
-        <v>0.31</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="99">
@@ -23453,7 +23453,7 @@
       </c>
       <c r="AR99" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>19.8</t>
         </is>
       </c>
       <c r="AS99" t="n">
@@ -23632,7 +23632,7 @@
       </c>
       <c r="AR100" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>19.0</t>
         </is>
       </c>
       <c r="AS100" t="n">
@@ -23817,7 +23817,7 @@
       </c>
       <c r="AR101" t="inlineStr">
         <is>
-          <t>11.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS101" t="n">
@@ -24008,7 +24008,7 @@
       </c>
       <c r="AR102" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS102" t="n">
@@ -24181,11 +24181,11 @@
       </c>
       <c r="AR103" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>10.2</t>
         </is>
       </c>
       <c r="AS103" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="104">
@@ -24358,7 +24358,7 @@
       </c>
       <c r="AR104" t="inlineStr">
         <is>
-          <t>8.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS104" t="n">
@@ -24538,11 +24538,11 @@
       </c>
       <c r="AR105" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS105" t="n">
-        <v>0.6</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="106">
@@ -24944,11 +24944,11 @@
       </c>
       <c r="AR107" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="AS107" t="n">
-        <v>0.49</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="108">
@@ -25132,7 +25132,7 @@
       </c>
       <c r="AR108" t="inlineStr">
         <is>
-          <t>8.9</t>
+          <t>9.1</t>
         </is>
       </c>
       <c r="AS108" t="n">
@@ -25321,7 +25321,7 @@
       </c>
       <c r="AR109" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS109" t="n">
@@ -25513,7 +25513,7 @@
       </c>
       <c r="AR110" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS110" t="n">
@@ -25698,7 +25698,7 @@
       </c>
       <c r="AR111" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS111" t="n">
@@ -26074,7 +26074,7 @@
       </c>
       <c r="AR113" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS113" t="n">
@@ -26259,7 +26259,7 @@
       </c>
       <c r="AR114" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS114" t="n">
@@ -26444,7 +26444,7 @@
       </c>
       <c r="AR115" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS115" t="n">
@@ -26633,11 +26633,11 @@
       </c>
       <c r="AR116" t="inlineStr">
         <is>
-          <t>13.4</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS116" t="n">
-        <v>0.65</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="117">
@@ -26818,7 +26818,7 @@
       </c>
       <c r="AR117" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS117" t="n">
@@ -26995,7 +26995,7 @@
       </c>
       <c r="AR118" t="inlineStr">
         <is>
-          <t>16.4</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS118" t="n">
@@ -27180,7 +27180,7 @@
       </c>
       <c r="AR119" t="inlineStr">
         <is>
-          <t>11.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS119" t="n">
@@ -27359,7 +27359,7 @@
       </c>
       <c r="AR120" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS120" t="n">
@@ -27540,11 +27540,11 @@
       </c>
       <c r="AR121" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS121" t="n">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="122">
@@ -27730,7 +27730,7 @@
       </c>
       <c r="AR122" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS122" t="n">
@@ -27919,7 +27919,7 @@
       </c>
       <c r="AR123" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS123" t="n">
@@ -28104,7 +28104,7 @@
       </c>
       <c r="AR124" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS124" t="n">
@@ -28289,7 +28289,7 @@
       </c>
       <c r="AR125" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS125" t="n">
@@ -28479,7 +28479,7 @@
       </c>
       <c r="AR126" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS126" t="n">
@@ -28664,7 +28664,7 @@
       </c>
       <c r="AR127" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS127" t="n">
@@ -28857,11 +28857,11 @@
       </c>
       <c r="AR128" t="inlineStr">
         <is>
-          <t>11.7</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS128" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="129">
@@ -29058,11 +29058,11 @@
       </c>
       <c r="AR129" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS129" t="n">
-        <v>0.36</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="130">
@@ -29251,11 +29251,11 @@
       </c>
       <c r="AR130" t="inlineStr">
         <is>
-          <t>13.5</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS130" t="n">
-        <v>0.65</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="131">
@@ -29449,7 +29449,7 @@
       </c>
       <c r="AR131" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS131" t="n">
@@ -29647,7 +29647,7 @@
       </c>
       <c r="AR132" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>9.2</t>
         </is>
       </c>
       <c r="AS132" t="n">
@@ -29836,7 +29836,7 @@
       </c>
       <c r="AR133" t="inlineStr">
         <is>
-          <t>17.1</t>
+          <t>17.8</t>
         </is>
       </c>
       <c r="AS133" t="n">
@@ -30021,7 +30021,7 @@
       </c>
       <c r="AR134" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS134" t="n">
@@ -30206,7 +30206,7 @@
       </c>
       <c r="AR135" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS135" t="n">
@@ -30395,7 +30395,7 @@
       </c>
       <c r="AR136" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS136" t="n">
@@ -30580,7 +30580,7 @@
       </c>
       <c r="AR137" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS137" t="n">
@@ -30753,11 +30753,11 @@
       </c>
       <c r="AR138" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS138" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="139">
@@ -30930,11 +30930,11 @@
       </c>
       <c r="AR139" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS139" t="n">
-        <v>0.5</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="140">
@@ -31123,7 +31123,7 @@
       </c>
       <c r="AR140" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.5</t>
         </is>
       </c>
       <c r="AS140" t="n">
@@ -31309,7 +31309,7 @@
       </c>
       <c r="AR141" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS141" t="n">
@@ -31495,7 +31495,7 @@
       </c>
       <c r="AR142" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS142" t="n">
@@ -31681,7 +31681,7 @@
       </c>
       <c r="AR143" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS143" t="n">
@@ -31871,7 +31871,7 @@
       </c>
       <c r="AR144" t="inlineStr">
         <is>
-          <t>11.8</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS144" t="n">
@@ -32052,7 +32052,7 @@
       </c>
       <c r="AR145" t="inlineStr">
         <is>
-          <t>13.5</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS145" t="n">
@@ -32241,7 +32241,7 @@
       </c>
       <c r="AR146" t="inlineStr">
         <is>
-          <t>16.2</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS146" t="n">
@@ -32426,7 +32426,7 @@
       </c>
       <c r="AR147" t="inlineStr">
         <is>
-          <t>13.5</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS147" t="n">
@@ -32611,7 +32611,7 @@
       </c>
       <c r="AR148" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS148" t="n">
@@ -32796,7 +32796,7 @@
       </c>
       <c r="AR149" t="inlineStr">
         <is>
-          <t>13.5</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS149" t="n">
@@ -32990,11 +32990,11 @@
       </c>
       <c r="AR150" t="inlineStr">
         <is>
-          <t>10.3</t>
+          <t>9.9</t>
         </is>
       </c>
       <c r="AS150" t="n">
-        <v>0.55</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="151">
@@ -33187,7 +33187,7 @@
       </c>
       <c r="AR151" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS151" t="n">
@@ -33372,7 +33372,7 @@
       </c>
       <c r="AR152" t="inlineStr">
         <is>
-          <t>13.5</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS152" t="n">
@@ -33549,11 +33549,11 @@
       </c>
       <c r="AR153" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS153" t="n">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="154">
@@ -33734,7 +33734,7 @@
       </c>
       <c r="AR154" t="inlineStr">
         <is>
-          <t>13.5</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS154" t="n">
@@ -33890,7 +33890,7 @@
         <v>87.5</v>
       </c>
       <c r="AL155" t="n">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="AM155" t="inlineStr">
         <is>
@@ -33919,7 +33919,7 @@
       </c>
       <c r="AR155" t="inlineStr">
         <is>
-          <t>13.5</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS155" t="n">
@@ -34109,7 +34109,7 @@
       </c>
       <c r="AR156" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="AS156" t="n">
@@ -34299,7 +34299,7 @@
       </c>
       <c r="AR157" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS157" t="n">
@@ -34460,7 +34460,7 @@
         <v>70</v>
       </c>
       <c r="AL158" t="n">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
       <c r="AM158" t="inlineStr">
         <is>
@@ -34485,7 +34485,7 @@
       </c>
       <c r="AR158" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>12.1</t>
         </is>
       </c>
       <c r="AS158" t="n">
@@ -34670,7 +34670,7 @@
       </c>
       <c r="AR159" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS159" t="n">
@@ -34847,7 +34847,7 @@
       </c>
       <c r="AR160" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>2.9</t>
         </is>
       </c>
       <c r="AS160" t="n">
@@ -35037,7 +35037,7 @@
       </c>
       <c r="AR161" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS161" t="n">
@@ -35214,7 +35214,7 @@
       </c>
       <c r="AR162" t="inlineStr">
         <is>
-          <t>13.3</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS162" t="n">
@@ -35391,7 +35391,7 @@
       </c>
       <c r="AR163" t="inlineStr">
         <is>
-          <t>13.3</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS163" t="n">
@@ -35570,7 +35570,7 @@
         <v>7</v>
       </c>
       <c r="AL164" t="n">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="AM164" t="inlineStr">
         <is>
@@ -35599,7 +35599,7 @@
       </c>
       <c r="AR164" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS164" t="n">
@@ -35784,7 +35784,7 @@
       </c>
       <c r="AR165" t="inlineStr">
         <is>
-          <t>13.3</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS165" t="n">
@@ -35981,11 +35981,11 @@
       </c>
       <c r="AR166" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="AS166" t="n">
-        <v>0.3</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="167">
@@ -36170,7 +36170,7 @@
       </c>
       <c r="AR167" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS167" t="n">
@@ -36355,7 +36355,7 @@
       </c>
       <c r="AR168" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS168" t="n">
@@ -36545,11 +36545,11 @@
       </c>
       <c r="AR169" t="inlineStr">
         <is>
-          <t>16.7</t>
+          <t>18.4</t>
         </is>
       </c>
       <c r="AS169" t="n">
-        <v>0.71</v>
+        <v>0.74</v>
       </c>
     </row>
     <row r="170">
@@ -36734,7 +36734,7 @@
       </c>
       <c r="AR170" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS170" t="n">
@@ -36911,11 +36911,11 @@
       </c>
       <c r="AR171" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS171" t="n">
-        <v>0.59</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="172">
@@ -37096,7 +37096,7 @@
       </c>
       <c r="AR172" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS172" t="n">
@@ -37273,11 +37273,11 @@
       </c>
       <c r="AR173" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS173" t="n">
-        <v>0.43</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="174">
@@ -37459,11 +37459,11 @@
       </c>
       <c r="AR174" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS174" t="n">
-        <v>0.37</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="175">
@@ -37648,7 +37648,7 @@
       </c>
       <c r="AR175" t="inlineStr">
         <is>
-          <t>13.5</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS175" t="n">
@@ -37825,7 +37825,7 @@
       </c>
       <c r="AR176" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS176" t="n">
@@ -38014,7 +38014,7 @@
       </c>
       <c r="AR177" t="inlineStr">
         <is>
-          <t>5.6</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS177" t="n">
@@ -38203,7 +38203,7 @@
       </c>
       <c r="AR178" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS178" t="n">
@@ -38396,7 +38396,7 @@
       </c>
       <c r="AR179" t="inlineStr">
         <is>
-          <t>8.6</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS179" t="n">
@@ -38590,7 +38590,7 @@
       </c>
       <c r="AR180" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS180" t="n">
@@ -38780,7 +38780,7 @@
       </c>
       <c r="AR181" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS181" t="n">
@@ -39166,11 +39166,11 @@
       </c>
       <c r="AR183" t="inlineStr">
         <is>
-          <t>17.9</t>
+          <t>19.8</t>
         </is>
       </c>
       <c r="AS183" t="n">
-        <v>0.31</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="184">
@@ -39549,7 +39549,7 @@
       </c>
       <c r="AR185" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS185" t="n">
@@ -39743,7 +39743,7 @@
       </c>
       <c r="AR186" t="inlineStr">
         <is>
-          <t>3.9</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS186" t="n">
@@ -39921,7 +39921,7 @@
       </c>
       <c r="AR187" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS187" t="n">
@@ -40118,7 +40118,7 @@
       </c>
       <c r="AR188" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="AS188" t="n">
@@ -40303,11 +40303,11 @@
       </c>
       <c r="AR189" t="inlineStr">
         <is>
-          <t>9.2</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS189" t="n">
-        <v>0.64</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="190">
@@ -40492,7 +40492,7 @@
       </c>
       <c r="AR190" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS190" t="n">
@@ -40665,11 +40665,11 @@
       </c>
       <c r="AR191" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.4</t>
         </is>
       </c>
       <c r="AS191" t="n">
-        <v>0.45</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="192">
@@ -40855,11 +40855,11 @@
       </c>
       <c r="AR192" t="inlineStr">
         <is>
-          <t>17.5</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS192" t="n">
-        <v>0.72</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="193">
@@ -41045,7 +41045,7 @@
       </c>
       <c r="AR193" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS193" t="n">
@@ -41193,7 +41193,7 @@
         <v>140</v>
       </c>
       <c r="AL194" t="n">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
       <c r="AM194" t="inlineStr">
         <is>
@@ -41218,11 +41218,11 @@
       </c>
       <c r="AR194" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS194" t="n">
-        <v>0.57</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="195">
@@ -41391,11 +41391,11 @@
       </c>
       <c r="AR195" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS195" t="n">
-        <v>0.57</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="196">
@@ -41568,11 +41568,11 @@
       </c>
       <c r="AR196" t="inlineStr">
         <is>
-          <t>8.9</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="AS196" t="n">
-        <v>0.63</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="197">
@@ -41741,11 +41741,11 @@
       </c>
       <c r="AR197" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="AS197" t="n">
-        <v>0.57</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="198">
@@ -41914,11 +41914,11 @@
       </c>
       <c r="AR198" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS198" t="n">
-        <v>0.39</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="199">
@@ -42091,11 +42091,11 @@
       </c>
       <c r="AR199" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS199" t="n">
-        <v>0.6</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="200">
@@ -42281,7 +42281,7 @@
       </c>
       <c r="AR200" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS200" t="n">
@@ -42471,7 +42471,7 @@
       </c>
       <c r="AR201" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS201" t="n">
@@ -42661,7 +42661,7 @@
       </c>
       <c r="AR202" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS202" t="n">
@@ -42851,7 +42851,7 @@
       </c>
       <c r="AR203" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS203" t="n">
@@ -43037,7 +43037,7 @@
       </c>
       <c r="AR204" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS204" t="n">
@@ -43223,7 +43223,7 @@
       </c>
       <c r="AR205" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS205" t="n">
@@ -43407,7 +43407,7 @@
       </c>
       <c r="AR206" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>5.2</t>
         </is>
       </c>
       <c r="AS206" t="n">
@@ -43597,7 +43597,7 @@
       </c>
       <c r="AR207" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS207" t="n">
@@ -43786,11 +43786,11 @@
       </c>
       <c r="AR208" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS208" t="n">
-        <v>0.67</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="209">
@@ -43946,7 +43946,7 @@
         <v>80</v>
       </c>
       <c r="AL209" t="n">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="AM209" t="inlineStr">
         <is>
@@ -43975,11 +43975,11 @@
       </c>
       <c r="AR209" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS209" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="210">
@@ -44160,11 +44160,11 @@
       </c>
       <c r="AR210" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="AS210" t="n">
-        <v>0.59</v>
+        <v>0.5600000000000001</v>
       </c>
     </row>
     <row r="211">
@@ -44349,11 +44349,11 @@
       </c>
       <c r="AR211" t="inlineStr">
         <is>
-          <t>9.9</t>
+          <t>8.3</t>
         </is>
       </c>
       <c r="AS211" t="n">
-        <v>0.39</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="212">
@@ -44542,11 +44542,11 @@
       </c>
       <c r="AR212" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS212" t="n">
-        <v>0.48</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="213">
@@ -44732,7 +44732,7 @@
       </c>
       <c r="AR213" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS213" t="n">
@@ -44897,7 +44897,7 @@
         <v>200</v>
       </c>
       <c r="AL214" t="n">
-        <v>0.27</v>
+        <v>0.28</v>
       </c>
       <c r="AM214" t="inlineStr">
         <is>
@@ -44922,7 +44922,7 @@
       </c>
       <c r="AR214" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS214" t="n">
@@ -45112,7 +45112,7 @@
       </c>
       <c r="AR215" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS215" t="n">
@@ -45303,7 +45303,7 @@
       </c>
       <c r="AR216" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS216" t="n">
@@ -45480,11 +45480,11 @@
       </c>
       <c r="AR217" t="inlineStr">
         <is>
-          <t>8.6</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS217" t="n">
-        <v>0.61</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="218">
@@ -45658,7 +45658,7 @@
       </c>
       <c r="AR218" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS218" t="n">
@@ -45843,11 +45843,11 @@
       </c>
       <c r="AR219" t="inlineStr">
         <is>
-          <t>12.3</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS219" t="n">
-        <v>0.62</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="220">
@@ -46020,11 +46020,11 @@
       </c>
       <c r="AR220" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>11.5</t>
         </is>
       </c>
       <c r="AS220" t="n">
-        <v>0.3</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="221">
@@ -46180,7 +46180,7 @@
         <v>7</v>
       </c>
       <c r="AL221" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="AM221" t="inlineStr">
         <is>
@@ -46365,7 +46365,7 @@
         <v>7</v>
       </c>
       <c r="AL222" t="n">
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="AM222" t="inlineStr">
         <is>
@@ -46394,7 +46394,7 @@
       </c>
       <c r="AR222" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS222" t="n">
@@ -46583,7 +46583,7 @@
       </c>
       <c r="AR223" t="inlineStr">
         <is>
-          <t>8.5</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS223" t="n">
@@ -46768,7 +46768,7 @@
       </c>
       <c r="AR224" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS224" t="n">
@@ -46958,7 +46958,7 @@
       </c>
       <c r="AR225" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS225" t="n">
@@ -47135,7 +47135,7 @@
       </c>
       <c r="AR226" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS226" t="n">
@@ -47313,11 +47313,11 @@
       </c>
       <c r="AR227" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS227" t="n">
-        <v>0.44</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="228">
@@ -47503,7 +47503,7 @@
       </c>
       <c r="AR228" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS228" t="n">
@@ -47681,11 +47681,11 @@
       </c>
       <c r="AR229" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS229" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="230">
@@ -47874,11 +47874,11 @@
       </c>
       <c r="AR230" t="inlineStr">
         <is>
-          <t>7.0</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS230" t="n">
-        <v>0.54</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="231">
@@ -48064,7 +48064,7 @@
       </c>
       <c r="AR231" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS231" t="n">
@@ -48253,7 +48253,7 @@
       </c>
       <c r="AR232" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS232" t="n">
@@ -48434,7 +48434,7 @@
       </c>
       <c r="AR233" t="inlineStr">
         <is>
-          <t>11.7</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS233" t="n">
@@ -48623,7 +48623,7 @@
       </c>
       <c r="AR234" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS234" t="n">
@@ -48812,7 +48812,7 @@
       </c>
       <c r="AR235" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS235" t="n">
@@ -49001,7 +49001,7 @@
       </c>
       <c r="AR236" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS236" t="n">
@@ -49190,7 +49190,7 @@
       </c>
       <c r="AR237" t="inlineStr">
         <is>
-          <t>6.2</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS237" t="n">
@@ -49379,7 +49379,7 @@
       </c>
       <c r="AR238" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS238" t="n">
@@ -49568,11 +49568,11 @@
       </c>
       <c r="AR239" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS239" t="n">
-        <v>0.39</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="240">
@@ -49753,7 +49753,7 @@
       </c>
       <c r="AR240" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS240" t="n">
@@ -49930,11 +49930,11 @@
       </c>
       <c r="AR241" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS241" t="n">
-        <v>0.39</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="242">
@@ -50115,7 +50115,7 @@
       </c>
       <c r="AR242" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS242" t="n">
@@ -50304,7 +50304,7 @@
       </c>
       <c r="AR243" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS243" t="n">
@@ -50493,7 +50493,7 @@
       </c>
       <c r="AR244" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS244" t="n">
@@ -50678,11 +50678,11 @@
       </c>
       <c r="AR245" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS245" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="246">
@@ -50867,7 +50867,7 @@
       </c>
       <c r="AR246" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS246" t="n">
@@ -51044,7 +51044,7 @@
       </c>
       <c r="AR247" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS247" t="n">
@@ -51213,11 +51213,11 @@
       </c>
       <c r="AR248" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS248" t="n">
-        <v>0.36</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="249">
@@ -51392,11 +51392,11 @@
       </c>
       <c r="AR249" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS249" t="n">
-        <v>0.44</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="250">
@@ -51570,11 +51570,11 @@
       </c>
       <c r="AR250" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS250" t="n">
-        <v>0.44</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="251">
@@ -51748,11 +51748,11 @@
       </c>
       <c r="AR251" t="inlineStr">
         <is>
-          <t>6.0</t>
+          <t>4.0</t>
         </is>
       </c>
       <c r="AS251" t="n">
-        <v>0.47</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="252">
@@ -51949,7 +51949,7 @@
       </c>
       <c r="AR252" t="inlineStr">
         <is>
-          <t>2.6</t>
+          <t>2.7</t>
         </is>
       </c>
       <c r="AS252" t="n">
@@ -52126,11 +52126,11 @@
       </c>
       <c r="AR253" t="inlineStr">
         <is>
-          <t>7.8</t>
+          <t>4.1</t>
         </is>
       </c>
       <c r="AS253" t="n">
-        <v>0.58</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="254">
@@ -52315,7 +52315,7 @@
       </c>
       <c r="AR254" t="inlineStr">
         <is>
-          <t>9.5</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS254" t="n">
@@ -52500,7 +52500,7 @@
       </c>
       <c r="AR255" t="inlineStr">
         <is>
-          <t>12.2</t>
+          <t>12.1</t>
         </is>
       </c>
       <c r="AS255" t="n">
@@ -52689,7 +52689,7 @@
       </c>
       <c r="AR256" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS256" t="n">
@@ -52882,7 +52882,7 @@
       </c>
       <c r="AR257" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS257" t="n">
@@ -53075,7 +53075,7 @@
       </c>
       <c r="AR258" t="inlineStr">
         <is>
-          <t>12.2</t>
+          <t>9.8</t>
         </is>
       </c>
       <c r="AS258" t="n">
@@ -53268,7 +53268,7 @@
       </c>
       <c r="AR259" t="inlineStr">
         <is>
-          <t>17.5</t>
+          <t>20.7</t>
         </is>
       </c>
       <c r="AS259" t="n">
@@ -53462,7 +53462,7 @@
       </c>
       <c r="AR260" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>12.0</t>
         </is>
       </c>
       <c r="AS260" t="n">
@@ -53655,7 +53655,7 @@
       </c>
       <c r="AR261" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS261" t="n">
@@ -53844,7 +53844,7 @@
       </c>
       <c r="AR262" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS262" t="n">
@@ -54029,11 +54029,11 @@
       </c>
       <c r="AR263" t="inlineStr">
         <is>
-          <t>4.5</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS263" t="n">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="264">
@@ -54218,11 +54218,11 @@
       </c>
       <c r="AR264" t="inlineStr">
         <is>
-          <t>16.4</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS264" t="n">
-        <v>0.71</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="265">
@@ -54411,7 +54411,7 @@
       </c>
       <c r="AR265" t="inlineStr">
         <is>
-          <t>8.3</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS265" t="n">
@@ -54605,7 +54605,7 @@
       </c>
       <c r="AR266" t="inlineStr">
         <is>
-          <t>16.4</t>
+          <t>20.7</t>
         </is>
       </c>
       <c r="AS266" t="n">
@@ -54794,11 +54794,11 @@
       </c>
       <c r="AR267" t="inlineStr">
         <is>
-          <t>8.4</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS267" t="n">
-        <v>0.46</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="268">
@@ -54979,11 +54979,11 @@
       </c>
       <c r="AR268" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>7.6</t>
         </is>
       </c>
       <c r="AS268" t="n">
-        <v>0.59</v>
+        <v>0.57</v>
       </c>
     </row>
     <row r="269">
@@ -55165,11 +55165,11 @@
       </c>
       <c r="AR269" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS269" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="270">
@@ -55351,11 +55351,11 @@
       </c>
       <c r="AR270" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS270" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="271">
@@ -55541,7 +55541,7 @@
       </c>
       <c r="AR271" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS271" t="n">
@@ -55731,7 +55731,7 @@
       </c>
       <c r="AR272" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS272" t="n">
@@ -55921,7 +55921,7 @@
       </c>
       <c r="AR273" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS273" t="n">
@@ -56107,11 +56107,11 @@
       </c>
       <c r="AR274" t="inlineStr">
         <is>
-          <t>7.6</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS274" t="n">
-        <v>0.57</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="275">
@@ -56300,7 +56300,7 @@
       </c>
       <c r="AR275" t="inlineStr">
         <is>
-          <t>10.9</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS275" t="n">
@@ -56490,11 +56490,11 @@
       </c>
       <c r="AR276" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS276" t="n">
-        <v>0.35</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="277">
@@ -56679,7 +56679,7 @@
       </c>
       <c r="AR277" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS277" t="n">
@@ -56864,7 +56864,7 @@
       </c>
       <c r="AR278" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS278" t="n">
@@ -57053,7 +57053,7 @@
       </c>
       <c r="AR279" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS279" t="n">
@@ -57239,7 +57239,7 @@
       </c>
       <c r="AR280" t="inlineStr">
         <is>
-          <t>7.3</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS280" t="n">
@@ -57428,7 +57428,7 @@
       </c>
       <c r="AR281" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS281" t="n">
@@ -57617,7 +57617,7 @@
       </c>
       <c r="AR282" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS282" t="n">
@@ -57806,7 +57806,7 @@
       </c>
       <c r="AR283" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS283" t="n">
@@ -57991,7 +57991,7 @@
       </c>
       <c r="AR284" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>3.4</t>
         </is>
       </c>
       <c r="AS284" t="n">
@@ -58176,7 +58176,7 @@
       </c>
       <c r="AR285" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS285" t="n">
@@ -58365,7 +58365,7 @@
       </c>
       <c r="AR286" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS286" t="n">
@@ -58550,7 +58550,7 @@
       </c>
       <c r="AR287" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS287" t="n">
@@ -58737,7 +58737,7 @@
       </c>
       <c r="AR288" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>19.8</t>
         </is>
       </c>
       <c r="AS288" t="n">
@@ -58926,11 +58926,11 @@
       </c>
       <c r="AR289" t="inlineStr">
         <is>
-          <t>14.4</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS289" t="n">
-        <v>0.67</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="290">
@@ -59111,11 +59111,11 @@
       </c>
       <c r="AR290" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>4.9</t>
         </is>
       </c>
       <c r="AS290" t="n">
-        <v>0.4</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="291">
@@ -59296,7 +59296,7 @@
       </c>
       <c r="AR291" t="inlineStr">
         <is>
-          <t>13.2</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS291" t="n">
@@ -59482,11 +59482,11 @@
       </c>
       <c r="AR292" t="inlineStr">
         <is>
-          <t>12.2</t>
+          <t>10.3</t>
         </is>
       </c>
       <c r="AS292" t="n">
-        <v>0.62</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="293">
@@ -59667,11 +59667,11 @@
       </c>
       <c r="AR293" t="inlineStr">
         <is>
-          <t>14.4</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS293" t="n">
-        <v>0.67</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="294">
@@ -59836,7 +59836,7 @@
       </c>
       <c r="AR294" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS294" t="n">
@@ -60026,7 +60026,7 @@
       </c>
       <c r="AR295" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS295" t="n">
@@ -60213,11 +60213,11 @@
       </c>
       <c r="AR296" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>5.5</t>
         </is>
       </c>
       <c r="AS296" t="n">
-        <v>0.51</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="297">
@@ -60403,11 +60403,11 @@
       </c>
       <c r="AR297" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS297" t="n">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="298">
@@ -60589,11 +60589,11 @@
       </c>
       <c r="AR298" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS298" t="n">
-        <v>0.52</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="299">
@@ -60762,11 +60762,11 @@
       </c>
       <c r="AR299" t="inlineStr">
         <is>
-          <t>5.9</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS299" t="n">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="300">
@@ -60931,7 +60931,7 @@
       </c>
       <c r="AR300" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS300" t="n">
@@ -61104,11 +61104,11 @@
       </c>
       <c r="AR301" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS301" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="302">
@@ -61277,11 +61277,11 @@
       </c>
       <c r="AR302" t="inlineStr">
         <is>
-          <t>7.4</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS302" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="303">
@@ -61446,11 +61446,11 @@
       </c>
       <c r="AR303" t="inlineStr">
         <is>
-          <t>10.6</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="AS303" t="n">
-        <v>0.68</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="304">
@@ -61615,11 +61615,11 @@
       </c>
       <c r="AR304" t="inlineStr">
         <is>
-          <t>9.5</t>
+          <t>8.5</t>
         </is>
       </c>
       <c r="AS304" t="n">
-        <v>0.65</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="305">
@@ -61784,11 +61784,11 @@
       </c>
       <c r="AR305" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS305" t="n">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="306">
@@ -61969,7 +61969,7 @@
       </c>
       <c r="AR306" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS306" t="n">
@@ -62154,7 +62154,7 @@
       </c>
       <c r="AR307" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS307" t="n">
@@ -62339,7 +62339,7 @@
       </c>
       <c r="AR308" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS308" t="n">
@@ -62524,7 +62524,7 @@
       </c>
       <c r="AR309" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS309" t="n">
@@ -62717,7 +62717,7 @@
       </c>
       <c r="AR310" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>6.7</t>
         </is>
       </c>
       <c r="AS310" t="n">
@@ -62910,7 +62910,7 @@
       </c>
       <c r="AR311" t="inlineStr">
         <is>
-          <t>12.1</t>
+          <t>9.7</t>
         </is>
       </c>
       <c r="AS311" t="n">
@@ -63083,11 +63083,11 @@
       </c>
       <c r="AR312" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS312" t="n">
-        <v>0.34</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="313">
@@ -63260,7 +63260,7 @@
       </c>
       <c r="AR313" t="inlineStr">
         <is>
-          <t>3.5</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS313" t="n">
@@ -63437,11 +63437,11 @@
       </c>
       <c r="AR314" t="inlineStr">
         <is>
-          <t>10.8</t>
+          <t>12.6</t>
         </is>
       </c>
       <c r="AS314" t="n">
-        <v>0.43</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="315">
@@ -63616,11 +63616,11 @@
       </c>
       <c r="AR315" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS315" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="316">
@@ -63806,7 +63806,7 @@
       </c>
       <c r="AR316" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>2.8</t>
         </is>
       </c>
       <c r="AS316" t="n">
@@ -63984,7 +63984,7 @@
       </c>
       <c r="AR317" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS317" t="n">
@@ -64174,11 +64174,11 @@
       </c>
       <c r="AR318" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS318" t="n">
-        <v>0.51</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="319">
@@ -64367,7 +64367,7 @@
       </c>
       <c r="AR319" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS319" t="n">
@@ -64556,7 +64556,7 @@
       </c>
       <c r="AR320" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS320" t="n">
@@ -64749,7 +64749,7 @@
       </c>
       <c r="AR321" t="inlineStr">
         <is>
-          <t>9.9</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS321" t="n">
@@ -64934,7 +64934,7 @@
       </c>
       <c r="AR322" t="inlineStr">
         <is>
-          <t>3.7</t>
+          <t>3.6</t>
         </is>
       </c>
       <c r="AS322" t="n">
@@ -65127,7 +65127,7 @@
       </c>
       <c r="AR323" t="inlineStr">
         <is>
-          <t>5.8</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS323" t="n">
@@ -65316,11 +65316,11 @@
       </c>
       <c r="AR324" t="inlineStr">
         <is>
-          <t>7.9</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS324" t="n">
-        <v>0.58</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="325">
@@ -65506,7 +65506,7 @@
       </c>
       <c r="AR325" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.3</t>
         </is>
       </c>
       <c r="AS325" t="n">
@@ -65675,11 +65675,11 @@
       </c>
       <c r="AR326" t="inlineStr">
         <is>
-          <t>10.9</t>
+          <t>12.6</t>
         </is>
       </c>
       <c r="AS326" t="n">
-        <v>0.43</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="327">
@@ -65864,7 +65864,7 @@
       </c>
       <c r="AR327" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>9.2</t>
         </is>
       </c>
       <c r="AS327" t="n">
@@ -66057,7 +66057,7 @@
       </c>
       <c r="AR328" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS328" t="n">
@@ -66214,7 +66214,7 @@
         <v>175</v>
       </c>
       <c r="AL329" t="n">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
       <c r="AM329" t="inlineStr">
         <is>
@@ -66243,11 +66243,11 @@
       </c>
       <c r="AR329" t="inlineStr">
         <is>
-          <t>5.3</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS329" t="n">
-        <v>0.41</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="330">
@@ -66403,7 +66403,7 @@
         <v>7</v>
       </c>
       <c r="AL330" t="n">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="AM330" t="inlineStr">
         <is>
@@ -66432,7 +66432,7 @@
       </c>
       <c r="AR330" t="inlineStr">
         <is>
-          <t>8.6</t>
+          <t>3.2</t>
         </is>
       </c>
       <c r="AS330" t="n">
@@ -66628,11 +66628,11 @@
       </c>
       <c r="AR331" t="inlineStr">
         <is>
-          <t>4.3</t>
+          <t>18.1</t>
         </is>
       </c>
       <c r="AS331" t="n">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="332">
@@ -66819,7 +66819,7 @@
       </c>
       <c r="AR332" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS332" t="n">
@@ -66992,11 +66992,11 @@
       </c>
       <c r="AR333" t="inlineStr">
         <is>
-          <t>11.7</t>
+          <t>8.7</t>
         </is>
       </c>
       <c r="AS333" t="n">
-        <v>0.47</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="334">
@@ -67161,7 +67161,7 @@
       </c>
       <c r="AR334" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS334" t="n">
@@ -67330,7 +67330,7 @@
       </c>
       <c r="AR335" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>6.3</t>
         </is>
       </c>
       <c r="AS335" t="n">
@@ -67515,7 +67515,7 @@
       </c>
       <c r="AR336" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS336" t="n">
@@ -67700,11 +67700,11 @@
       </c>
       <c r="AR337" t="inlineStr">
         <is>
-          <t>8.6</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS337" t="n">
-        <v>0.61</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="338">
@@ -67856,7 +67856,7 @@
         <v>7</v>
       </c>
       <c r="AL338" t="n">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="AM338" t="inlineStr">
         <is>
@@ -67885,7 +67885,7 @@
       </c>
       <c r="AR338" t="inlineStr">
         <is>
-          <t>16.6</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS338" t="n">
@@ -68071,11 +68071,11 @@
       </c>
       <c r="AR339" t="inlineStr">
         <is>
-          <t>7.7</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS339" t="n">
-        <v>0.57</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="340">
@@ -68252,7 +68252,7 @@
       </c>
       <c r="AR340" t="inlineStr">
         <is>
-          <t>2.4</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS340" t="n">
@@ -68438,7 +68438,7 @@
       </c>
       <c r="AR341" t="inlineStr">
         <is>
-          <t>3.4</t>
+          <t>3.3</t>
         </is>
       </c>
       <c r="AS341" t="n">
@@ -68633,7 +68633,7 @@
       </c>
       <c r="AR342" t="inlineStr">
         <is>
-          <t>5.4</t>
+          <t>9.0</t>
         </is>
       </c>
       <c r="AS342" t="n">
@@ -68829,11 +68829,11 @@
       </c>
       <c r="AR343" t="inlineStr">
         <is>
-          <t>8.8</t>
+          <t>10.5</t>
         </is>
       </c>
       <c r="AS343" t="n">
-        <v>0.32</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="344">
@@ -68998,11 +68998,11 @@
       </c>
       <c r="AR344" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>10.2</t>
         </is>
       </c>
       <c r="AS344" t="n">
-        <v>0.44</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="345">
@@ -69185,7 +69185,7 @@
       </c>
       <c r="AR345" t="inlineStr">
         <is>
-          <t>8.0</t>
+          <t>12.5</t>
         </is>
       </c>
       <c r="AS345" t="n">
@@ -69371,7 +69371,7 @@
       </c>
       <c r="AR346" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS346" t="n">
@@ -69557,7 +69557,7 @@
       </c>
       <c r="AR347" t="inlineStr">
         <is>
-          <t>9.6</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS347" t="n">
@@ -69726,11 +69726,11 @@
       </c>
       <c r="AR348" t="inlineStr">
         <is>
-          <t>7.1</t>
+          <t>8.2</t>
         </is>
       </c>
       <c r="AS348" t="n">
-        <v>0.54</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="349">
@@ -69870,7 +69870,7 @@
         <v>7</v>
       </c>
       <c r="AL349" t="n">
-        <v>0.29</v>
+        <v>0.3</v>
       </c>
       <c r="AM349" t="inlineStr">
         <is>
@@ -69895,7 +69895,7 @@
       </c>
       <c r="AR349" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS349" t="n">
@@ -70064,11 +70064,11 @@
       </c>
       <c r="AR350" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS350" t="n">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="351">
@@ -70233,11 +70233,11 @@
       </c>
       <c r="AR351" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>7.3</t>
         </is>
       </c>
       <c r="AS351" t="n">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="352">
@@ -70402,7 +70402,7 @@
       </c>
       <c r="AR352" t="inlineStr">
         <is>
-          <t>11.0</t>
+          <t>7.4</t>
         </is>
       </c>
       <c r="AS352" t="n">
@@ -70571,11 +70571,11 @@
       </c>
       <c r="AR353" t="inlineStr">
         <is>
-          <t>6.9</t>
+          <t>6.6</t>
         </is>
       </c>
       <c r="AS353" t="n">
-        <v>0.53</v>
+        <v>0.51</v>
       </c>
     </row>
     <row r="354">
@@ -70760,7 +70760,7 @@
       </c>
       <c r="AR354" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>4.7</t>
         </is>
       </c>
       <c r="AS354" t="n">
@@ -70937,7 +70937,7 @@
       </c>
       <c r="AR355" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>6.1</t>
         </is>
       </c>
       <c r="AS355" t="n">
@@ -71123,7 +71123,7 @@
       </c>
       <c r="AR356" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS356" t="n">
@@ -71301,11 +71301,11 @@
       </c>
       <c r="AR357" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS357" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="358">
@@ -71479,7 +71479,7 @@
       </c>
       <c r="AR358" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS358" t="n">
@@ -71665,7 +71665,7 @@
       </c>
       <c r="AR359" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS359" t="n">
@@ -71850,7 +71850,7 @@
       </c>
       <c r="AR360" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS360" t="n">
@@ -72171,7 +72171,7 @@
         <v>175</v>
       </c>
       <c r="AL362" t="n">
-        <v>0.93</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="AM362" t="inlineStr">
         <is>
@@ -72200,11 +72200,11 @@
       </c>
       <c r="AR362" t="inlineStr">
         <is>
-          <t>10.2</t>
+          <t>4.4</t>
         </is>
       </c>
       <c r="AS362" t="n">
-        <v>0.67</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="363">
@@ -72378,7 +72378,7 @@
       </c>
       <c r="AR363" t="inlineStr">
         <is>
-          <t>4.0</t>
+          <t>3.8</t>
         </is>
       </c>
       <c r="AS363" t="n">
@@ -72757,7 +72757,7 @@
       </c>
       <c r="AR365" t="inlineStr">
         <is>
-          <t>13.7</t>
+          <t>10.1</t>
         </is>
       </c>
       <c r="AS365" t="n">
@@ -72950,7 +72950,7 @@
       </c>
       <c r="AR366" t="inlineStr">
         <is>
-          <t>13.7</t>
+          <t>10.1</t>
         </is>
       </c>
       <c r="AS366" t="n">
@@ -73143,7 +73143,7 @@
       </c>
       <c r="AR367" t="inlineStr">
         <is>
-          <t>4.2</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS367" t="n">
@@ -73320,7 +73320,7 @@
       </c>
       <c r="AR368" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>5.7</t>
         </is>
       </c>
       <c r="AS368" t="n">
@@ -73497,7 +73497,7 @@
       </c>
       <c r="AR369" t="inlineStr">
         <is>
-          <t>4.8</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS369" t="n">
@@ -73677,11 +73677,11 @@
       </c>
       <c r="AR370" t="inlineStr">
         <is>
-          <t>6.3</t>
+          <t>5.6</t>
         </is>
       </c>
       <c r="AS370" t="n">
-        <v>0.5</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="371">
@@ -73854,7 +73854,7 @@
       </c>
       <c r="AR371" t="inlineStr">
         <is>
-          <t>8.1</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS371" t="n">
@@ -74032,11 +74032,11 @@
       </c>
       <c r="AR372" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS372" t="n">
-        <v>0.39</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="373">
@@ -74226,7 +74226,7 @@
       </c>
       <c r="AR373" t="inlineStr">
         <is>
-          <t>6.6</t>
+          <t>4.6</t>
         </is>
       </c>
       <c r="AS373" t="n">
@@ -74406,11 +74406,11 @@
       </c>
       <c r="AR374" t="inlineStr">
         <is>
-          <t>5.7</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS374" t="n">
-        <v>0.44</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="375">
@@ -74586,11 +74586,11 @@
       </c>
       <c r="AR375" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS375" t="n">
-        <v>0.48</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="376">
@@ -74783,7 +74783,7 @@
       </c>
       <c r="AR376" t="inlineStr">
         <is>
-          <t>3.8</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS376" t="n">
@@ -74968,7 +74968,7 @@
       </c>
       <c r="AR377" t="inlineStr">
         <is>
-          <t>3.1</t>
+          <t>3.0</t>
         </is>
       </c>
       <c r="AS377" t="n">
@@ -75154,7 +75154,7 @@
       </c>
       <c r="AR378" t="inlineStr">
         <is>
-          <t>3.2</t>
+          <t>2.6</t>
         </is>
       </c>
       <c r="AS378" t="n">
@@ -75332,11 +75332,11 @@
       </c>
       <c r="AR379" t="inlineStr">
         <is>
-          <t>6.8</t>
+          <t>5.8</t>
         </is>
       </c>
       <c r="AS379" t="n">
-        <v>0.52</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="380">
@@ -75509,7 +75509,7 @@
       </c>
       <c r="AR380" t="inlineStr">
         <is>
-          <t>13.7</t>
+          <t>10.1</t>
         </is>
       </c>
       <c r="AS380" t="n">
@@ -75686,7 +75686,7 @@
       </c>
       <c r="AR381" t="inlineStr">
         <is>
-          <t>13.7</t>
+          <t>10.1</t>
         </is>
       </c>
       <c r="AS381" t="n">
@@ -75863,7 +75863,7 @@
       </c>
       <c r="AR382" t="inlineStr">
         <is>
-          <t>13.7</t>
+          <t>10.1</t>
         </is>
       </c>
       <c r="AS382" t="n">
@@ -76040,7 +76040,7 @@
       </c>
       <c r="AR383" t="inlineStr">
         <is>
-          <t>9.3</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS383" t="n">
@@ -76217,7 +76217,7 @@
       </c>
       <c r="AR384" t="inlineStr">
         <is>
-          <t>5.1</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS384" t="n">
@@ -76394,7 +76394,7 @@
       </c>
       <c r="AR385" t="inlineStr">
         <is>
-          <t>9.7</t>
+          <t>4.3</t>
         </is>
       </c>
       <c r="AS385" t="n">
@@ -76572,11 +76572,11 @@
       </c>
       <c r="AR386" t="inlineStr">
         <is>
-          <t>6.7</t>
+          <t>12.0</t>
         </is>
       </c>
       <c r="AS386" t="n">
-        <v>0.3</v>
+        <v>0.48</v>
       </c>
     </row>
     <row r="387">
@@ -76749,7 +76749,7 @@
       </c>
       <c r="AR387" t="inlineStr">
         <is>
-          <t>3.0</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS387" t="n">
@@ -76926,11 +76926,11 @@
       </c>
       <c r="AR388" t="inlineStr">
         <is>
-          <t>5.2</t>
+          <t>5.0</t>
         </is>
       </c>
       <c r="AS388" t="n">
-        <v>0.41</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="389">
@@ -77096,11 +77096,11 @@
       </c>
       <c r="AR389" t="inlineStr">
         <is>
-          <t>4.6</t>
+          <t>5.9</t>
         </is>
       </c>
       <c r="AS389" t="n">
-        <v>0.34</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="390">
@@ -77274,11 +77274,11 @@
       </c>
       <c r="AR390" t="inlineStr">
         <is>
-          <t>4.7</t>
+          <t>4.5</t>
         </is>
       </c>
       <c r="AS390" t="n">
-        <v>0.35</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="391">
@@ -77460,11 +77460,11 @@
       </c>
       <c r="AR391" t="inlineStr">
         <is>
-          <t>6.4</t>
+          <t>5.1</t>
         </is>
       </c>
       <c r="AS391" t="n">
-        <v>0.31</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="392">
@@ -77638,7 +77638,7 @@
       </c>
       <c r="AR392" t="inlineStr">
         <is>
-          <t>9.4</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS392" t="n">
@@ -77824,11 +77824,11 @@
       </c>
       <c r="AR393" t="inlineStr">
         <is>
-          <t>5.8</t>
+          <t>4.2</t>
         </is>
       </c>
       <c r="AS393" t="n">
-        <v>0.46</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="394">
@@ -78001,7 +78001,7 @@
       </c>
       <c r="AR394" t="inlineStr">
         <is>
-          <t>10.3</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS394" t="n">
@@ -78178,7 +78178,7 @@
       </c>
       <c r="AR395" t="inlineStr">
         <is>
-          <t>10.3</t>
+          <t>3.7</t>
         </is>
       </c>
       <c r="AS395" t="n">
@@ -78371,7 +78371,7 @@
       </c>
       <c r="AR396" t="inlineStr">
         <is>
-          <t>3.6</t>
+          <t>3.9</t>
         </is>
       </c>
       <c r="AS396" t="n">
@@ -78548,7 +78548,7 @@
       </c>
       <c r="AR397" t="inlineStr">
         <is>
-          <t>9.1</t>
+          <t>4.8</t>
         </is>
       </c>
       <c r="AS397" t="n">
@@ -78626,36 +78626,36 @@
     <row r="7" ht="90" customHeight="1">
       <c r="A7" s="111" t="inlineStr">
         <is>
-          <t>The chart illustrates the Friction Pareto Analysis of the 80/20 Rule Application, showcasing the distribution of friction points across various categories. | Key: The top two categories, Scheduling &amp; Planning and Configuration &amp; Data, account for a significant proportion of friction points, with 7,230 and 6,130 points, respectively. | Action: To optimize the application of the 80/20 rule, focus on addressing the high-friction categories, such as Scheduling &amp; Planning and Configuration &amp; Data, to achieve the greatest impact on reducing overall friction.</t>
+          <t>The chart presents a Friction Pareto Analysis of an 80/20 Rule Application, illustrating the distribution of friction points across various categories. | Key: The top two categories, Scheduling &amp; Planning and Configuration &amp; Data, account for the majority of friction points, with 7230 and 6130 points, respectively. | Action: Focusing on optimizing the top two categories, Scheduling &amp; Planning and Configuration &amp; Data, could lead to substantial reductions in overall friction points.</t>
         </is>
       </c>
       <c r="N7" s="111" t="inlineStr">
         <is>
-          <t>The chart illustrates the distribution of risk origin sources in a risk management context, categorized by internal and external factors. | Key: The majority of risk origins (89.9%) are internal, while external factors account for a smaller proportion (10.1%). | Action: To address this imbalance, it is essential to focus on internal risk management strategies and processes to mitigate the impact of internal risk sources. This may involve improving internal controls, enhancing risk awareness, and developing more effective risk management practices.</t>
+          <t>The chart shows the Risk Origin Distribution of an Escalation Source Analysis, with a focus on Internal and External sources. | Key: The majority of the risk originates from internal sources, with 89.9% of the total risk. | Action: To mitigate risk, it is essential to focus on internal sources, as they account for the majority of the risk. This could involve implementing internal controls, improving processes, and addressing internal factors that contribute to risk.</t>
         </is>
       </c>
     </row>
-    <row r="29" ht="90" customHeight="1">
+    <row r="29" ht="84" customHeight="1">
       <c r="A29" s="111" t="inlineStr">
         <is>
-          <t>The chart illustrates the historical performance of a risk score over a 3-month period, comparing it to a target value. | Key: The risk score is consistently above the target value, indicating a higher level of risk. | Action: Given the persistent high risk score, it is recommended to continue monitoring and adjusting strategies to bring the risk score in line with the target value.</t>
+          <t>The chart presents a risk trend analysis, comparing historical performance to a target score over a four-month period. | Key: The risk score has decreased from 48 to 40, indicating a significant improvement in performance. | Action: The data suggests that the current strategy or approach is effective in reducing risk, and it is recommended to continue this approach to maintain or further improve performance.</t>
         </is>
       </c>
       <c r="N29" s="111" t="inlineStr">
         <is>
-          <t>The chart is a Severity-Impact Matrix, also known as a SI-Matrix, which is a tool used to analyze and prioritize security incidents based on their impact and severity. | Key: The chart shows that the majority of incidents (30) have a significant impact on business operations, with 25 of those incidents being critical. This suggests that critical incidents are the most common and have the most significant impact on business operations. | Action: Based on the chart, it is recommended that organizations prioritize resources and attention to critical incidents that have a significant impact on business operations. This can help to mitigate the impact of these incidents and reduce the overall risk to the organization.</t>
+          <t>The chart is a Severity-Impact Matrix Escalation Distribution Analysis, showing the distribution of business impact and severity levels for a given dataset. | Key: The majority of the data points (30) fall into the Severe category, indicating a significant impact on business operations. | Action: Given the high number of Severe data points, it is recommended to prioritize resources and attention to these critical business operations to mitigate potential risks and impacts.</t>
         </is>
       </c>
     </row>
-    <row r="51" ht="84" customHeight="1">
+    <row r="51" ht="90" customHeight="1">
       <c r="A51" s="111" t="inlineStr">
         <is>
-          <t>The chart displays a daily escalation count for breaches, with a focus on smart alert thresholds. | Key: The chart shows a significant spike in breaches on September 25, 2025, with a count of 38/119 (32%), indicating a notable increase in breach activity. | Action: Based on the chart, it is recommended to monitor the daily escalation count for breaches and adjust smart alert thresholds accordingly to account for the potential for increased or decreased activity.</t>
+          <t>The chart displays a daily escalation count over a period of time, with a focus on the number of breaches and smart alert thresholds. | Key: The chart shows a significant increase in breaches from 2025-09 to 2025-11, with a peak of 38 breaches in 2025-10. | Action: It is recommended to monitor and address the increase in breaches, particularly in 2025-10, to prevent further escalation.</t>
         </is>
       </c>
       <c r="N51" s="111" t="inlineStr">
         <is>
-          <t>The chart displays a daily friction score with smart alert thresholds, showing a significant increase in scores over time. | Key: The chart reveals a notable spike in daily friction scores, with a peak of approximately 800, indicating a critical zone. | Action: Given the significant increase in daily friction scores, it is recommended to closely monitor and address any potential issues or breaches to maintain optimal performance.</t>
+          <t>The chart displays a daily friction score with smart alert thresholds, showing a significant increase in daily friction scores over time. | Key: The daily friction score has increased from approximately 200 to over 800, indicating a substantial rise in daily friction. | Action: Given the significant increase in daily friction scores, it is recommended to review and adjust the smart alert thresholds to ensure they remain effective in detecting and responding to changes in daily friction.</t>
         </is>
       </c>
     </row>
@@ -78669,12 +78669,12 @@
     <row r="77" ht="90" customHeight="1">
       <c r="A77" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a performance risk assessment of engineers based on their friction scores, with scores ranging from 150 to 225. | Key: The chart reveals that Manos Antonopoulos and Ankush Juneja have the highest friction scores, both scoring 281, while most engineers have scores between 150 and 188. | Action: To improve performance, engineers with lower scores should focus on reducing their friction score, while those with high scores should maintain their performance to maintain their position.</t>
+          <t>The chart presents a bar graph illustrating the performance of engineers in a friction analysis, with scores ranging from 150 to 225. | Key: The top-performing engineers, Manos Antonopoulos and Ankush Juneja, both achieved a score of 281, while Milind Desai scored 225, indicating a significant gap between the top performers and others. | Action: To further improve performance, engineers should focus on identifying and addressing any areas of improvement, particularly those with scores below 200, to bridge the gap between themselves and the top performers.</t>
         </is>
       </c>
       <c r="N77" s="111" t="inlineStr">
         <is>
-          <t>The chart displays the Engineer Learning Progress, comparing issue resolution (green) and repeat patterns (yellow) across various engineers. | Key: Yashpal Hans has the highest number of issues resolved (11), while Surendra Nehra has the most repeat patterns (44). | Action: To improve learning progress, engineers with high repeat patterns (Surendra Nehra, Daniel Lamas) should focus on addressing these issues to reduce their impact on overall progress.</t>
+          <t>The chart displays the Engineer Learning Progress, comparing issue resolution (green bars) to repeat patterns (yellow bars) across various engineers. | Key: Yashpal Hans has the highest number of issues resolved (11) and the lowest number of repeat patterns (96), indicating a significant improvement in his learning progress. | Action: Based on the chart, it appears that Yashpal Hans is making the most progress in learning, and it would be beneficial to focus on his development and provide him with more resources or support to further improve his learning progress.</t>
         </is>
       </c>
     </row>
@@ -78688,19 +78688,19 @@
     <row r="103" ht="90" customHeight="1">
       <c r="A103" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the LOB Friction Distribution Business Unit Performance, with an average score of 62.3. | Key: The PAG business unit has the highest score at 129.5, while the Optimization business unit has the lowest score at 29.0. | Action: The PAG business unit is performing well and should be continued. The Optimization business unit needs improvement and should be addressed.</t>
+          <t>The chart illustrates the LOB Friction Distribution Business Unit Performance, showcasing the average score of 62.3 and the distribution of scores across various business units. | Key: The PAG business unit stands out with the highest score of 129.5, significantly outperforming the average. | Action: To further improve performance, it is recommended to focus on the PAG business unit, which has already achieved an excellent score, and explore ways to maintain or increase this performance. Additionally, the PM business unit should be targeted for improvement to bring its score closer to the averag</t>
         </is>
       </c>
       <c r="N103" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the performance of various business processes, including Design, Field, Integration, Optimization, PAG, and PM, across three metrics: Volume (normalized), Friction Score, and Resolution Time (normalized). | Key: The Friction Score is the lowest for Design and the highest for PAG, indicating that PAG has the most friction in its business process. | Action: To improve the overall performance of the business processes, it is recommended to focus on reducing the Friction Score, particularly for PAG, which has the highest Friction Score among all the business processes. This could be achieved by identifying and addressing the specific challenges or ineffi</t>
+          <t>The chart compares the performance of three metrics - Volume (normalized), Friction Score, and Resolution Time (normalized) - across different business areas. | Key: The Friction Score is the highest among the three metrics, with a score of 129 in PAG, indicating a significant improvement in this area. | Action: To further improve performance, focus on reducing Friction Score in areas where it is below 100, such as Design (54) and Field (48), to achieve better results.</t>
         </is>
       </c>
     </row>
-    <row r="125" ht="90" customHeight="1">
+    <row r="125" ht="84" customHeight="1">
       <c r="A125" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the LOB (Line of Business) category breakdown of issue distribution by business unit. | Key: The chart highlights that PM (Project Management) has the highest number of issues, with over 140 issues, while Field and PAG (Project-Related) have the fewest issues, with around 20-30 issues. | Action: Based on the chart, it appears that PM is the most critical business unit, with the most issues. Therefore, it may be beneficial to focus on improving PM processes and reducing the number of issues in this area.</t>
+          <t>The chart illustrates the distribution of issues across various categories, with a focus on the number of issues per category. | Key: The category with the highest number of issues is PM, with over 150 issues, while others like Design, Integration, and Field have fewer than 20 issues. | Action: Given the high number of issues in the PM category, it may be beneficial to focus on addressing these issues first to improve overall performance.</t>
         </is>
       </c>
     </row>
@@ -78714,36 +78714,36 @@
     <row r="151" ht="90" customHeight="1">
       <c r="A151" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the root cause analysis of top escalation drivers, with Scheduling &amp; Planning being the leading cause. | Key: Scheduling &amp; Planning is the most common root cause of escalations, accounting for 136 occurrences. | Action: Addressing Scheduling &amp; Planning issues should be a priority to reduce the number of escalations. This could involve improving planning processes, increasing resources, or implementing more effective scheduling tools.</t>
+          <t>The chart shows the Root Cause Analysis of Top Escalation Drivers, providing insights into the most common reasons for escalations. | Key: Scheduling &amp; Planning is the leading cause of escalations, accounting for 136 occurrences, followed by Configuration &amp; Data Mismatch with 98 occurrences. | Action: Addressing Scheduling &amp; Planning and Configuration &amp; Data Mismatch issues should be a priority to reduce the number of escalations. This could involve improving planning processes, enhancing configuration management, and ensuring data accuracy to prevent these types of issues.</t>
         </is>
       </c>
       <c r="N151" s="111" t="inlineStr">
         <is>
-          <t>The chart presents four pie charts that display the performance of a Learning System Integrity Health Metrics Dashboard, focusing on Data Quality, Model Accuracy, Model Feedback, and Data Quality. | Key: The Data Quality pie chart shows that 92% of data is of high quality, while the Model Accuracy pie chart indicates that 87% of models are accurate. | Action: Based on these charts, it appears that the Learning System is performing well in terms of data quality and model accuracy, but it would be beneficial to review and improve the model feedback process to further enhance overall performance.</t>
+          <t>The chart displays four pie charts representing different metrics for a health metrics dashboard, including data quality, model accuracy, learning system integrity, and feedback loop. | Key: The learning system integrity health metrics dashboard has a high level of model accuracy, with 87% of data being accurate. | Action: The data quality metric should be improved to match the model accuracy metric. This can be achieved by implementing more robust data collection and data quality checks. This will ensure that the data is accurate and reliable, which is essential for making informed decisions. By improving data qualit</t>
         </is>
       </c>
     </row>
     <row r="173" ht="90" customHeight="1">
       <c r="A173" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a distribution of escalations across various categories, with Scheduling &amp; Planning having the highest number of escalations. | Key: The category with the most escalations is Scheduling &amp; Planning, with 85 escalations, while Nesting &amp; Tool Errors has the fewest with 15. | Action: Addressing the high number of Scheduling &amp; Planning escalations is crucial, but it's also essential to investigate and address the low number of Nesting &amp; Tool Errors to ensure all categories are performing optimally.</t>
+          <t>The chart presents a distribution of escalations across various categories, providing insights into the frequency and nature of these issues. | Key: The category with the highest number of escalations is Scheduling &amp; Planning, accounting for 85% of the total, followed by Documentation &amp; Reporting with 45%. | Action: Given the high frequency of Scheduling &amp; Planning and Document &amp; Reporting issues, it is recommended that these areas be given priority in terms of resource allocation and resource planning to address these issues effectively.</t>
         </is>
       </c>
       <c r="N173" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the distribution of ticket volume across categories and subcategories, providing insights into the relative importance of each. | Key: The "Scheduling &amp; Planning" category has the highest ticket volume, with 43 tickets in Sub-Cat-1 and 43 in Sub-Cat-2, indicating a significant focus on this area. | Action: Given the high ticket volume in the "Scheduling &amp; Planning" category, it may be beneficial to focus resources on this area to address any potential issues or concerns.</t>
+          <t>The chart shows a comparison of ticket volume heatmaps for categories and subcategories. | Key: The category "Scheduling &amp; Planning" has the highest ticket volume, with 43 tickets in Sub-Cat-1 and 33 in Sub-Cat-2. | Action: It is recommended to focus on improving the process of Scheduling &amp; Planning to reduce the high number of tickets in this category.</t>
         </is>
       </c>
     </row>
     <row r="195" ht="90" customHeight="1">
       <c r="A195" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the baseline and recent periods for various categories, highlighting changes in category drift. | Key: The chart shows that most categories have experienced a decline in recent times, with only a few exceptions. | Action: Given the decline in category drift, it is recommended to focus on improving categories that have experienced a significant decline, such as Scheduling &amp; Planning (-58%), Process Compliance (-50%), and Communication &amp; Response (-17%). This could involve re-evaluating processes, training, or resource</t>
+          <t>The chart shows a comparison of category drift between baseline and recent periods, with categories on the y-axis and percentage changes on the x-axis. | Key: The chart highlights a significant increase in category drift, with most categories experiencing a decline in performance. | Action: Based on the chart, it appears that there is a need to review and address the performance decline in these categories, potentially through further analysis or action.</t>
         </is>
       </c>
       <c r="N195" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the distribution of categories between Baseline (60%) and Recent (40%) data sets. | Key: The category with the highest percentage in both Baseline and Recent data sets is "Scheduling &amp; Planning" with 58% and 42% respectively. | Action: Given the stable distribution of categories, it may be beneficial to focus on improving the performance of categories with lower percentages, such as "Process Compliance" and "Nesting &amp; Tool Errors", to further improve overall performance.</t>
+          <t>The chart compares the distribution of categories between a baseline (60%) and a recent (40%) dataset, highlighting differences in category distribution. | Key: The most significant difference is in the "Scheduling &amp; Planning" category, which has a much higher percentage in the recent dataset (58%) compared to the baseline (4%). | Action: Based on the chart, it appears that there is a shift in focus towards more planning and preparation in the recent dataset, which could be a good thing. However, it also means that there is less emphasis on communication and data management, which could be a concern. It would be worth exploring why t</t>
         </is>
       </c>
     </row>
@@ -78754,22 +78754,22 @@
         </is>
       </c>
     </row>
-    <row r="221" ht="84" customHeight="1">
+    <row r="221" ht="90" customHeight="1">
       <c r="A221" s="111" t="inlineStr">
         <is>
-          <t>The chart presents a comparison of model performance across three metrics - accuracy, precision, and recall - over a six-week period. | Key: The model's performance is consistently high across all three metrics, with scores above 80% for all weeks. | Action: Given the high scores and improving trend, it is recommended to continue monitoring and fine-tuning the model to maintain or further improve its performance.</t>
+          <t>The chart shows a comparison of model performance over time, with scores for predictive model accuracy, model performance trend analysis, and model performance trend analysis. | Key: The chart shows that all three models (Predictive Model Accuracy, Model Performance Trend Analysis, and Model Performance Trend Analysis) have similar scores, with Predictive Model Accuracy having the highest score. | Action: Based on the chart, it appears that Predictive Model Accuracy is the most accurate model, and it is recommended to use this model for future predictions.</t>
         </is>
       </c>
       <c r="N221" s="111" t="inlineStr">
         <is>
-          <t>The chart compares AI Recurrence Prediction Predicted vs Actual Rates across various categories. | Key: The actual rates are generally higher than the predicted rates, with Process Complia. having the largest difference at 10%. | Action: To improve accuracy, consider re-evaluating the AI Recurrence Prediction model and/or gathering more data to better understand the actual rates.</t>
+          <t>The chart compares AI Recurrence Prediction Predicted vs. Actual Rates across various categories. | Key: The chart shows that the actual rates are generally higher than the predicted rates, with Process Complia. having the largest difference at 5%. | Action: To improve the accuracy of the AI Recurrence Prediction, it is recommended to re-evaluate and adjust the prediction models to better align with actual rates, particularly for categories like Process Complia. with high prediction-actual rate differences.</t>
         </is>
       </c>
     </row>
     <row r="243" ht="90" customHeight="1">
       <c r="A243" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a box-and-whisker plot of resolution time distribution for various categories, with a target resolution time of 2.5 days. | Key: The actual resolution times for most categories are significantly longer than the target, with most categories having resolution times between 10-20 days. | Action: Given the significant gap between actual and target resolution times, it may be necessary to re-evaluate and improve processes or resource allocation to meet the target resolution time of 2.5 days.</t>
+          <t>The chart shows a box-and-whisker plot of resolution time distribution for various categories, with a target resolution time of 3 days. | Key: The actual resolution times for most categories are much longer than the target, with most categories having a median resolution time of around 10-20 days. | Action: Based on the chart, it appears that most categories need to improve their process or resource allocation to meet the target resolution time of 3 days. This could be achieved through process improvement, resource allocation, or both.</t>
         </is>
       </c>
     </row>
@@ -78783,12 +78783,12 @@
     <row r="269" ht="90" customHeight="1">
       <c r="A269" s="111" t="inlineStr">
         <is>
-          <t>The chart provides a financial impact analysis of various categories, including direct and indirect costs, and potential savings. | Key: The chart highlights that configuration and validation &amp; QA have the highest potential savings, with configuration having a potential saving of $9,000 and validation &amp; QA having a potential saving of $3,000. | Action: Based on the chart, it is recommended that companies focus on configuration and validation &amp; QA to reduce costs and increase potential savings. This can be achieved by investing in these areas and implementing cost-reducing strategies.</t>
+          <t>The chart provides a financial impact analysis of various categories, including direct and indirect costs, as well as potential savings. | Key: The chart highlights that configuration &amp;. and site readiness have the highest potential savings, with configuration &amp;. having the highest direct and indirect costs. | Action: Based on the chart, it is recommended to focus on configuration &amp;. and site readiness to achieve the most significant potential savings. This could involve investing in these areas to reduce costs and increase savings.</t>
         </is>
       </c>
       <c r="N269" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the financial impact of various subcategories of cost drivers on a company's operations, with a total financial impact of $810,000. | Key: The chart highlights that Backhaul Issues have the most significant financial impact, accounting for $180,000 of the total, while Backhaul Issues and MW/Transmission Issues together account for over 50% of the total financial impact. | Action: The company should focus on addressing Backhaul Issues and MW/Transmission Issues to reduce their financial impact and improve overall operations.</t>
+          <t>The chart provides a breakdown of the financial impact of various subcategories of cost drivers on a project or company. | Key: The chart reveals that Backhaul Issues have the most significant financial impact, with a total of $180,000, while Backhaul Issues and MW/Transmission Issues account for the majority of the financial impact. | Action: To reduce the financial impact of these issues, it is essential to address the most critical and high-impact issues first, such as Backhaul Issues and MW/Transmission Issues. This can be achieved by prioritizing these issues and allocating resources to address them.</t>
         </is>
       </c>
     </row>
@@ -78799,34 +78799,34 @@
         </is>
       </c>
     </row>
-    <row r="295" ht="90" customHeight="1">
+    <row r="295" ht="84" customHeight="1">
       <c r="A295" s="111" t="inlineStr">
         <is>
-          <t>The chart shows the distribution of similar ticket counts for 396 tickets analyzed, with an average of 3.4 matches per ticket. | Key: The distribution is skewed towards tickets with few matches, with a mean of 3.4 and a median of 5, indicating that most tickets have fewer matches. | Action: Given the skewness of the distribution, it may be worth exploring why most tickets have fewer matches, and whether there are any patterns or issues that could be addressed to improve the number of matches.</t>
+          <t>The chart shows the distribution of similar ticket counts for 396 tickets analyzed, with an average of 3.4 matches per ticket. | Key: The chart shows that most tickets have 0-1 similar tickets, with a significant spike in tickets with 5 similar tickets. | Action: Given the high number of tickets with 5 similar tickets, it may be worth investigating why this is happening, as it could be a sign of a specific issue or problem that needs to be addressed.</t>
         </is>
       </c>
       <c r="N295" s="111" t="inlineStr">
         <is>
-          <t>The chart provides a resolution consistency analysis based on similar ticket patterns, offering insights into the resolution process. | Key: The chart reveals that Scheduling &amp; Planning has the highest number of Inconsistencies (122), followed by Configuration &amp; Data (63), and then Documentation &amp; Readiness (25). | Action: To improve the resolution process, it is recommended to focus on Scheduling &amp; Planning and Configuration &amp; Data, as they have the most Inconsistencies. This could involve training or resources to improve these areas.</t>
+          <t>The chart presents a bar chart comparing resolution consistency analysis based on similar ticket patterns, providing insights into the number of Inconsistencies by Category. | Key: The chart reveals that Scheduling &amp; Planning has the highest number of Inconsistencies by Category, with 122, while Scheduling &amp; Planning has the lowest number of Inconsist… | Action: The chart suggests that S… The chart shows that S…</t>
         </is>
       </c>
     </row>
     <row r="317" ht="90" customHeight="1">
       <c r="A317" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a distribution of similarity scores for 321 matches, with a focus on high and medium confidence scores. | Key: The chart highlights a significant difference in distribution between high and medium confidence scores, with high confidence scores having a much higher average score. | Action: Based on the chart, it appears that high confidence scores are more likely to be similar to each other, which could be used to improve the accuracy of the model by focusing on these high- confidence scores.</t>
+          <t>The chart shows a distribution of similarity scores for 321 matches analyzed, with a focus on high and medium confidence scores. | Key: The chart highlights a significant difference in distribution between high and medium confidence scores, with high confidence scores being much more frequent. | Action: The chart suggests that there is a need for further analysis of high- and medium- confidence scores to better understand their respective distributions and potential causes of these differences.</t>
         </is>
       </c>
       <c r="N317" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the mean absolute differences in resolution times for similar ticket analysis and AI prediction. | Key: The mean absolute difference for similar ticket analysis is around 10.0 days, while for AI prediction, it's around 5.0 days, indicating that AI prediction is generally more accurate. | Action: Based on the chart, it appears that AI prediction is a more accurate method for predicting resolution times, and therefore, it is recommended to use AI prediction for similar ticket analysis.</t>
+          <t>The chart compares the resolution time of similar ticket analysis between expected (similar tickets) and AI-predicted (AI predicted) categories. | Key: The chart shows that AI-predicted categories have a higher mean difference of 9.6 days compared to expected (similar tickets) categories. | Action: Based on the chart, it appears that AI-prediction is not as accurate as expected (similar tickets) for certain categories, which may require further investigation and improvement.</t>
         </is>
       </c>
     </row>
     <row r="339" ht="90" customHeight="1">
       <c r="A339" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a comparison of similarity search effectiveness across various categories and origins, with a focus on match effectiveness. | Key: The chart highlights the significant difference in match effectiveness between internal and external sources, with internal sources performing better in most categories. | Action: Based on the chart, it is recommended to focus on internal sources for better match effectiveness, especially in categories like Configuration &amp;.. and Process Complia.., where internal sources perform better.</t>
+          <t>The chart presents a comparison of similarity search effectiveness across various categories and origins, with a focus on match effectiveness. | Key: The chart reveals that Site Readiness and Site Readiness-related categories (Site Readiness, Site Readiness: Site Readiness) have the highest match effectiveness, with values above 90%. This suggests that these categories are particularly effective in achieving similar results. | Action: Based on the chart, it appears that focusing on categories like Site Readiness and Site Readiness: Site Readness could lead to more effective similarity searches. These categories seem to have higher match effectiveness, which could be valuable for various applications.</t>
         </is>
       </c>
     </row>
@@ -78840,31 +78840,31 @@
     <row r="365" ht="90" customHeight="1">
       <c r="A365" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a bar chart of learning effectiveness scores for various categories. | Key: The category with the lowest learning effectiveness score is Process Compliancy with a score of F (2), while Nesting &amp; Tool Error has the highest score of F (12). | Action: Based on the chart, it is recommended to review and improve the learning effectiveness of all categories, especially Process Compliancy, to ensure that they meet the minimum learning effectiveness score of D (35-49). This can be achieved by providing more resources, resources, and resources. This ca</t>
+          <t>This chart presents a bar chart of learning effectiveness scores for various categories, based on recurrence, lesson completion, and consistency. | Key: The category with the lowest learning effectiveness score is "Nesting &amp; Tool Error" with a score of F (12), while "Process Compliance" has the highest score of F (2). | Action: Based on the chart, it appears that most categories have room for improvement in learning effectiveness, particularly "Nestings &amp; Tool Error" which has the lowest score. This suggests that these categories may benefit from additional resources or resources to improve learning effectiveness.</t>
         </is>
       </c>
       <c r="N365" s="111" t="inlineStr">
         <is>
-          <t>The chart shows a comparison of lesson completion rates between "Documented" and "Completed" lessons. | Key: Both "Documented" and "Completed" lessons have a completion rate of 0, indicating that neither category has any lessons that have been completed. | Action: Given that both categories have zero completion rates, it may be worth re-evaluating the lesson content or teaching methods to improve student engagement and completion rates.</t>
+          <t>The chart shows the lesson documentation and completion rates for various categories. | Key: The chart indicates that all categories have a completion rate of 0%, suggesting that no lessons were completed in any of these categories. | Action: Given the lack of completed lessons in any category, it is recommended to review and improve the lesson content and/or teaching methods to increase the completion rate. This could involve re-­­­­­­­­­­­­­­­­­­­­­­­­­­­­­­­</t>
         </is>
       </c>
     </row>
     <row r="387" ht="90" customHeight="1">
       <c r="A387" s="111" t="inlineStr">
         <is>
-          <t>The chart compares the Recurrence Rate of lessons and the Recurrence Rate of code, with both axes representing the percentage of code or lessons that are successfully completed. | Key: The chart shows that for both code and lessons, there is a high Recurrence Rate, with most code and lessons having a Recurrence Rate above 80%. However, there is a significant difference in the Recurrence Rate of code and lessons, with code having a much higher Recurrence Rate. | Action: Based on the chart, it appears that code is more likely to be successfully completed than lessons. This could be due to various factors, such as the more [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [...] [.</t>
+          <t>The chart compares the Recurrence Rate of different processes in an educational setting, with a focus on the ideal balance between Low Recurrence and High Completion. | Key: The chart highlights that Process Comp. and Config. have the highest Recurrence Rate, while Process Comp. has the lowest Recurrence Rate among all processes. | Action: To improve the Recurrence Rate, it is recommended to focus on processes with lower Recurrence Rates, such as Process Comp. and Config., and implement strategies to increase their Recurrence Rates.</t>
         </is>
       </c>
       <c r="N387" s="111" t="inlineStr">
         <is>
-          <t>The chart illustrates the learning effectiveness of various categories across different business markets, with scores ranging from 0 to 100. | Key: The category with the highest learning score is "Communication &amp;..." with a score of 78, while "Nesting &amp; Tool" has the lowest score of 12. | Action: To improve learning effectiveness, focus on categories with lower scores, such as "Nesting &amp; Tool" and "Scheduling &amp; PI", and consider investing in training or resources to improve these areas.</t>
+          <t>The chart presents a learning effectiveness matrix for various categories, with green indicating good learning, red indicating needs attention, and green and red combined indicating good learning with needs for attention. | Key: The chart highlights that most categories have a good learning effect, with only a few categories requiring attention. The category with the most attention needed is "Nesting &amp; Tool" with 72%. | Action: Based on the chart, it is recommended to focus on categories with needs for attention, such as "Nesting &amp; Tool" and "Scheduling &amp; PI", to improve their learning effect. This can be done by providing more resources or training to these categories.</t>
         </is>
       </c>
     </row>
-    <row r="409" ht="90" customHeight="1">
+    <row r="409" ht="84" customHeight="1">
       <c r="A409" s="111" t="inlineStr">
         <is>
-          <t>The chart presents AI-generated improvement recommendations for various aspects of an organization, including Process Compliance, Scheduling &amp; Planning, Site Readiness, Documentation &amp; Reporting, and Validation &amp; Quality (QA) for Process Improvement. | Key: The chart highlights that all five areas have a critical (C) rating, indicating that they are critical to the success of the organization. | Action: Given that all five areas have a critical (C) rating, it is essential to focus on improving all of them to ensure the success of the organization. This can be achieved by investing in resources, training, and resources to improve process compliance, scheduling and planning, site readiness, documenta</t>
+          <t>The chart presents an AI-generated improvement recommendations chart for various AI-generated improvement recommendations. | Key: The chart shows that all categories have a critical score of C, indicating that all areas need improvement. | Action: Based on the chart, it is recommended to focus on process compliance, scheduling and planning, site readiness, documentation and reporting, and validation and quality to improve scores and overall performance.</t>
         </is>
       </c>
     </row>

</xml_diff>